<commit_message>
finished mapping the data from the data frame into the OOP
</commit_message>
<xml_diff>
--- a/python-notebooks/billing.xlsx
+++ b/python-notebooks/billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\klowe\go\src\stash.teslamotors.com\kevin-personal\energy-project\python-notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649A3E8B-F80C-4096-91BF-4865E1D48B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2243F54-1682-4A5B-BF2A-F2FE45077D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Billing" sheetId="1" r:id="rId1"/>
@@ -429,14 +429,15 @@
     <t>Table subheader</t>
   </si>
   <si>
-    <t>Service End Date [Date]</t>
-  </si>
-  <si>
     <t>Billing Date [Date]
 (43)</t>
   </si>
   <si>
     <t>Allocated Export Credits</t>
+  </si>
+  <si>
+    <t>Service End Date [Date]
+(44)</t>
   </si>
 </sst>
 </file>
@@ -448,8 +449,8 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot; &quot;yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -693,8 +694,8 @@
     <xf numFmtId="44" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="5" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="5" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="5" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -709,10 +710,10 @@
     <xf numFmtId="44" fontId="4" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="5" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="5" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="5" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="5" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="5" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -749,13 +750,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="5" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="5" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -994,11 +995,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BE1013"/>
+  <dimension ref="A1:BE1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH12" sqref="AH12"/>
+      <selection pane="topRight" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1112,7 +1113,7 @@
       <c r="BD2" s="87"/>
       <c r="BE2" s="87"/>
     </row>
-    <row r="3" spans="1:57" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:57" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1131,7 +1132,7 @@
       <c r="H3" s="89"/>
       <c r="I3" s="89"/>
       <c r="J3" s="88" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K3" s="89"/>
       <c r="L3" s="89"/>
@@ -1492,10 +1493,10 @@
         <v>106</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>56</v>
@@ -1792,18 +1793,18 @@
         <v>395</v>
       </c>
       <c r="AN7" s="11">
-        <f>D7-J7</f>
+        <f t="shared" ref="AN7:AN17" si="8">D7-J7</f>
         <v>-449</v>
       </c>
       <c r="AO7" s="11">
-        <f>E7-K7</f>
+        <f t="shared" ref="AO7:AO17" si="9">E7-K7</f>
         <v>-58</v>
       </c>
       <c r="AP7" s="12">
         <v>-507</v>
       </c>
       <c r="AQ7" s="13">
-        <f>AP7/F7</f>
+        <f t="shared" ref="AQ7:AQ14" si="10">AP7/F7</f>
         <v>0.50801603206412826</v>
       </c>
       <c r="AR7" s="11">
@@ -1825,7 +1826,7 @@
         <v>5.8379099999999999</v>
       </c>
       <c r="AW7" s="14">
-        <f t="shared" ref="AW7:AW8" si="8">AV7+AU7</f>
+        <f t="shared" ref="AW7:AW8" si="11">AV7+AU7</f>
         <v>-13.174499999999998</v>
       </c>
       <c r="AX7" s="14">
@@ -1836,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="AZ7" s="17">
-        <f t="shared" ref="AZ7:AZ8" si="9">AY7+AX7+AW7</f>
+        <f t="shared" ref="AZ7:AZ8" si="12">AY7+AX7+AW7</f>
         <v>-14.684499999999998</v>
       </c>
       <c r="BA7" s="18">
@@ -1863,7 +1864,7 @@
         <v>45456</v>
       </c>
       <c r="D8" s="11">
-        <f t="shared" ref="D8" si="10">ROUND(J8/M8,0)</f>
+        <f t="shared" ref="D8" si="13">ROUND(J8/M8,0)</f>
         <v>-1411</v>
       </c>
       <c r="E8" s="11">
@@ -1874,49 +1875,49 @@
         <v>-1601</v>
       </c>
       <c r="G8" s="11">
-        <f t="shared" ref="G8:H8" si="11">G9+G10</f>
+        <f t="shared" ref="G8:H8" si="14">G9+G10</f>
         <v>330</v>
       </c>
       <c r="H8" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>121</v>
       </c>
       <c r="I8" s="12">
         <v>451</v>
       </c>
       <c r="J8" s="11">
-        <f t="shared" ref="J8:K8" si="12">J9+J10</f>
+        <f t="shared" ref="J8:K8" si="15">J9+J10</f>
         <v>-704</v>
       </c>
       <c r="K8" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-95</v>
       </c>
       <c r="L8" s="12">
         <v>-799</v>
       </c>
       <c r="M8" s="13">
-        <f t="shared" ref="M8" si="13">L8/F8</f>
+        <f t="shared" ref="M8" si="16">L8/F8</f>
         <v>0.49906308557151779</v>
       </c>
       <c r="N8" s="11">
-        <f t="shared" ref="N8:R8" si="14">N9+N10</f>
+        <f t="shared" ref="N8:R8" si="17">N9+N10</f>
         <v>-374</v>
       </c>
       <c r="O8" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>26</v>
       </c>
       <c r="P8" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-348</v>
       </c>
       <c r="Q8" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-47.806659999999994</v>
       </c>
       <c r="R8" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>3.8457699999999995</v>
       </c>
       <c r="S8" s="14">
@@ -1972,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="AH8" s="20">
-        <f t="shared" ref="AH7:AH8" si="15">AE8+AF8+AG8</f>
+        <f t="shared" ref="AH8" si="18">AE8+AF8+AG8</f>
         <v>21.75</v>
       </c>
       <c r="AI8" s="11"/>
@@ -1981,53 +1982,53 @@
         <v>21.75</v>
       </c>
       <c r="AK8" s="11">
-        <f t="shared" ref="AK8:AL8" si="16">AR8-AN8</f>
+        <f t="shared" ref="AK8:AL8" si="19">AR8-AN8</f>
         <v>349</v>
       </c>
       <c r="AL8" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>102</v>
       </c>
       <c r="AM8" s="12">
         <v>451</v>
       </c>
       <c r="AN8" s="11">
-        <f>D8-J8</f>
+        <f t="shared" si="8"/>
         <v>-707</v>
       </c>
       <c r="AO8" s="11">
-        <f>E8-K8</f>
+        <f t="shared" si="9"/>
         <v>-95</v>
       </c>
       <c r="AP8" s="12">
         <v>-802</v>
       </c>
       <c r="AQ8" s="13">
-        <f>AP8/F8</f>
+        <f t="shared" si="10"/>
         <v>0.50093691442848221</v>
       </c>
       <c r="AR8" s="11">
-        <f t="shared" ref="AR8:AV8" si="17">AR9+AR10</f>
+        <f t="shared" ref="AR8:AV8" si="20">AR9+AR10</f>
         <v>-358</v>
       </c>
       <c r="AS8" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>7</v>
       </c>
       <c r="AT8" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>-351</v>
       </c>
       <c r="AU8" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>-45.9373</v>
       </c>
       <c r="AV8" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.77081</v>
       </c>
       <c r="AW8" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-45.166490000000003</v>
       </c>
       <c r="AX8" s="14">
@@ -2038,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="AZ8" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-48.806490000000004</v>
       </c>
       <c r="BA8" s="18">
@@ -2052,7 +2053,7 @@
       </c>
       <c r="BD8" s="14"/>
       <c r="BE8" s="21">
-        <f t="shared" ref="BE7:BE8" si="18">BC8+BB8+BD8</f>
+        <f t="shared" ref="BE8" si="21">BC8+BB8+BD8</f>
         <v>11.75</v>
       </c>
     </row>
@@ -2087,7 +2088,7 @@
         <v>27</v>
       </c>
       <c r="P9" s="24">
-        <f t="shared" ref="P9:P11" si="19">O9+N9</f>
+        <f t="shared" ref="P9:P11" si="22">O9+N9</f>
         <v>-273</v>
       </c>
       <c r="Q9" s="27">
@@ -2117,25 +2118,25 @@
       <c r="AI9" s="27"/>
       <c r="AJ9" s="27"/>
       <c r="AK9" s="11">
-        <f t="shared" ref="AK9:AL9" si="20">AR9-AN9</f>
+        <f t="shared" ref="AK9:AL9" si="23">AR9-AN9</f>
         <v>-842</v>
       </c>
       <c r="AL9" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>-64</v>
       </c>
       <c r="AM9" s="24"/>
       <c r="AN9" s="11">
-        <f>D9-J9</f>
+        <f t="shared" si="8"/>
         <v>573</v>
       </c>
       <c r="AO9" s="11">
-        <f>E9-K9</f>
+        <f t="shared" si="9"/>
         <v>77</v>
       </c>
       <c r="AP9" s="24"/>
       <c r="AQ9" s="13" t="e">
-        <f>AP9/F9</f>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AR9" s="24">
@@ -2145,7 +2146,7 @@
         <v>13</v>
       </c>
       <c r="AT9" s="24">
-        <f t="shared" ref="AT9:AT11" si="21">AS9+AR9</f>
+        <f t="shared" ref="AT9:AT11" si="24">AS9+AR9</f>
         <v>-256</v>
       </c>
       <c r="AU9" s="27">
@@ -2197,15 +2198,15 @@
         <v>-1</v>
       </c>
       <c r="P10" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>-75</v>
       </c>
       <c r="Q10" s="27">
-        <f t="shared" ref="Q10:Q11" si="22">N10*0.13559</f>
+        <f t="shared" ref="Q10:Q11" si="25">N10*0.13559</f>
         <v>-10.033659999999999</v>
       </c>
       <c r="R10" s="27">
-        <f t="shared" ref="R10:R11" si="23">O10*0.19586</f>
+        <f t="shared" ref="R10:R11" si="26">O10*0.19586</f>
         <v>-0.19586000000000001</v>
       </c>
       <c r="S10" s="27"/>
@@ -2227,25 +2228,25 @@
       <c r="AI10" s="27"/>
       <c r="AJ10" s="27"/>
       <c r="AK10" s="11">
-        <f t="shared" ref="AK10:AL10" si="24">AR10-AN10</f>
+        <f t="shared" ref="AK10:AL10" si="27">AR10-AN10</f>
         <v>-220</v>
       </c>
       <c r="AL10" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>-24</v>
       </c>
       <c r="AM10" s="24"/>
       <c r="AN10" s="11">
-        <f>D10-J10</f>
+        <f t="shared" si="8"/>
         <v>131</v>
       </c>
       <c r="AO10" s="11">
-        <f>E10-K10</f>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="AP10" s="24"/>
       <c r="AQ10" s="13" t="e">
-        <f>AP10/F10</f>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AR10" s="24">
@@ -2255,15 +2256,15 @@
         <v>-6</v>
       </c>
       <c r="AT10" s="24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>-95</v>
       </c>
       <c r="AU10" s="27">
-        <f t="shared" ref="AU10:AU11" si="25">AR10*0.13559</f>
+        <f t="shared" ref="AU10:AU11" si="28">AR10*0.13559</f>
         <v>-12.067509999999999</v>
       </c>
       <c r="AV10" s="27">
-        <f t="shared" ref="AV10:AV11" si="26">AS10*0.19586</f>
+        <f t="shared" ref="AV10:AV11" si="29">AS10*0.19586</f>
         <v>-1.17516</v>
       </c>
       <c r="AW10" s="27"/>
@@ -2296,22 +2297,22 @@
         <v>-1750</v>
       </c>
       <c r="G11" s="11">
-        <f t="shared" ref="G11:H11" si="27">G12+G13</f>
+        <f t="shared" ref="G11:H11" si="30">G12+G13</f>
         <v>393</v>
       </c>
       <c r="H11" s="11">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>250</v>
       </c>
       <c r="I11" s="12">
         <v>643</v>
       </c>
       <c r="J11" s="11">
-        <f t="shared" ref="J11:K11" si="28">J12+J13</f>
+        <f t="shared" ref="J11:K11" si="31">J12+J13</f>
         <v>-1001</v>
       </c>
       <c r="K11" s="11">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>-131</v>
       </c>
       <c r="L11" s="12">
@@ -2328,15 +2329,15 @@
         <v>119</v>
       </c>
       <c r="P11" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>-489</v>
       </c>
       <c r="Q11" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>-82.438719999999989</v>
       </c>
       <c r="R11" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>23.30734</v>
       </c>
       <c r="S11" s="14">
@@ -2401,29 +2402,29 @@
         <v>22.53</v>
       </c>
       <c r="AK11" s="11">
-        <f t="shared" ref="AK11:AL11" si="29">AR11-AN11</f>
+        <f t="shared" ref="AK11:AL11" si="32">AR11-AN11</f>
         <v>276</v>
       </c>
       <c r="AL11" s="11">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>53</v>
       </c>
       <c r="AM11" s="12">
         <v>329</v>
       </c>
       <c r="AN11" s="11">
-        <f>D11-J11</f>
+        <f t="shared" si="8"/>
         <v>-546</v>
       </c>
       <c r="AO11" s="11">
-        <f>E11-K11</f>
+        <f t="shared" si="9"/>
         <v>-72</v>
       </c>
       <c r="AP11" s="12">
         <v>-618</v>
       </c>
       <c r="AQ11" s="13">
-        <f>AP11/F11</f>
+        <f t="shared" si="10"/>
         <v>0.35314285714285715</v>
       </c>
       <c r="AR11" s="11">
@@ -2433,15 +2434,15 @@
         <v>-19</v>
       </c>
       <c r="AT11" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>-289</v>
       </c>
       <c r="AU11" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>-36.609299999999998</v>
       </c>
       <c r="AV11" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>-3.7213400000000001</v>
       </c>
       <c r="AW11" s="14">
@@ -2522,25 +2523,25 @@
       <c r="AI12" s="35"/>
       <c r="AJ12" s="35"/>
       <c r="AK12" s="11">
-        <f t="shared" ref="AK12:AL12" si="30">AR12-AN12</f>
+        <f t="shared" ref="AK12:AL12" si="33">AR12-AN12</f>
         <v>-775</v>
       </c>
       <c r="AL12" s="11">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>-109</v>
       </c>
       <c r="AM12" s="31"/>
       <c r="AN12" s="11">
-        <f>D12-J12</f>
+        <f t="shared" si="8"/>
         <v>775</v>
       </c>
       <c r="AO12" s="11">
-        <f>E12-K12</f>
+        <f t="shared" si="9"/>
         <v>109</v>
       </c>
       <c r="AP12" s="31"/>
       <c r="AQ12" s="13" t="e">
-        <f>AP12/F12</f>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AR12" s="31"/>
@@ -2606,25 +2607,25 @@
       <c r="AI13" s="35"/>
       <c r="AJ13" s="35"/>
       <c r="AK13" s="11">
-        <f t="shared" ref="AK13:AL13" si="31">AR13-AN13</f>
+        <f t="shared" ref="AK13:AL13" si="34">AR13-AN13</f>
         <v>-226</v>
       </c>
       <c r="AL13" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>-22</v>
       </c>
       <c r="AM13" s="31"/>
       <c r="AN13" s="11">
-        <f>D13-J13</f>
+        <f t="shared" si="8"/>
         <v>226</v>
       </c>
       <c r="AO13" s="11">
-        <f>E13-K13</f>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="AP13" s="31"/>
       <c r="AQ13" s="13" t="e">
-        <f>AP13/F13</f>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AR13" s="31"/>
@@ -2684,23 +2685,23 @@
         <v>0.40445402298850575</v>
       </c>
       <c r="N14" s="37">
-        <f t="shared" ref="N14:P14" si="32">N15+N16</f>
+        <f t="shared" ref="N14:P14" si="35">N15+N16</f>
         <v>-267</v>
       </c>
       <c r="O14" s="37">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>86</v>
       </c>
       <c r="P14" s="38">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>-181</v>
       </c>
       <c r="Q14" s="14">
-        <f t="shared" ref="Q14:R14" si="33">SUM(Q15:Q16)</f>
+        <f t="shared" ref="Q14:R14" si="36">SUM(Q15:Q16)</f>
         <v>-35.405396597999996</v>
       </c>
       <c r="R14" s="14">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>16.917801365000003</v>
       </c>
       <c r="S14" s="14">
@@ -2765,49 +2766,49 @@
         <v>21.36</v>
       </c>
       <c r="AK14" s="11">
-        <f t="shared" ref="AK14:AL14" si="34">AR14-AN14</f>
+        <f t="shared" ref="AK14:AL14" si="37">AR14-AN14</f>
         <v>409</v>
       </c>
       <c r="AL14" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>132</v>
       </c>
       <c r="AM14" s="12">
         <v>541</v>
       </c>
       <c r="AN14" s="11">
-        <f>D14-J14</f>
+        <f t="shared" si="8"/>
         <v>-723</v>
       </c>
       <c r="AO14" s="11">
-        <f>E14-K14</f>
+        <f t="shared" si="9"/>
         <v>-106</v>
       </c>
       <c r="AP14" s="12">
         <v>-829</v>
       </c>
       <c r="AQ14" s="13">
-        <f>AP14/F14</f>
+        <f t="shared" si="10"/>
         <v>0.59554597701149425</v>
       </c>
       <c r="AR14" s="11">
-        <f t="shared" ref="AR14:AT14" si="35">AR15+AR16</f>
+        <f t="shared" ref="AR14:AT14" si="38">AR15+AR16</f>
         <v>-314</v>
       </c>
       <c r="AS14" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>26</v>
       </c>
       <c r="AT14" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>-288</v>
       </c>
       <c r="AU14" s="14">
-        <f t="shared" ref="AU14:AV14" si="36">SUM(AU15:AU16)</f>
+        <f t="shared" ref="AU14:AV14" si="39">SUM(AU15:AU16)</f>
         <v>-41.637807834999997</v>
       </c>
       <c r="AV14" s="14">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>5.1146840949999994</v>
       </c>
       <c r="AW14" s="14">
@@ -2893,20 +2894,20 @@
       <c r="AI15" s="43"/>
       <c r="AJ15" s="43"/>
       <c r="AK15" s="38">
-        <f t="shared" ref="AK15:AL15" si="37">AR15-AN15</f>
+        <f t="shared" ref="AK15:AL15" si="40">AR15-AN15</f>
         <v>-64.965500000000006</v>
       </c>
       <c r="AL15" s="38">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>20.620699999999999</v>
       </c>
       <c r="AM15" s="43"/>
       <c r="AN15" s="38">
-        <f>D15-J15</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AO15" s="38">
-        <f>E15-K15</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AP15" s="44"/>
@@ -2918,7 +2919,7 @@
         <v>20.620699999999999</v>
       </c>
       <c r="AT15" s="44">
-        <f t="shared" ref="AT15:AT17" si="38">AS15+AR15</f>
+        <f t="shared" ref="AT15:AT17" si="41">AS15+AR15</f>
         <v>-44.344800000000006</v>
       </c>
       <c r="AU15" s="43">
@@ -2980,7 +2981,7 @@
         <v>-28.712348573999996</v>
       </c>
       <c r="R16" s="43">
-        <f t="shared" ref="R16:R17" si="39">O16*0.20001</f>
+        <f t="shared" ref="R16:R17" si="42">O16*0.20001</f>
         <v>3.5587979309999995</v>
       </c>
       <c r="S16" s="43"/>
@@ -3002,20 +3003,20 @@
       <c r="AI16" s="43"/>
       <c r="AJ16" s="43"/>
       <c r="AK16" s="38">
-        <f t="shared" ref="AK16:AL16" si="40">AR16-AN16</f>
+        <f t="shared" ref="AK16:AL16" si="43">AR16-AN16</f>
         <v>-249.03450000000001</v>
       </c>
       <c r="AL16" s="38">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>5.3792999999999997</v>
       </c>
       <c r="AM16" s="43"/>
       <c r="AN16" s="38">
-        <f>D16-J16</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AO16" s="38">
-        <f>E16-K16</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AP16" s="44"/>
@@ -3027,7 +3028,7 @@
         <v>5.3792999999999997</v>
       </c>
       <c r="AT16" s="44">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>-243.65520000000001</v>
       </c>
       <c r="AU16" s="43">
@@ -3035,7 +3036,7 @@
         <v>-33.766587854999997</v>
       </c>
       <c r="AV16" s="43">
-        <f t="shared" ref="AV16:AV17" si="41">AS16*0.20001</f>
+        <f t="shared" ref="AV16:AV17" si="44">AS16*0.20001</f>
         <v>1.075913793</v>
       </c>
       <c r="AW16" s="43"/>
@@ -3068,22 +3069,22 @@
         <v>-1516</v>
       </c>
       <c r="G17" s="11">
-        <f t="shared" ref="G17:H17" si="42">G18+G19</f>
+        <f t="shared" ref="G17:H17" si="45">G18+G19</f>
         <v>175</v>
       </c>
       <c r="H17" s="11">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>145</v>
       </c>
       <c r="I17" s="12">
         <v>320</v>
       </c>
       <c r="J17" s="11">
-        <f t="shared" ref="J17:K17" si="43">J18+J19</f>
+        <f t="shared" ref="J17:K17" si="46">J18+J19</f>
         <v>-386</v>
       </c>
       <c r="K17" s="11">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>-50</v>
       </c>
       <c r="L17" s="12">
@@ -3108,7 +3109,7 @@
         <v>-25.56476</v>
       </c>
       <c r="R17" s="14">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>19.00095</v>
       </c>
       <c r="S17" s="14">
@@ -3173,22 +3174,22 @@
         <v>21.75</v>
       </c>
       <c r="AK17" s="11">
-        <f t="shared" ref="AK17:AL17" si="44">AR17-AN17</f>
+        <f t="shared" ref="AK17:AL17" si="47">AR17-AN17</f>
         <v>519</v>
       </c>
       <c r="AL17" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>203</v>
       </c>
       <c r="AM17" s="12">
         <v>726</v>
       </c>
       <c r="AN17" s="11">
-        <f>D17-J17</f>
+        <f t="shared" si="8"/>
         <v>-953</v>
       </c>
       <c r="AO17" s="11">
-        <f>E17-K17</f>
+        <f t="shared" si="9"/>
         <v>-123</v>
       </c>
       <c r="AP17" s="12">
@@ -3205,7 +3206,7 @@
         <v>80</v>
       </c>
       <c r="AT17" s="11">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>-354</v>
       </c>
       <c r="AU17" s="14">
@@ -3213,7 +3214,7 @@
         <v>-52.583440000000003</v>
       </c>
       <c r="AV17" s="14">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>16.000799999999998</v>
       </c>
       <c r="AW17" s="14">
@@ -3407,7 +3408,7 @@
         <v>69</v>
       </c>
       <c r="P20" s="24">
-        <f t="shared" ref="P20:P22" si="45">O20+N20</f>
+        <f t="shared" ref="P20:P22" si="48">O20+N20</f>
         <v>-76</v>
       </c>
       <c r="Q20" s="27">
@@ -3437,20 +3438,20 @@
       <c r="AI20" s="27"/>
       <c r="AJ20" s="27"/>
       <c r="AK20" s="11">
-        <f t="shared" ref="AK20:AL20" si="46">AR20-AN20</f>
+        <f t="shared" ref="AK20:AL20" si="49">AR20-AN20</f>
         <v>-275</v>
       </c>
       <c r="AL20" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>99</v>
       </c>
       <c r="AM20" s="24"/>
       <c r="AN20" s="11">
-        <f>D20-J20</f>
+        <f t="shared" ref="AN20:AO22" si="50">D20-J20</f>
         <v>0</v>
       </c>
       <c r="AO20" s="11">
-        <f>E20-K20</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AP20" s="24"/>
@@ -3462,7 +3463,7 @@
         <v>99</v>
       </c>
       <c r="AT20" s="24">
-        <f t="shared" ref="AT20:AT22" si="47">AS20+AR20</f>
+        <f t="shared" ref="AT20:AT22" si="51">AS20+AR20</f>
         <v>-176</v>
       </c>
       <c r="AU20" s="27">
@@ -3482,7 +3483,7 @@
       <c r="BC20" s="17"/>
       <c r="BD20" s="27"/>
       <c r="BE20" s="21">
-        <f t="shared" ref="BE20:BE22" si="48">BC20+BB20+BD20</f>
+        <f t="shared" ref="BE20:BE22" si="52">BC20+BB20+BD20</f>
         <v>0</v>
       </c>
     </row>
@@ -3509,7 +3510,7 @@
         <v>62</v>
       </c>
       <c r="P21" s="24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>64</v>
       </c>
       <c r="Q21" s="27">
@@ -3539,20 +3540,20 @@
       <c r="AI21" s="27"/>
       <c r="AJ21" s="27"/>
       <c r="AK21" s="11">
-        <f t="shared" ref="AK21:AL21" si="49">AR21-AN21</f>
+        <f t="shared" ref="AK21:AL21" si="53">AR21-AN21</f>
         <v>-46</v>
       </c>
       <c r="AL21" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>33</v>
       </c>
       <c r="AM21" s="24"/>
       <c r="AN21" s="11">
-        <f>D21-J21</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AO21" s="11">
-        <f>E21-K21</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="AP21" s="24"/>
@@ -3564,7 +3565,7 @@
         <v>33</v>
       </c>
       <c r="AT21" s="24">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>-13</v>
       </c>
       <c r="AU21" s="27">
@@ -3584,7 +3585,7 @@
       <c r="BC21" s="17"/>
       <c r="BD21" s="27"/>
       <c r="BE21" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
     </row>
@@ -3608,22 +3609,22 @@
         <v>-1292</v>
       </c>
       <c r="G22" s="11">
-        <f t="shared" ref="G22:H22" si="50">G23+G24</f>
+        <f t="shared" ref="G22:H22" si="54">G23+G24</f>
         <v>191</v>
       </c>
       <c r="H22" s="11">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>157</v>
       </c>
       <c r="I22" s="12">
         <v>348</v>
       </c>
       <c r="J22" s="11">
-        <f t="shared" ref="J22:K22" si="51">J23+J24</f>
+        <f t="shared" ref="J22:K22" si="55">J23+J24</f>
         <v>-334</v>
       </c>
       <c r="K22" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>-26</v>
       </c>
       <c r="L22" s="12">
@@ -3634,23 +3635,23 @@
         <v>0.27863777089783281</v>
       </c>
       <c r="N22" s="11">
-        <f t="shared" ref="N22:O22" si="52">N21+N20</f>
+        <f t="shared" ref="N22:O22" si="56">N21+N20</f>
         <v>-143</v>
       </c>
       <c r="O22" s="11">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>131</v>
       </c>
       <c r="P22" s="11">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>-12</v>
       </c>
       <c r="Q22" s="14">
-        <f t="shared" ref="Q22:R22" si="53">Q20+Q21</f>
+        <f t="shared" ref="Q22:R22" si="57">Q20+Q21</f>
         <v>-17.332979999999999</v>
       </c>
       <c r="R22" s="14">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>22.664209999999997</v>
       </c>
       <c r="S22" s="14">
@@ -3717,22 +3718,22 @@
         <v>-33.03</v>
       </c>
       <c r="AK22" s="11">
-        <f t="shared" ref="AK22:AL22" si="54">AR22-AN22</f>
+        <f t="shared" ref="AK22:AL22" si="58">AR22-AN22</f>
         <v>544</v>
       </c>
       <c r="AL22" s="11">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>199</v>
       </c>
       <c r="AM22" s="12">
         <v>743</v>
       </c>
       <c r="AN22" s="11">
-        <f>D22-J22</f>
+        <f t="shared" si="50"/>
         <v>-865</v>
       </c>
       <c r="AO22" s="11">
-        <f>E22-K22</f>
+        <f t="shared" si="50"/>
         <v>-67</v>
       </c>
       <c r="AP22" s="12">
@@ -3751,15 +3752,15 @@
         <v>132</v>
       </c>
       <c r="AT22" s="11">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>-189</v>
       </c>
       <c r="AU22" s="14">
-        <f t="shared" ref="AU22:AV22" si="55">AU20+AU21</f>
+        <f t="shared" ref="AU22:AV22" si="59">AU20+AU21</f>
         <v>-38.729060000000004</v>
       </c>
       <c r="AV22" s="14">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>24.51867</v>
       </c>
       <c r="AW22" s="14">
@@ -3790,7 +3791,7 @@
         <v>-55.17</v>
       </c>
       <c r="BE22" s="21">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>-43.03</v>
       </c>
     </row>
@@ -3941,11 +3942,11 @@
         <v>45610</v>
       </c>
       <c r="D25" s="51">
-        <f t="shared" ref="D25:D27" si="56">ROUND(J25/M25,0)</f>
+        <f t="shared" ref="D25:D27" si="60">ROUND(J25/M25,0)</f>
         <v>-973</v>
       </c>
       <c r="E25" s="51">
-        <f t="shared" ref="E25:E27" si="57">ROUND(K25/M25,0)</f>
+        <f t="shared" ref="E25:E27" si="61">ROUND(K25/M25,0)</f>
         <v>-17</v>
       </c>
       <c r="F25" s="51">
@@ -3970,7 +3971,7 @@
         <v>-357</v>
       </c>
       <c r="M25" s="52">
-        <f t="shared" ref="M25:M27" si="58">L25/F25</f>
+        <f t="shared" ref="M25:M27" si="62">L25/F25</f>
         <v>0.3606060606060606</v>
       </c>
       <c r="N25" s="53">
@@ -3980,19 +3981,19 @@
         <v>191</v>
       </c>
       <c r="P25" s="53">
-        <f t="shared" ref="P25:P27" si="59">O25+N25</f>
+        <f t="shared" ref="P25:P27" si="63">O25+N25</f>
         <v>59</v>
       </c>
       <c r="Q25" s="54">
-        <f t="shared" ref="Q25:Q27" si="60">N25*0.11761</f>
+        <f t="shared" ref="Q25:Q27" si="64">N25*0.11761</f>
         <v>-15.524520000000001</v>
       </c>
       <c r="R25" s="54">
-        <f t="shared" ref="R25:R27" si="61">O25*0.14296</f>
+        <f t="shared" ref="R25:R27" si="65">O25*0.14296</f>
         <v>27.30536</v>
       </c>
       <c r="S25" s="54">
-        <f t="shared" ref="S25:S27" si="62">R25+Q25</f>
+        <f t="shared" ref="S25:S27" si="66">R25+Q25</f>
         <v>11.78084</v>
       </c>
       <c r="T25" s="54">
@@ -4000,19 +4001,19 @@
         <v>-1.32</v>
       </c>
       <c r="U25" s="15">
-        <f t="shared" ref="U25:U27" si="63">(ABS(Q25)+ABS(R25))/(ABS(N25)+ABS(O25))</f>
+        <f t="shared" ref="U25:U27" si="67">(ABS(Q25)+ABS(R25))/(ABS(N25)+ABS(O25))</f>
         <v>0.13260024767801859</v>
       </c>
       <c r="V25" s="16">
-        <f t="shared" ref="V25:V27" si="64">ABS(R25)/ABS(O25)</f>
+        <f t="shared" ref="V25:V27" si="68">ABS(R25)/ABS(O25)</f>
         <v>0.14296</v>
       </c>
       <c r="W25" s="16">
-        <f t="shared" ref="W25:W27" si="65">Q25/N25</f>
+        <f t="shared" ref="W25:W27" si="69">Q25/N25</f>
         <v>0.11761000000000001</v>
       </c>
       <c r="X25" s="17">
-        <f t="shared" ref="X25:X26" si="66">Q25+R25+T25+0.02</f>
+        <f t="shared" ref="X25:X26" si="70">Q25+R25+T25+0.02</f>
         <v>10.480839999999999</v>
       </c>
       <c r="Y25" s="18">
@@ -4031,7 +4032,7 @@
         <v>3.43</v>
       </c>
       <c r="AD25" s="17">
-        <f t="shared" ref="AD25:AD27" si="67">AC25+AB25+AA25</f>
+        <f t="shared" ref="AD25:AD27" si="71">AC25+AB25+AA25</f>
         <v>25.380000000000003</v>
       </c>
       <c r="AE25" s="54">
@@ -4044,7 +4045,7 @@
         <v>0</v>
       </c>
       <c r="AH25" s="55">
-        <f t="shared" ref="AH25:AH27" si="68">AE25+AF25+AG25</f>
+        <f t="shared" ref="AH25:AH27" si="72">AE25+AF25+AG25</f>
         <v>21.36</v>
       </c>
       <c r="AI25" s="56"/>
@@ -4081,19 +4082,19 @@
         <v>157</v>
       </c>
       <c r="AT25" s="53">
-        <f t="shared" ref="AT25:AT27" si="69">AS25+AR25</f>
+        <f t="shared" ref="AT25:AT27" si="73">AS25+AR25</f>
         <v>22</v>
       </c>
       <c r="AU25" s="54">
-        <f t="shared" ref="AU25:AU27" si="70">AR25*0.11761</f>
+        <f t="shared" ref="AU25:AU27" si="74">AR25*0.11761</f>
         <v>-15.877350000000002</v>
       </c>
       <c r="AV25" s="54">
-        <f t="shared" ref="AV25:AV27" si="71">AS25*0.14296</f>
+        <f t="shared" ref="AV25:AV27" si="75">AS25*0.14296</f>
         <v>22.44472</v>
       </c>
       <c r="AW25" s="54">
-        <f t="shared" ref="AW25:AW27" si="72">AV25+AU25</f>
+        <f t="shared" ref="AW25:AW27" si="76">AV25+AU25</f>
         <v>6.5673699999999986</v>
       </c>
       <c r="AX25" s="54">
@@ -4104,7 +4105,7 @@
         <v>0.01</v>
       </c>
       <c r="AZ25" s="17">
-        <f t="shared" ref="AZ25:AZ27" si="73">AY25+AX25+AW25</f>
+        <f t="shared" ref="AZ25:AZ27" si="77">AY25+AX25+AW25</f>
         <v>5.2273699999999987</v>
       </c>
       <c r="BA25" s="18">
@@ -4118,24 +4119,24 @@
       </c>
       <c r="BD25" s="54"/>
       <c r="BE25" s="21">
-        <f t="shared" ref="BE25:BE27" si="74">BC25+BB25+BD25</f>
+        <f t="shared" ref="BE25:BE27" si="78">BC25+BB25+BD25</f>
         <v>11.36</v>
       </c>
     </row>
     <row r="26" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="9">
-        <v>45996</v>
+        <v>45631</v>
       </c>
       <c r="C26" s="10">
         <v>45643</v>
       </c>
       <c r="D26" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>-605</v>
       </c>
       <c r="E26" s="11">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="F26" s="12">
@@ -4160,7 +4161,7 @@
         <v>-206</v>
       </c>
       <c r="M26" s="13">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>0.34049586776859503</v>
       </c>
       <c r="N26" s="11">
@@ -4170,38 +4171,38 @@
         <v>214</v>
       </c>
       <c r="P26" s="11">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>358</v>
       </c>
       <c r="Q26" s="14">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>16.935840000000002</v>
       </c>
       <c r="R26" s="14">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>30.593440000000001</v>
       </c>
       <c r="S26" s="14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>47.52928</v>
       </c>
       <c r="T26" s="14">
         <v>0</v>
       </c>
       <c r="U26" s="15">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>0.13276335195530725</v>
       </c>
       <c r="V26" s="16">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>0.14296</v>
       </c>
       <c r="W26" s="16">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.11761000000000002</v>
       </c>
       <c r="X26" s="17">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>47.549280000000003</v>
       </c>
       <c r="Y26" s="18">
@@ -4220,7 +4221,7 @@
         <v>8.11</v>
       </c>
       <c r="AD26" s="17">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>92.03</v>
       </c>
       <c r="AE26" s="14">
@@ -4233,7 +4234,7 @@
         <v>0</v>
       </c>
       <c r="AH26" s="20">
-        <f t="shared" si="68"/>
+        <f t="shared" si="72"/>
         <v>22.14</v>
       </c>
       <c r="AI26" s="57"/>
@@ -4242,11 +4243,11 @@
         <v>22.14</v>
       </c>
       <c r="AK26" s="11">
-        <f t="shared" ref="AK26:AL26" si="75">AR26-AN26</f>
+        <f t="shared" ref="AK26:AL26" si="79">AR26-AN26</f>
         <v>599</v>
       </c>
       <c r="AL26" s="11">
-        <f t="shared" si="75"/>
+        <f t="shared" si="79"/>
         <v>242</v>
       </c>
       <c r="AM26" s="12">
@@ -4274,19 +4275,19 @@
         <v>242</v>
       </c>
       <c r="AT26" s="11">
-        <f t="shared" si="69"/>
+        <f t="shared" si="73"/>
         <v>442</v>
       </c>
       <c r="AU26" s="14">
-        <f t="shared" si="70"/>
+        <f t="shared" si="74"/>
         <v>23.522000000000002</v>
       </c>
       <c r="AV26" s="14">
-        <f t="shared" si="71"/>
+        <f t="shared" si="75"/>
         <v>34.596319999999999</v>
       </c>
       <c r="AW26" s="14">
-        <f t="shared" si="72"/>
+        <f t="shared" si="76"/>
         <v>58.118319999999997</v>
       </c>
       <c r="AX26" s="14">
@@ -4296,7 +4297,7 @@
         <v>0.13</v>
       </c>
       <c r="AZ26" s="17">
-        <f t="shared" si="73"/>
+        <f t="shared" si="77"/>
         <v>58.24832</v>
       </c>
       <c r="BA26" s="18">
@@ -4310,7 +4311,7 @@
       </c>
       <c r="BD26" s="14"/>
       <c r="BE26" s="21">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>12.14</v>
       </c>
     </row>
@@ -4323,40 +4324,40 @@
         <v>45673</v>
       </c>
       <c r="D27" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="60"/>
         <v>-309</v>
       </c>
       <c r="E27" s="11">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="F27" s="12">
         <v>-309</v>
       </c>
       <c r="G27" s="11">
-        <f t="shared" ref="G27:H27" si="76">G28+G29</f>
+        <f t="shared" ref="G27:H27" si="80">G28+G29</f>
         <v>489</v>
       </c>
       <c r="H27" s="11">
-        <f t="shared" si="76"/>
+        <f t="shared" si="80"/>
         <v>332</v>
       </c>
       <c r="I27" s="12">
         <v>821</v>
       </c>
       <c r="J27" s="11">
-        <f t="shared" ref="J27:K27" si="77">J28+J29</f>
+        <f t="shared" ref="J27:K27" si="81">J28+J29</f>
         <v>-210</v>
       </c>
       <c r="K27" s="11">
-        <f t="shared" si="77"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="L27" s="12">
         <v>-210</v>
       </c>
       <c r="M27" s="13">
-        <f t="shared" si="58"/>
+        <f t="shared" si="62"/>
         <v>0.67961165048543692</v>
       </c>
       <c r="N27" s="11">
@@ -4366,34 +4367,34 @@
         <v>332</v>
       </c>
       <c r="P27" s="11">
-        <f t="shared" si="59"/>
+        <f t="shared" si="63"/>
         <v>611</v>
       </c>
       <c r="Q27" s="14">
-        <f t="shared" si="60"/>
+        <f t="shared" si="64"/>
         <v>32.813189999999999</v>
       </c>
       <c r="R27" s="14">
-        <f t="shared" si="61"/>
+        <f t="shared" si="65"/>
         <v>47.462720000000004</v>
       </c>
       <c r="S27" s="14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="66"/>
         <v>80.27591000000001</v>
       </c>
       <c r="T27" s="14">
         <v>0</v>
       </c>
       <c r="U27" s="15">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>0.1313844680851064</v>
       </c>
       <c r="V27" s="16">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>0.14296</v>
       </c>
       <c r="W27" s="16">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.11760999999999999</v>
       </c>
       <c r="X27" s="17">
@@ -4416,7 +4417,7 @@
         <v>12.56</v>
       </c>
       <c r="AD27" s="17">
-        <f t="shared" si="67"/>
+        <f t="shared" si="71"/>
         <v>172.51999999999998</v>
       </c>
       <c r="AE27" s="14">
@@ -4429,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="AH27" s="20">
-        <f t="shared" si="68"/>
+        <f t="shared" si="72"/>
         <v>22.53</v>
       </c>
       <c r="AI27" s="57"/>
@@ -4438,11 +4439,11 @@
         <v>22.53</v>
       </c>
       <c r="AK27" s="11">
-        <f t="shared" ref="AK27:AL27" si="78">AR27-AN27</f>
+        <f t="shared" ref="AK27:AL27" si="82">AR27-AN27</f>
         <v>693</v>
       </c>
       <c r="AL27" s="11">
-        <f t="shared" si="78"/>
+        <f t="shared" si="82"/>
         <v>231</v>
       </c>
       <c r="AM27" s="12">
@@ -4470,19 +4471,19 @@
         <v>231</v>
       </c>
       <c r="AT27" s="11">
-        <f t="shared" si="69"/>
+        <f t="shared" si="73"/>
         <v>825</v>
       </c>
       <c r="AU27" s="14">
-        <f t="shared" si="70"/>
+        <f t="shared" si="74"/>
         <v>69.860340000000008</v>
       </c>
       <c r="AV27" s="14">
-        <f t="shared" si="71"/>
+        <f t="shared" si="75"/>
         <v>33.023760000000003</v>
       </c>
       <c r="AW27" s="14">
-        <f t="shared" si="72"/>
+        <f t="shared" si="76"/>
         <v>102.88410000000002</v>
       </c>
       <c r="AX27" s="14">
@@ -4492,7 +4493,7 @@
         <v>0.25</v>
       </c>
       <c r="AZ27" s="17">
-        <f t="shared" si="73"/>
+        <f t="shared" si="77"/>
         <v>103.13410000000002</v>
       </c>
       <c r="BA27" s="19">
@@ -4506,7 +4507,7 @@
       </c>
       <c r="BD27" s="14"/>
       <c r="BE27" s="21">
-        <f t="shared" si="74"/>
+        <f t="shared" si="78"/>
         <v>12.53</v>
       </c>
     </row>
@@ -4710,15 +4711,15 @@
         <v>-10</v>
       </c>
       <c r="U30" s="15">
-        <f t="shared" ref="U30:U31" si="79">(ABS(Q30)+ABS(R30))/(ABS(N30)+ABS(O30))</f>
+        <f t="shared" ref="U30:U31" si="83">(ABS(Q30)+ABS(R30))/(ABS(N30)+ABS(O30))</f>
         <v>0.12236459709379127</v>
       </c>
       <c r="V30" s="16">
-        <f t="shared" ref="V30:V31" si="80">ABS(R30)/ABS(O30)</f>
+        <f t="shared" ref="V30:V31" si="84">ABS(R30)/ABS(O30)</f>
         <v>0.14295774647887324</v>
       </c>
       <c r="W30" s="16">
-        <f t="shared" ref="W30:W31" si="81">Q30/N30</f>
+        <f t="shared" ref="W30:W31" si="85">Q30/N30</f>
         <v>0.11760975609756097</v>
       </c>
       <c r="X30" s="17">
@@ -4755,7 +4756,7 @@
         <v>0</v>
       </c>
       <c r="AH30" s="20">
-        <f t="shared" ref="AH30:AH31" si="82">AE30+AF30+AG30</f>
+        <f t="shared" ref="AH30:AH31" si="86">AE30+AF30+AG30</f>
         <v>21.36</v>
       </c>
       <c r="AI30" s="57"/>
@@ -4764,11 +4765,11 @@
         <v>89.57</v>
       </c>
       <c r="AK30" s="11">
-        <f t="shared" ref="AK30:AL30" si="83">AR30-AN30</f>
+        <f t="shared" ref="AK30:AL30" si="87">AR30-AN30</f>
         <v>732</v>
       </c>
       <c r="AL30" s="11">
-        <f t="shared" si="83"/>
+        <f t="shared" si="87"/>
         <v>9</v>
       </c>
       <c r="AM30" s="12">
@@ -4795,7 +4796,7 @@
         <v>199</v>
       </c>
       <c r="AT30" s="11">
-        <f t="shared" ref="AT30:AT32" si="84">AS30+AR30</f>
+        <f t="shared" ref="AT30:AT32" si="88">AS30+AR30</f>
         <v>931</v>
       </c>
       <c r="AU30" s="14">
@@ -4807,7 +4808,7 @@
         <v>28.44904</v>
       </c>
       <c r="AW30" s="14">
-        <f t="shared" ref="AW30:AW31" si="85">AV30+AU30</f>
+        <f t="shared" ref="AW30:AW31" si="89">AV30+AU30</f>
         <v>114.53955999999999</v>
       </c>
       <c r="AX30" s="14">
@@ -4817,7 +4818,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="AZ30" s="17">
-        <f t="shared" ref="AZ30:AZ31" si="86">AY30+AX30+AW30</f>
+        <f t="shared" ref="AZ30:AZ31" si="90">AY30+AX30+AW30</f>
         <v>114.81956</v>
       </c>
       <c r="BA30" s="18">
@@ -4831,7 +4832,7 @@
       </c>
       <c r="BD30" s="14"/>
       <c r="BE30" s="21">
-        <f t="shared" ref="BE30:BE31" si="87">BC30+BB30+BD30</f>
+        <f t="shared" ref="BE30:BE31" si="91">BC30+BB30+BD30</f>
         <v>88.07</v>
       </c>
     </row>
@@ -4855,22 +4856,22 @@
         <v>-762</v>
       </c>
       <c r="G31" s="11">
-        <f t="shared" ref="G31:H31" si="88">G32+G33</f>
+        <f t="shared" ref="G31:H31" si="92">G32+G33</f>
         <v>321</v>
       </c>
       <c r="H31" s="11">
-        <f t="shared" si="88"/>
+        <f t="shared" si="92"/>
         <v>286</v>
       </c>
       <c r="I31" s="12">
         <v>607</v>
       </c>
       <c r="J31" s="11">
-        <f t="shared" ref="J31:K31" si="89">J32+J33</f>
+        <f t="shared" ref="J31:K31" si="93">J32+J33</f>
         <v>-304</v>
       </c>
       <c r="K31" s="11">
-        <f t="shared" si="89"/>
+        <f t="shared" si="93"/>
         <v>-1</v>
       </c>
       <c r="L31" s="12">
@@ -4890,30 +4891,30 @@
         <v>302</v>
       </c>
       <c r="Q31" s="20">
-        <f t="shared" ref="Q31:S31" si="90">Q32+Q33</f>
+        <f t="shared" ref="Q31:S31" si="94">Q32+Q33</f>
         <v>1.9100000000000001</v>
       </c>
       <c r="R31" s="20">
-        <f t="shared" si="90"/>
+        <f t="shared" si="94"/>
         <v>38.949999999999996</v>
       </c>
       <c r="S31" s="20">
-        <f t="shared" si="90"/>
+        <f t="shared" si="94"/>
         <v>40.859999999999992</v>
       </c>
       <c r="T31" s="20">
         <v>0</v>
       </c>
       <c r="U31" s="15">
-        <f t="shared" si="79"/>
+        <f t="shared" si="83"/>
         <v>0.1352980132450331</v>
       </c>
       <c r="V31" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="84"/>
         <v>0.13666666666666666</v>
       </c>
       <c r="W31" s="16">
-        <f t="shared" si="81"/>
+        <f t="shared" si="85"/>
         <v>0.1123529411764706</v>
       </c>
       <c r="X31" s="17">
@@ -4948,7 +4949,7 @@
         <v>0</v>
       </c>
       <c r="AH31" s="20">
-        <f t="shared" si="82"/>
+        <f t="shared" si="86"/>
         <v>21.82</v>
       </c>
       <c r="AI31" s="11"/>
@@ -4957,11 +4958,11 @@
         <v>62.77</v>
       </c>
       <c r="AK31" s="11">
-        <f t="shared" ref="AK31:AL31" si="91">AR31-AN31</f>
+        <f t="shared" ref="AK31:AL31" si="95">AR31-AN31</f>
         <v>592</v>
       </c>
       <c r="AL31" s="11">
-        <f t="shared" si="91"/>
+        <f t="shared" si="95"/>
         <v>242</v>
       </c>
       <c r="AM31" s="12">
@@ -4983,27 +4984,27 @@
         <v>0.59973753280839892</v>
       </c>
       <c r="AR31" s="11">
-        <f t="shared" ref="AR31:AS31" si="92">AR32+AR33</f>
+        <f t="shared" ref="AR31:AS31" si="96">AR32+AR33</f>
         <v>136</v>
       </c>
       <c r="AS31" s="11">
-        <f t="shared" si="92"/>
+        <f t="shared" si="96"/>
         <v>241</v>
       </c>
       <c r="AT31" s="11">
-        <f t="shared" si="84"/>
+        <f t="shared" si="88"/>
         <v>377</v>
       </c>
       <c r="AU31" s="14">
-        <f t="shared" ref="AU31:AV31" si="93">AU32+AU33</f>
+        <f t="shared" ref="AU31:AV31" si="97">AU32+AU33</f>
         <v>15.293426873</v>
       </c>
       <c r="AV31" s="14">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>32.941085250999997</v>
       </c>
       <c r="AW31" s="14">
-        <f t="shared" si="85"/>
+        <f t="shared" si="89"/>
         <v>48.234512123999998</v>
       </c>
       <c r="AX31" s="14">
@@ -5013,7 +5014,7 @@
         <v>0.11</v>
       </c>
       <c r="AZ31" s="17">
-        <f t="shared" si="86"/>
+        <f t="shared" si="90"/>
         <v>48.344512123999998</v>
       </c>
       <c r="BA31" s="19">
@@ -5028,7 +5029,7 @@
       </c>
       <c r="BD31" s="14"/>
       <c r="BE31" s="21">
-        <f t="shared" si="87"/>
+        <f t="shared" si="91"/>
         <v>60.164512123999998</v>
       </c>
     </row>
@@ -5066,7 +5067,7 @@
         <v>32.159999999999997</v>
       </c>
       <c r="S32" s="44">
-        <f t="shared" ref="S32:S33" si="94">Q32+R32</f>
+        <f t="shared" ref="S32:S33" si="98">Q32+R32</f>
         <v>33.739999999999995</v>
       </c>
       <c r="T32" s="44"/>
@@ -5100,7 +5101,7 @@
         <v>200.83330000000001</v>
       </c>
       <c r="AT32" s="44">
-        <f t="shared" si="84"/>
+        <f t="shared" si="88"/>
         <v>314.16660000000002</v>
       </c>
       <c r="AU32" s="43">
@@ -5155,7 +5156,7 @@
         <v>6.79</v>
       </c>
       <c r="S33" s="44">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>7.12</v>
       </c>
       <c r="T33" s="44"/>
@@ -5332,22 +5333,22 @@
         <v>207.22</v>
       </c>
       <c r="AK34" s="11">
-        <f t="shared" ref="AK34:AL34" si="95">AR34-AN34</f>
+        <f t="shared" ref="AK34:AL34" si="99">AR34-AN34</f>
         <v>582</v>
       </c>
       <c r="AL34" s="11">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>212</v>
       </c>
       <c r="AM34" s="12">
         <v>794</v>
       </c>
       <c r="AN34" s="11">
-        <f t="shared" ref="AN34:AO34" si="96">D34-J34</f>
+        <f t="shared" ref="AN34:AO34" si="100">D34-J34</f>
         <v>-670</v>
       </c>
       <c r="AO34" s="11">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>-60</v>
       </c>
       <c r="AP34" s="12">
@@ -5404,51 +5405,51 @@
         <v>321.20999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y35" s="68"/>
+      <c r="AD35" s="68"/>
+    </row>
     <row r="36" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y36" s="68"/>
-      <c r="AD36" s="68"/>
+      <c r="V36" s="68"/>
+      <c r="W36" s="68"/>
+      <c r="X36" s="68"/>
     </row>
     <row r="37" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="V37" s="68"/>
-      <c r="W37" s="68"/>
-      <c r="X37" s="68"/>
+      <c r="Z37" s="69"/>
+      <c r="AA37" s="69"/>
     </row>
     <row r="38" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Z38" s="69"/>
-      <c r="AA38" s="69"/>
+      <c r="T38" s="70"/>
+      <c r="Y38" s="68"/>
+      <c r="Z38" s="71"/>
+      <c r="AA38" s="68"/>
     </row>
     <row r="39" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P39" s="68"/>
       <c r="T39" s="70"/>
-      <c r="Y39" s="68"/>
       <c r="Z39" s="71"/>
       <c r="AA39" s="68"/>
     </row>
-    <row r="40" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="P40" s="68"/>
-      <c r="T40" s="70"/>
-      <c r="Z40" s="71"/>
-      <c r="AA40" s="68"/>
+    <row r="40" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T41" s="70"/>
     </row>
-    <row r="41" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="T42" s="70"/>
+    <row r="42" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T43" s="70"/>
+      <c r="Z43" s="68"/>
+      <c r="AA43" s="68"/>
     </row>
-    <row r="43" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="T44" s="70"/>
-      <c r="Z44" s="68"/>
-      <c r="AA44" s="68"/>
+    <row r="44" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Z45" s="68"/>
+      <c r="AA45" s="68"/>
     </row>
-    <row r="45" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z46" s="68"/>
       <c r="AA46" s="68"/>
     </row>
-    <row r="47" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Z47" s="68"/>
-      <c r="AA47" s="68"/>
-    </row>
+    <row r="47" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6414,7 +6415,6 @@
     <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1013" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="B3:C3"/>

</xml_diff>

<commit_message>
minor color formatting changes to billing excel sheet
</commit_message>
<xml_diff>
--- a/python-notebooks/billing.xlsx
+++ b/python-notebooks/billing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\klowe\go\src\stash.teslamotors.com\kevin-personal\energy-project\python-notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382BDCC1-CF79-4A16-A1F6-BCD21D8EED3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE071BFE-75F7-4F88-8193-446CAE5A2EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,6 +574,42 @@
         <bgColor rgb="FFB3E5A1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFC1E4F5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -601,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -705,6 +741,16 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="6" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="6" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,9 +968,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AU4" sqref="AU4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1939,11 +1985,11 @@
         <v>0.50093691442848221</v>
       </c>
       <c r="AR8" s="16">
-        <f t="shared" ref="AR8:AV8" si="20">AR9+AR10</f>
+        <f>AR9+AR10</f>
         <v>-358</v>
       </c>
       <c r="AS8" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="AR8:AV8" si="20">AS9+AS10</f>
         <v>7</v>
       </c>
       <c r="AT8" s="16">
@@ -2046,26 +2092,26 @@
       <c r="AF9" s="32"/>
       <c r="AG9" s="32"/>
       <c r="AH9" s="32"/>
-      <c r="AI9" s="32"/>
-      <c r="AJ9" s="32"/>
-      <c r="AK9" s="16">
+      <c r="AI9" s="77"/>
+      <c r="AJ9" s="77"/>
+      <c r="AK9" s="78">
         <f t="shared" ref="AK9:AL9" si="23">AR9-AN9</f>
         <v>-842</v>
       </c>
-      <c r="AL9" s="16">
+      <c r="AL9" s="78">
         <f t="shared" si="23"/>
         <v>-64</v>
       </c>
-      <c r="AM9" s="29"/>
-      <c r="AN9" s="16">
+      <c r="AM9" s="79"/>
+      <c r="AN9" s="78">
         <f t="shared" si="8"/>
         <v>573</v>
       </c>
-      <c r="AO9" s="16">
+      <c r="AO9" s="78">
         <f t="shared" si="9"/>
         <v>77</v>
       </c>
-      <c r="AP9" s="29"/>
+      <c r="AP9" s="79"/>
       <c r="AQ9" s="29"/>
       <c r="AR9" s="29">
         <v>-269</v>
@@ -2153,26 +2199,26 @@
       <c r="AF10" s="32"/>
       <c r="AG10" s="32"/>
       <c r="AH10" s="32"/>
-      <c r="AI10" s="32"/>
-      <c r="AJ10" s="32"/>
-      <c r="AK10" s="16">
+      <c r="AI10" s="77"/>
+      <c r="AJ10" s="77"/>
+      <c r="AK10" s="78">
         <f t="shared" ref="AK10:AL10" si="27">AR10-AN10</f>
         <v>-220</v>
       </c>
-      <c r="AL10" s="16">
+      <c r="AL10" s="78">
         <f t="shared" si="27"/>
         <v>-24</v>
       </c>
-      <c r="AM10" s="29"/>
-      <c r="AN10" s="16">
+      <c r="AM10" s="79"/>
+      <c r="AN10" s="78">
         <f t="shared" si="8"/>
         <v>131</v>
       </c>
-      <c r="AO10" s="16">
+      <c r="AO10" s="78">
         <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="AP10" s="29"/>
+      <c r="AP10" s="79"/>
       <c r="AQ10" s="29"/>
       <c r="AR10" s="29">
         <v>-89</v>
@@ -2446,26 +2492,26 @@
       <c r="AG12" s="39"/>
       <c r="AH12" s="39"/>
       <c r="AI12" s="39"/>
-      <c r="AJ12" s="39"/>
-      <c r="AK12" s="16">
+      <c r="AJ12" s="80"/>
+      <c r="AK12" s="81">
         <f t="shared" ref="AK12:AL12" si="33">AR12-AN12</f>
         <v>-775</v>
       </c>
-      <c r="AL12" s="16">
+      <c r="AL12" s="81">
         <f t="shared" si="33"/>
         <v>-109</v>
       </c>
-      <c r="AM12" s="35"/>
-      <c r="AN12" s="16">
+      <c r="AM12" s="82"/>
+      <c r="AN12" s="81">
         <f t="shared" si="8"/>
         <v>775</v>
       </c>
-      <c r="AO12" s="16">
+      <c r="AO12" s="81">
         <f t="shared" si="9"/>
         <v>109</v>
       </c>
-      <c r="AP12" s="35"/>
-      <c r="AQ12" s="35"/>
+      <c r="AP12" s="82"/>
+      <c r="AQ12" s="82"/>
       <c r="AR12" s="35"/>
       <c r="AS12" s="35"/>
       <c r="AT12" s="35"/>
@@ -2527,26 +2573,26 @@
       <c r="AG13" s="39"/>
       <c r="AH13" s="39"/>
       <c r="AI13" s="39"/>
-      <c r="AJ13" s="39"/>
-      <c r="AK13" s="16">
+      <c r="AJ13" s="80"/>
+      <c r="AK13" s="81">
         <f t="shared" ref="AK13:AL13" si="34">AR13-AN13</f>
         <v>-226</v>
       </c>
-      <c r="AL13" s="16">
+      <c r="AL13" s="81">
         <f t="shared" si="34"/>
         <v>-22</v>
       </c>
-      <c r="AM13" s="35"/>
-      <c r="AN13" s="16">
+      <c r="AM13" s="82"/>
+      <c r="AN13" s="81">
         <f t="shared" si="8"/>
         <v>226</v>
       </c>
-      <c r="AO13" s="16">
+      <c r="AO13" s="81">
         <f t="shared" si="9"/>
         <v>22</v>
       </c>
-      <c r="AP13" s="35"/>
-      <c r="AQ13" s="35"/>
+      <c r="AP13" s="82"/>
+      <c r="AQ13" s="82"/>
       <c r="AR13" s="35"/>
       <c r="AS13" s="35"/>
       <c r="AT13" s="35"/>
@@ -2811,25 +2857,25 @@
       <c r="AG15" s="46"/>
       <c r="AH15" s="46"/>
       <c r="AI15" s="46"/>
-      <c r="AJ15" s="46"/>
-      <c r="AK15" s="41">
+      <c r="AJ15" s="83"/>
+      <c r="AK15" s="84">
         <f t="shared" ref="AK15:AL15" si="40">AR15-AN15</f>
         <v>-64.965500000000006</v>
       </c>
-      <c r="AL15" s="41">
+      <c r="AL15" s="84">
         <f t="shared" si="40"/>
         <v>20.620699999999999</v>
       </c>
-      <c r="AM15" s="46"/>
-      <c r="AN15" s="41">
+      <c r="AM15" s="83"/>
+      <c r="AN15" s="84">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AO15" s="41">
+      <c r="AO15" s="84">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AP15" s="47"/>
+      <c r="AP15" s="85"/>
       <c r="AQ15" s="48"/>
       <c r="AR15" s="43">
         <v>-64.965500000000006</v>
@@ -2910,25 +2956,25 @@
       <c r="AG16" s="46"/>
       <c r="AH16" s="46"/>
       <c r="AI16" s="46"/>
-      <c r="AJ16" s="46"/>
-      <c r="AK16" s="41">
+      <c r="AJ16" s="83"/>
+      <c r="AK16" s="84">
         <f t="shared" ref="AK16:AL16" si="43">AR16-AN16</f>
         <v>-249.03450000000001</v>
       </c>
-      <c r="AL16" s="41">
+      <c r="AL16" s="84">
         <f t="shared" si="43"/>
         <v>5.3792999999999997</v>
       </c>
-      <c r="AM16" s="46"/>
-      <c r="AN16" s="41">
+      <c r="AM16" s="83"/>
+      <c r="AN16" s="84">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AO16" s="41">
+      <c r="AO16" s="84">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AP16" s="47"/>
+      <c r="AP16" s="85"/>
       <c r="AQ16" s="45"/>
       <c r="AR16" s="47">
         <v>-249.03450000000001</v>
@@ -3345,25 +3391,25 @@
       <c r="AG20" s="32"/>
       <c r="AH20" s="32"/>
       <c r="AI20" s="32"/>
-      <c r="AJ20" s="32"/>
-      <c r="AK20" s="16">
+      <c r="AJ20" s="77"/>
+      <c r="AK20" s="78">
         <f t="shared" ref="AK20:AL20" si="49">AR20-AN20</f>
         <v>-275</v>
       </c>
-      <c r="AL20" s="16">
+      <c r="AL20" s="78">
         <f t="shared" si="49"/>
         <v>99</v>
       </c>
-      <c r="AM20" s="29"/>
-      <c r="AN20" s="16">
+      <c r="AM20" s="79"/>
+      <c r="AN20" s="78">
         <f t="shared" ref="AN20:AO22" si="50">D20-J20</f>
         <v>0</v>
       </c>
-      <c r="AO20" s="16">
+      <c r="AO20" s="78">
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="AP20" s="29"/>
+      <c r="AP20" s="79"/>
       <c r="AQ20" s="31"/>
       <c r="AR20" s="29">
         <v>-275</v>
@@ -3383,22 +3429,15 @@
         <f>AS20*0.20001</f>
         <v>19.800989999999999</v>
       </c>
-      <c r="AW20" s="32"/>
-      <c r="AX20" s="32"/>
-      <c r="AY20" s="32"/>
-      <c r="AZ20" s="22"/>
-      <c r="BA20" s="23">
-        <v>0</v>
-      </c>
-      <c r="BB20" s="23">
-        <v>0</v>
-      </c>
-      <c r="BC20" s="22"/>
-      <c r="BD20" s="32"/>
-      <c r="BE20" s="26">
-        <f t="shared" ref="BE20:BE22" si="52">BC20+BB20+BD20</f>
-        <v>0</v>
-      </c>
+      <c r="AW20" s="77"/>
+      <c r="AX20" s="77"/>
+      <c r="AY20" s="77"/>
+      <c r="AZ20" s="86"/>
+      <c r="BA20" s="86"/>
+      <c r="BB20" s="86"/>
+      <c r="BC20" s="86"/>
+      <c r="BD20" s="77"/>
+      <c r="BE20" s="77"/>
     </row>
     <row r="21" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
@@ -3451,25 +3490,25 @@
       <c r="AG21" s="32"/>
       <c r="AH21" s="32"/>
       <c r="AI21" s="32"/>
-      <c r="AJ21" s="32"/>
-      <c r="AK21" s="16">
-        <f t="shared" ref="AK21:AL21" si="53">AR21-AN21</f>
+      <c r="AJ21" s="77"/>
+      <c r="AK21" s="78">
+        <f t="shared" ref="AK21:AL21" si="52">AR21-AN21</f>
         <v>-46</v>
       </c>
-      <c r="AL21" s="16">
-        <f t="shared" si="53"/>
+      <c r="AL21" s="78">
+        <f t="shared" si="52"/>
         <v>33</v>
       </c>
-      <c r="AM21" s="29"/>
-      <c r="AN21" s="16">
+      <c r="AM21" s="79"/>
+      <c r="AN21" s="78">
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="AO21" s="16">
+      <c r="AO21" s="78">
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="AP21" s="29"/>
+      <c r="AP21" s="79"/>
       <c r="AQ21" s="31"/>
       <c r="AR21" s="29">
         <v>-46</v>
@@ -3489,22 +3528,15 @@
         <f>AS21*0.14296</f>
         <v>4.7176800000000005</v>
       </c>
-      <c r="AW21" s="32"/>
-      <c r="AX21" s="32"/>
-      <c r="AY21" s="32"/>
-      <c r="AZ21" s="22"/>
-      <c r="BA21" s="23">
-        <v>0</v>
-      </c>
-      <c r="BB21" s="23">
-        <v>0</v>
-      </c>
-      <c r="BC21" s="22"/>
-      <c r="BD21" s="32"/>
-      <c r="BE21" s="26">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
+      <c r="AW21" s="77"/>
+      <c r="AX21" s="77"/>
+      <c r="AY21" s="77"/>
+      <c r="AZ21" s="86"/>
+      <c r="BA21" s="86"/>
+      <c r="BB21" s="86"/>
+      <c r="BC21" s="86"/>
+      <c r="BD21" s="77"/>
+      <c r="BE21" s="77"/>
     </row>
     <row r="22" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
@@ -3526,22 +3558,22 @@
         <v>-1292</v>
       </c>
       <c r="G22" s="16">
-        <f t="shared" ref="G22:H22" si="54">G23+G24</f>
+        <f t="shared" ref="G22:H22" si="53">G23+G24</f>
         <v>191</v>
       </c>
       <c r="H22" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="53"/>
         <v>157</v>
       </c>
       <c r="I22" s="17">
         <v>348</v>
       </c>
       <c r="J22" s="16">
-        <f t="shared" ref="J22:K22" si="55">J23+J24</f>
+        <f t="shared" ref="J22:K22" si="54">J23+J24</f>
         <v>-334</v>
       </c>
       <c r="K22" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="54"/>
         <v>-26</v>
       </c>
       <c r="L22" s="17">
@@ -3552,11 +3584,11 @@
         <v>0.27863777089783281</v>
       </c>
       <c r="N22" s="16">
-        <f t="shared" ref="N22:O22" si="56">N21+N20</f>
+        <f t="shared" ref="N22:O22" si="55">N21+N20</f>
         <v>-143</v>
       </c>
       <c r="O22" s="16">
-        <f t="shared" si="56"/>
+        <f t="shared" si="55"/>
         <v>131</v>
       </c>
       <c r="P22" s="16">
@@ -3564,11 +3596,11 @@
         <v>-12</v>
       </c>
       <c r="Q22" s="19">
-        <f t="shared" ref="Q22:R22" si="57">Q20+Q21</f>
+        <f t="shared" ref="Q22:R22" si="56">Q20+Q21</f>
         <v>-17.332979999999999</v>
       </c>
       <c r="R22" s="19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="56"/>
         <v>22.664209999999997</v>
       </c>
       <c r="S22" s="19">
@@ -3635,11 +3667,11 @@
         <v>-33.03</v>
       </c>
       <c r="AK22" s="16">
-        <f t="shared" ref="AK22:AL22" si="58">AR22-AN22</f>
+        <f t="shared" ref="AK22:AL22" si="57">AR22-AN22</f>
         <v>544</v>
       </c>
       <c r="AL22" s="16">
-        <f t="shared" si="58"/>
+        <f t="shared" si="57"/>
         <v>199</v>
       </c>
       <c r="AM22" s="17">
@@ -3673,11 +3705,11 @@
         <v>-189</v>
       </c>
       <c r="AU22" s="19">
-        <f t="shared" ref="AU22:AV22" si="59">AU20+AU21</f>
+        <f t="shared" ref="AU22:AV22" si="58">AU20+AU21</f>
         <v>-38.729060000000004</v>
       </c>
       <c r="AV22" s="19">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>24.51867</v>
       </c>
       <c r="AW22" s="19">
@@ -3708,7 +3740,7 @@
         <v>-55.17</v>
       </c>
       <c r="BE22" s="26">
-        <f t="shared" si="52"/>
+        <f t="shared" ref="BE20:BE22" si="59">BC22+BB22+BD22</f>
         <v>-43.03</v>
       </c>
     </row>

</xml_diff>

<commit_message>
realizing that I don't actually know the peak and off peak usage on meter channel 1 for the ADU. Formatting in red
</commit_message>
<xml_diff>
--- a/python-notebooks/billing.xlsx
+++ b/python-notebooks/billing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\klowe\go\src\stash.teslamotors.com\kevin-personal\energy-project\python-notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE071BFE-75F7-4F88-8193-446CAE5A2EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8206FA0C-29F0-4133-AE10-3C08CFB3219D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -610,6 +610,18 @@
         <bgColor rgb="FFC1E4F5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -637,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -722,6 +734,19 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="6" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="6" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="6" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -741,16 +766,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="6" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="6" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="6" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="6" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,9 +983,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AQ19" sqref="AQ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1023,150 +1038,150 @@
       <c r="A2" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="71" t="s">
+      <c r="C2" s="83"/>
+      <c r="D2" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="71"/>
-      <c r="Z2" s="71"/>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="71"/>
-      <c r="AC2" s="71"/>
-      <c r="AD2" s="71"/>
-      <c r="AE2" s="71"/>
-      <c r="AF2" s="71"/>
-      <c r="AG2" s="71"/>
-      <c r="AH2" s="71"/>
-      <c r="AI2" s="71"/>
-      <c r="AJ2" s="71"/>
-      <c r="AK2" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="72"/>
-      <c r="AM2" s="72"/>
-      <c r="AN2" s="72"/>
-      <c r="AO2" s="72"/>
-      <c r="AP2" s="72"/>
-      <c r="AQ2" s="72"/>
-      <c r="AR2" s="72"/>
-      <c r="AS2" s="72"/>
-      <c r="AT2" s="72"/>
-      <c r="AU2" s="72"/>
-      <c r="AV2" s="72"/>
-      <c r="AW2" s="72"/>
-      <c r="AX2" s="72"/>
-      <c r="AY2" s="72"/>
-      <c r="AZ2" s="72"/>
-      <c r="BA2" s="72"/>
-      <c r="BB2" s="72"/>
-      <c r="BC2" s="72"/>
-      <c r="BD2" s="72"/>
-      <c r="BE2" s="72"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84"/>
+      <c r="X2" s="84"/>
+      <c r="Y2" s="84"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="84"/>
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
+      <c r="AD2" s="84"/>
+      <c r="AE2" s="84"/>
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="84"/>
+      <c r="AH2" s="84"/>
+      <c r="AI2" s="84"/>
+      <c r="AJ2" s="84"/>
+      <c r="AK2" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="85"/>
+      <c r="AM2" s="85"/>
+      <c r="AN2" s="85"/>
+      <c r="AO2" s="85"/>
+      <c r="AP2" s="85"/>
+      <c r="AQ2" s="85"/>
+      <c r="AR2" s="85"/>
+      <c r="AS2" s="85"/>
+      <c r="AT2" s="85"/>
+      <c r="AU2" s="85"/>
+      <c r="AV2" s="85"/>
+      <c r="AW2" s="85"/>
+      <c r="AX2" s="85"/>
+      <c r="AY2" s="85"/>
+      <c r="AZ2" s="85"/>
+      <c r="BA2" s="85"/>
+      <c r="BB2" s="85"/>
+      <c r="BC2" s="85"/>
+      <c r="BD2" s="85"/>
+      <c r="BE2" s="85"/>
     </row>
     <row r="3" spans="1:57" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="76" t="s">
+      <c r="C3" s="83"/>
+      <c r="D3" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="73" t="s">
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="73" t="s">
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="73" t="s">
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="75" t="s">
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="74"/>
-      <c r="U3" s="74"/>
-      <c r="V3" s="74"/>
-      <c r="W3" s="74"/>
-      <c r="X3" s="74"/>
-      <c r="Y3" s="74"/>
-      <c r="Z3" s="74"/>
-      <c r="AA3" s="73" t="s">
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="74"/>
-      <c r="AC3" s="74"/>
-      <c r="AD3" s="74"/>
-      <c r="AE3" s="74"/>
-      <c r="AF3" s="74"/>
-      <c r="AG3" s="74"/>
-      <c r="AH3" s="74"/>
+      <c r="AB3" s="87"/>
+      <c r="AC3" s="87"/>
+      <c r="AD3" s="87"/>
+      <c r="AE3" s="87"/>
+      <c r="AF3" s="87"/>
+      <c r="AG3" s="87"/>
+      <c r="AH3" s="87"/>
       <c r="AI3" s="68" t="s">
         <v>6</v>
       </c>
       <c r="AJ3" s="69"/>
-      <c r="AK3" s="73" t="s">
+      <c r="AK3" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="AL3" s="74"/>
-      <c r="AM3" s="74"/>
-      <c r="AN3" s="73" t="s">
+      <c r="AL3" s="87"/>
+      <c r="AM3" s="87"/>
+      <c r="AN3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="AO3" s="74"/>
-      <c r="AP3" s="74"/>
-      <c r="AQ3" s="74"/>
-      <c r="AR3" s="73" t="s">
+      <c r="AO3" s="87"/>
+      <c r="AP3" s="87"/>
+      <c r="AQ3" s="87"/>
+      <c r="AR3" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="AS3" s="74"/>
-      <c r="AT3" s="74"/>
-      <c r="AU3" s="75" t="s">
+      <c r="AS3" s="87"/>
+      <c r="AT3" s="87"/>
+      <c r="AU3" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="AV3" s="74"/>
-      <c r="AW3" s="74"/>
-      <c r="AX3" s="74"/>
-      <c r="AY3" s="74"/>
-      <c r="AZ3" s="74"/>
-      <c r="BA3" s="74"/>
-      <c r="BB3" s="74"/>
+      <c r="AV3" s="87"/>
+      <c r="AW3" s="87"/>
+      <c r="AX3" s="87"/>
+      <c r="AY3" s="87"/>
+      <c r="AZ3" s="87"/>
+      <c r="BA3" s="87"/>
+      <c r="BB3" s="87"/>
       <c r="BC3" s="68" t="s">
         <v>8</v>
       </c>
@@ -1770,11 +1785,11 @@
         <v>395</v>
       </c>
       <c r="AN7" s="16">
-        <f t="shared" ref="AN7:AN17" si="8">D7-J7</f>
+        <f t="shared" ref="AN7:AN14" si="8">D7-J7</f>
         <v>-449</v>
       </c>
       <c r="AO7" s="16">
-        <f t="shared" ref="AO7:AO17" si="9">E7-K7</f>
+        <f t="shared" ref="AO7:AO14" si="9">E7-K7</f>
         <v>-58</v>
       </c>
       <c r="AP7" s="17">
@@ -1989,7 +2004,7 @@
         <v>-358</v>
       </c>
       <c r="AS8" s="16">
-        <f t="shared" ref="AR8:AV8" si="20">AS9+AS10</f>
+        <f t="shared" ref="AS8:AV8" si="20">AS9+AS10</f>
         <v>7</v>
       </c>
       <c r="AT8" s="16">
@@ -2092,26 +2107,14 @@
       <c r="AF9" s="32"/>
       <c r="AG9" s="32"/>
       <c r="AH9" s="32"/>
-      <c r="AI9" s="77"/>
-      <c r="AJ9" s="77"/>
-      <c r="AK9" s="78">
-        <f t="shared" ref="AK9:AL9" si="23">AR9-AN9</f>
-        <v>-842</v>
-      </c>
-      <c r="AL9" s="78">
-        <f t="shared" si="23"/>
-        <v>-64</v>
-      </c>
-      <c r="AM9" s="79"/>
-      <c r="AN9" s="78">
-        <f t="shared" si="8"/>
-        <v>573</v>
-      </c>
-      <c r="AO9" s="78">
-        <f t="shared" si="9"/>
-        <v>77</v>
-      </c>
-      <c r="AP9" s="79"/>
+      <c r="AI9" s="70"/>
+      <c r="AJ9" s="70"/>
+      <c r="AK9" s="71"/>
+      <c r="AL9" s="71"/>
+      <c r="AM9" s="72"/>
+      <c r="AN9" s="82"/>
+      <c r="AO9" s="82"/>
+      <c r="AP9" s="72"/>
       <c r="AQ9" s="29"/>
       <c r="AR9" s="29">
         <v>-269</v>
@@ -2120,7 +2123,7 @@
         <v>13</v>
       </c>
       <c r="AT9" s="29">
-        <f t="shared" ref="AT9:AT11" si="24">AS9+AR9</f>
+        <f t="shared" ref="AT9:AT11" si="23">AS9+AR9</f>
         <v>-256</v>
       </c>
       <c r="AU9" s="32">
@@ -2176,11 +2179,11 @@
         <v>-75</v>
       </c>
       <c r="Q10" s="32">
-        <f t="shared" ref="Q10:Q11" si="25">N10*0.13559</f>
+        <f t="shared" ref="Q10:Q11" si="24">N10*0.13559</f>
         <v>-10.033659999999999</v>
       </c>
       <c r="R10" s="32">
-        <f t="shared" ref="R10:R11" si="26">O10*0.19586</f>
+        <f t="shared" ref="R10:R11" si="25">O10*0.19586</f>
         <v>-0.19586000000000001</v>
       </c>
       <c r="S10" s="32"/>
@@ -2199,26 +2202,14 @@
       <c r="AF10" s="32"/>
       <c r="AG10" s="32"/>
       <c r="AH10" s="32"/>
-      <c r="AI10" s="77"/>
-      <c r="AJ10" s="77"/>
-      <c r="AK10" s="78">
-        <f t="shared" ref="AK10:AL10" si="27">AR10-AN10</f>
-        <v>-220</v>
-      </c>
-      <c r="AL10" s="78">
-        <f t="shared" si="27"/>
-        <v>-24</v>
-      </c>
-      <c r="AM10" s="79"/>
-      <c r="AN10" s="78">
-        <f t="shared" si="8"/>
-        <v>131</v>
-      </c>
-      <c r="AO10" s="78">
-        <f t="shared" si="9"/>
-        <v>18</v>
-      </c>
-      <c r="AP10" s="79"/>
+      <c r="AI10" s="70"/>
+      <c r="AJ10" s="70"/>
+      <c r="AK10" s="71"/>
+      <c r="AL10" s="71"/>
+      <c r="AM10" s="72"/>
+      <c r="AN10" s="82"/>
+      <c r="AO10" s="82"/>
+      <c r="AP10" s="72"/>
       <c r="AQ10" s="29"/>
       <c r="AR10" s="29">
         <v>-89</v>
@@ -2227,15 +2218,15 @@
         <v>-6</v>
       </c>
       <c r="AT10" s="29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>-95</v>
       </c>
       <c r="AU10" s="32">
-        <f t="shared" ref="AU10:AU11" si="28">AR10*0.13559</f>
+        <f t="shared" ref="AU10:AU11" si="26">AR10*0.13559</f>
         <v>-12.067509999999999</v>
       </c>
       <c r="AV10" s="32">
-        <f t="shared" ref="AV10:AV11" si="29">AS10*0.19586</f>
+        <f t="shared" ref="AV10:AV11" si="27">AS10*0.19586</f>
         <v>-1.17516</v>
       </c>
       <c r="AW10" s="32"/>
@@ -2268,22 +2259,22 @@
         <v>-1750</v>
       </c>
       <c r="G11" s="16">
-        <f t="shared" ref="G11:H11" si="30">G12+G13</f>
+        <f t="shared" ref="G11:H11" si="28">G12+G13</f>
         <v>393</v>
       </c>
       <c r="H11" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>250</v>
       </c>
       <c r="I11" s="17">
         <v>643</v>
       </c>
       <c r="J11" s="16">
-        <f t="shared" ref="J11:K11" si="31">J12+J13</f>
+        <f t="shared" ref="J11:K11" si="29">J12+J13</f>
         <v>-1001</v>
       </c>
       <c r="K11" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>-131</v>
       </c>
       <c r="L11" s="17">
@@ -2304,11 +2295,11 @@
         <v>-489</v>
       </c>
       <c r="Q11" s="19">
+        <f t="shared" si="24"/>
+        <v>-82.438719999999989</v>
+      </c>
+      <c r="R11" s="19">
         <f t="shared" si="25"/>
-        <v>-82.438719999999989</v>
-      </c>
-      <c r="R11" s="19">
-        <f t="shared" si="26"/>
         <v>23.30734</v>
       </c>
       <c r="S11" s="19">
@@ -2373,11 +2364,11 @@
         <v>22.53</v>
       </c>
       <c r="AK11" s="16">
-        <f t="shared" ref="AK11:AL11" si="32">AR11-AN11</f>
+        <f t="shared" ref="AK11:AL11" si="30">AR11-AN11</f>
         <v>276</v>
       </c>
       <c r="AL11" s="16">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>53</v>
       </c>
       <c r="AM11" s="17">
@@ -2405,15 +2396,15 @@
         <v>-19</v>
       </c>
       <c r="AT11" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>-289</v>
       </c>
       <c r="AU11" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>-36.609299999999998</v>
       </c>
       <c r="AV11" s="19">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>-3.7213400000000001</v>
       </c>
       <c r="AW11" s="19">
@@ -2492,26 +2483,14 @@
       <c r="AG12" s="39"/>
       <c r="AH12" s="39"/>
       <c r="AI12" s="39"/>
-      <c r="AJ12" s="80"/>
-      <c r="AK12" s="81">
-        <f t="shared" ref="AK12:AL12" si="33">AR12-AN12</f>
-        <v>-775</v>
-      </c>
-      <c r="AL12" s="81">
-        <f t="shared" si="33"/>
-        <v>-109</v>
-      </c>
-      <c r="AM12" s="82"/>
-      <c r="AN12" s="81">
-        <f t="shared" si="8"/>
-        <v>775</v>
-      </c>
-      <c r="AO12" s="81">
-        <f t="shared" si="9"/>
-        <v>109</v>
-      </c>
-      <c r="AP12" s="82"/>
-      <c r="AQ12" s="82"/>
+      <c r="AJ12" s="73"/>
+      <c r="AK12" s="74"/>
+      <c r="AL12" s="74"/>
+      <c r="AM12" s="75"/>
+      <c r="AN12" s="74"/>
+      <c r="AO12" s="74"/>
+      <c r="AP12" s="75"/>
+      <c r="AQ12" s="75"/>
       <c r="AR12" s="35"/>
       <c r="AS12" s="35"/>
       <c r="AT12" s="35"/>
@@ -2573,26 +2552,14 @@
       <c r="AG13" s="39"/>
       <c r="AH13" s="39"/>
       <c r="AI13" s="39"/>
-      <c r="AJ13" s="80"/>
-      <c r="AK13" s="81">
-        <f t="shared" ref="AK13:AL13" si="34">AR13-AN13</f>
-        <v>-226</v>
-      </c>
-      <c r="AL13" s="81">
-        <f t="shared" si="34"/>
-        <v>-22</v>
-      </c>
-      <c r="AM13" s="82"/>
-      <c r="AN13" s="81">
-        <f t="shared" si="8"/>
-        <v>226</v>
-      </c>
-      <c r="AO13" s="81">
-        <f t="shared" si="9"/>
-        <v>22</v>
-      </c>
-      <c r="AP13" s="82"/>
-      <c r="AQ13" s="82"/>
+      <c r="AJ13" s="73"/>
+      <c r="AK13" s="74"/>
+      <c r="AL13" s="74"/>
+      <c r="AM13" s="75"/>
+      <c r="AN13" s="74"/>
+      <c r="AO13" s="74"/>
+      <c r="AP13" s="75"/>
+      <c r="AQ13" s="75"/>
       <c r="AR13" s="35"/>
       <c r="AS13" s="35"/>
       <c r="AT13" s="35"/>
@@ -2650,23 +2617,23 @@
         <v>0.40445402298850575</v>
       </c>
       <c r="N14" s="40">
-        <f t="shared" ref="N14:P14" si="35">N15+N16</f>
+        <f t="shared" ref="N14:P14" si="31">N15+N16</f>
         <v>-267</v>
       </c>
       <c r="O14" s="40">
-        <f t="shared" si="35"/>
+        <f t="shared" si="31"/>
         <v>86</v>
       </c>
       <c r="P14" s="41">
-        <f t="shared" si="35"/>
+        <f t="shared" si="31"/>
         <v>-181</v>
       </c>
       <c r="Q14" s="19">
-        <f t="shared" ref="Q14:R14" si="36">SUM(Q15:Q16)</f>
+        <f t="shared" ref="Q14:R14" si="32">SUM(Q15:Q16)</f>
         <v>-35.405396597999996</v>
       </c>
       <c r="R14" s="19">
-        <f t="shared" si="36"/>
+        <f t="shared" si="32"/>
         <v>16.917801365000003</v>
       </c>
       <c r="S14" s="19">
@@ -2731,11 +2698,11 @@
         <v>21.36</v>
       </c>
       <c r="AK14" s="16">
-        <f t="shared" ref="AK14:AL14" si="37">AR14-AN14</f>
+        <f t="shared" ref="AK14:AL14" si="33">AR14-AN14</f>
         <v>409</v>
       </c>
       <c r="AL14" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="33"/>
         <v>132</v>
       </c>
       <c r="AM14" s="17">
@@ -2757,23 +2724,23 @@
         <v>0.59554597701149425</v>
       </c>
       <c r="AR14" s="16">
-        <f t="shared" ref="AR14:AT14" si="38">AR15+AR16</f>
+        <f t="shared" ref="AR14:AT14" si="34">AR15+AR16</f>
         <v>-314</v>
       </c>
       <c r="AS14" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="34"/>
         <v>26</v>
       </c>
       <c r="AT14" s="16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="34"/>
         <v>-288</v>
       </c>
       <c r="AU14" s="19">
-        <f t="shared" ref="AU14:AV14" si="39">SUM(AU15:AU16)</f>
+        <f t="shared" ref="AU14:AV14" si="35">SUM(AU15:AU16)</f>
         <v>-41.637807834999997</v>
       </c>
       <c r="AV14" s="19">
-        <f t="shared" si="39"/>
+        <f t="shared" si="35"/>
         <v>5.1146840949999994</v>
       </c>
       <c r="AW14" s="19">
@@ -2857,25 +2824,13 @@
       <c r="AG15" s="46"/>
       <c r="AH15" s="46"/>
       <c r="AI15" s="46"/>
-      <c r="AJ15" s="83"/>
-      <c r="AK15" s="84">
-        <f t="shared" ref="AK15:AL15" si="40">AR15-AN15</f>
-        <v>-64.965500000000006</v>
-      </c>
-      <c r="AL15" s="84">
-        <f t="shared" si="40"/>
-        <v>20.620699999999999</v>
-      </c>
-      <c r="AM15" s="83"/>
-      <c r="AN15" s="84">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AO15" s="84">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AP15" s="85"/>
+      <c r="AJ15" s="76"/>
+      <c r="AK15" s="77"/>
+      <c r="AL15" s="77"/>
+      <c r="AM15" s="76"/>
+      <c r="AN15" s="81"/>
+      <c r="AO15" s="81"/>
+      <c r="AP15" s="78"/>
       <c r="AQ15" s="48"/>
       <c r="AR15" s="43">
         <v>-64.965500000000006</v>
@@ -2884,7 +2839,7 @@
         <v>20.620699999999999</v>
       </c>
       <c r="AT15" s="47">
-        <f t="shared" ref="AT15:AT17" si="41">AS15+AR15</f>
+        <f t="shared" ref="AT15:AT17" si="36">AS15+AR15</f>
         <v>-44.344800000000006</v>
       </c>
       <c r="AU15" s="46">
@@ -2936,7 +2891,7 @@
         <v>-28.712348573999996</v>
       </c>
       <c r="R16" s="46">
-        <f t="shared" ref="R16:R17" si="42">O16*0.20001</f>
+        <f t="shared" ref="R16:R17" si="37">O16*0.20001</f>
         <v>3.5587979309999995</v>
       </c>
       <c r="S16" s="46"/>
@@ -2956,25 +2911,13 @@
       <c r="AG16" s="46"/>
       <c r="AH16" s="46"/>
       <c r="AI16" s="46"/>
-      <c r="AJ16" s="83"/>
-      <c r="AK16" s="84">
-        <f t="shared" ref="AK16:AL16" si="43">AR16-AN16</f>
-        <v>-249.03450000000001</v>
-      </c>
-      <c r="AL16" s="84">
-        <f t="shared" si="43"/>
-        <v>5.3792999999999997</v>
-      </c>
-      <c r="AM16" s="83"/>
-      <c r="AN16" s="84">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AO16" s="84">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AP16" s="85"/>
+      <c r="AJ16" s="76"/>
+      <c r="AK16" s="77"/>
+      <c r="AL16" s="77"/>
+      <c r="AM16" s="76"/>
+      <c r="AN16" s="81"/>
+      <c r="AO16" s="81"/>
+      <c r="AP16" s="78"/>
       <c r="AQ16" s="45"/>
       <c r="AR16" s="47">
         <v>-249.03450000000001</v>
@@ -2983,7 +2926,7 @@
         <v>5.3792999999999997</v>
       </c>
       <c r="AT16" s="47">
-        <f t="shared" si="41"/>
+        <f t="shared" si="36"/>
         <v>-243.65520000000001</v>
       </c>
       <c r="AU16" s="46">
@@ -2991,7 +2934,7 @@
         <v>-33.766587854999997</v>
       </c>
       <c r="AV16" s="46">
-        <f t="shared" ref="AV16:AV17" si="44">AS16*0.20001</f>
+        <f t="shared" ref="AV16:AV17" si="38">AS16*0.20001</f>
         <v>1.075913793</v>
       </c>
       <c r="AW16" s="46"/>
@@ -3024,22 +2967,22 @@
         <v>-1516</v>
       </c>
       <c r="G17" s="16">
-        <f t="shared" ref="G17:H17" si="45">G18+G19</f>
+        <f t="shared" ref="G17:H17" si="39">G18+G19</f>
         <v>175</v>
       </c>
       <c r="H17" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="39"/>
         <v>145</v>
       </c>
       <c r="I17" s="17">
         <v>320</v>
       </c>
       <c r="J17" s="16">
-        <f t="shared" ref="J17:K17" si="46">J18+J19</f>
+        <f t="shared" ref="J17:K17" si="40">J18+J19</f>
         <v>-386</v>
       </c>
       <c r="K17" s="16">
-        <f t="shared" si="46"/>
+        <f t="shared" si="40"/>
         <v>-50</v>
       </c>
       <c r="L17" s="17">
@@ -3064,7 +3007,7 @@
         <v>-25.56476</v>
       </c>
       <c r="R17" s="19">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>19.00095</v>
       </c>
       <c r="S17" s="19">
@@ -3129,22 +3072,22 @@
         <v>21.75</v>
       </c>
       <c r="AK17" s="16">
-        <f t="shared" ref="AK17:AL17" si="47">AR17-AN17</f>
+        <f t="shared" ref="AK17:AL17" si="41">AR17-AN17</f>
         <v>519</v>
       </c>
       <c r="AL17" s="16">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>203</v>
       </c>
       <c r="AM17" s="17">
         <v>726</v>
       </c>
       <c r="AN17" s="16">
-        <f t="shared" si="8"/>
+        <f>D17-J17</f>
         <v>-953</v>
       </c>
       <c r="AO17" s="16">
-        <f t="shared" si="9"/>
+        <f>E17-K17</f>
         <v>-123</v>
       </c>
       <c r="AP17" s="17">
@@ -3161,7 +3104,7 @@
         <v>80</v>
       </c>
       <c r="AT17" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="36"/>
         <v>-354</v>
       </c>
       <c r="AU17" s="19">
@@ -3169,7 +3112,7 @@
         <v>-52.583440000000003</v>
       </c>
       <c r="AV17" s="19">
-        <f t="shared" si="44"/>
+        <f t="shared" si="38"/>
         <v>16.000799999999998</v>
       </c>
       <c r="AW17" s="19">
@@ -3363,7 +3306,7 @@
         <v>69</v>
       </c>
       <c r="P20" s="29">
-        <f t="shared" ref="P20:P22" si="48">O20+N20</f>
+        <f t="shared" ref="P20:P22" si="42">O20+N20</f>
         <v>-76</v>
       </c>
       <c r="Q20" s="32">
@@ -3391,25 +3334,13 @@
       <c r="AG20" s="32"/>
       <c r="AH20" s="32"/>
       <c r="AI20" s="32"/>
-      <c r="AJ20" s="77"/>
-      <c r="AK20" s="78">
-        <f t="shared" ref="AK20:AL20" si="49">AR20-AN20</f>
-        <v>-275</v>
-      </c>
-      <c r="AL20" s="78">
-        <f t="shared" si="49"/>
-        <v>99</v>
-      </c>
-      <c r="AM20" s="79"/>
-      <c r="AN20" s="78">
-        <f t="shared" ref="AN20:AO22" si="50">D20-J20</f>
-        <v>0</v>
-      </c>
-      <c r="AO20" s="78">
-        <f t="shared" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="AP20" s="79"/>
+      <c r="AJ20" s="70"/>
+      <c r="AK20" s="71"/>
+      <c r="AL20" s="71"/>
+      <c r="AM20" s="72"/>
+      <c r="AN20" s="82"/>
+      <c r="AO20" s="82"/>
+      <c r="AP20" s="72"/>
       <c r="AQ20" s="31"/>
       <c r="AR20" s="29">
         <v>-275</v>
@@ -3418,7 +3349,7 @@
         <v>99</v>
       </c>
       <c r="AT20" s="29">
-        <f t="shared" ref="AT20:AT22" si="51">AS20+AR20</f>
+        <f t="shared" ref="AT20:AT22" si="43">AS20+AR20</f>
         <v>-176</v>
       </c>
       <c r="AU20" s="32">
@@ -3429,15 +3360,15 @@
         <f>AS20*0.20001</f>
         <v>19.800989999999999</v>
       </c>
-      <c r="AW20" s="77"/>
-      <c r="AX20" s="77"/>
-      <c r="AY20" s="77"/>
-      <c r="AZ20" s="86"/>
-      <c r="BA20" s="86"/>
-      <c r="BB20" s="86"/>
-      <c r="BC20" s="86"/>
-      <c r="BD20" s="77"/>
-      <c r="BE20" s="77"/>
+      <c r="AW20" s="70"/>
+      <c r="AX20" s="70"/>
+      <c r="AY20" s="70"/>
+      <c r="AZ20" s="79"/>
+      <c r="BA20" s="79"/>
+      <c r="BB20" s="79"/>
+      <c r="BC20" s="79"/>
+      <c r="BD20" s="70"/>
+      <c r="BE20" s="70"/>
     </row>
     <row r="21" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
@@ -3462,7 +3393,7 @@
         <v>62</v>
       </c>
       <c r="P21" s="29">
-        <f t="shared" si="48"/>
+        <f t="shared" si="42"/>
         <v>64</v>
       </c>
       <c r="Q21" s="32">
@@ -3490,25 +3421,13 @@
       <c r="AG21" s="32"/>
       <c r="AH21" s="32"/>
       <c r="AI21" s="32"/>
-      <c r="AJ21" s="77"/>
-      <c r="AK21" s="78">
-        <f t="shared" ref="AK21:AL21" si="52">AR21-AN21</f>
-        <v>-46</v>
-      </c>
-      <c r="AL21" s="78">
-        <f t="shared" si="52"/>
-        <v>33</v>
-      </c>
-      <c r="AM21" s="79"/>
-      <c r="AN21" s="78">
-        <f t="shared" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="AO21" s="78">
-        <f t="shared" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="AP21" s="79"/>
+      <c r="AJ21" s="70"/>
+      <c r="AK21" s="71"/>
+      <c r="AL21" s="71"/>
+      <c r="AM21" s="72"/>
+      <c r="AN21" s="82"/>
+      <c r="AO21" s="82"/>
+      <c r="AP21" s="72"/>
       <c r="AQ21" s="31"/>
       <c r="AR21" s="29">
         <v>-46</v>
@@ -3517,7 +3436,7 @@
         <v>33</v>
       </c>
       <c r="AT21" s="29">
-        <f t="shared" si="51"/>
+        <f t="shared" si="43"/>
         <v>-13</v>
       </c>
       <c r="AU21" s="32">
@@ -3528,15 +3447,15 @@
         <f>AS21*0.14296</f>
         <v>4.7176800000000005</v>
       </c>
-      <c r="AW21" s="77"/>
-      <c r="AX21" s="77"/>
-      <c r="AY21" s="77"/>
-      <c r="AZ21" s="86"/>
-      <c r="BA21" s="86"/>
-      <c r="BB21" s="86"/>
-      <c r="BC21" s="86"/>
-      <c r="BD21" s="77"/>
-      <c r="BE21" s="77"/>
+      <c r="AW21" s="70"/>
+      <c r="AX21" s="70"/>
+      <c r="AY21" s="70"/>
+      <c r="AZ21" s="79"/>
+      <c r="BA21" s="79"/>
+      <c r="BB21" s="79"/>
+      <c r="BC21" s="79"/>
+      <c r="BD21" s="70"/>
+      <c r="BE21" s="70"/>
     </row>
     <row r="22" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
@@ -3558,22 +3477,22 @@
         <v>-1292</v>
       </c>
       <c r="G22" s="16">
-        <f t="shared" ref="G22:H22" si="53">G23+G24</f>
+        <f t="shared" ref="G22:H22" si="44">G23+G24</f>
         <v>191</v>
       </c>
       <c r="H22" s="16">
-        <f t="shared" si="53"/>
+        <f t="shared" si="44"/>
         <v>157</v>
       </c>
       <c r="I22" s="17">
         <v>348</v>
       </c>
       <c r="J22" s="16">
-        <f t="shared" ref="J22:K22" si="54">J23+J24</f>
+        <f t="shared" ref="J22:K22" si="45">J23+J24</f>
         <v>-334</v>
       </c>
       <c r="K22" s="16">
-        <f t="shared" si="54"/>
+        <f t="shared" si="45"/>
         <v>-26</v>
       </c>
       <c r="L22" s="17">
@@ -3584,23 +3503,23 @@
         <v>0.27863777089783281</v>
       </c>
       <c r="N22" s="16">
-        <f t="shared" ref="N22:O22" si="55">N21+N20</f>
+        <f t="shared" ref="N22:O22" si="46">N21+N20</f>
         <v>-143</v>
       </c>
       <c r="O22" s="16">
-        <f t="shared" si="55"/>
+        <f t="shared" si="46"/>
         <v>131</v>
       </c>
       <c r="P22" s="16">
-        <f t="shared" si="48"/>
+        <f t="shared" si="42"/>
         <v>-12</v>
       </c>
       <c r="Q22" s="19">
-        <f t="shared" ref="Q22:R22" si="56">Q20+Q21</f>
+        <f t="shared" ref="Q22:R22" si="47">Q20+Q21</f>
         <v>-17.332979999999999</v>
       </c>
       <c r="R22" s="19">
-        <f t="shared" si="56"/>
+        <f t="shared" si="47"/>
         <v>22.664209999999997</v>
       </c>
       <c r="S22" s="19">
@@ -3667,22 +3586,22 @@
         <v>-33.03</v>
       </c>
       <c r="AK22" s="16">
-        <f t="shared" ref="AK22:AL22" si="57">AR22-AN22</f>
+        <f t="shared" ref="AK22:AL22" si="48">AR22-AN22</f>
         <v>544</v>
       </c>
       <c r="AL22" s="16">
-        <f t="shared" si="57"/>
+        <f t="shared" si="48"/>
         <v>199</v>
       </c>
       <c r="AM22" s="17">
         <v>743</v>
       </c>
       <c r="AN22" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" ref="AN22:AO22" si="49">D22-J22</f>
         <v>-865</v>
       </c>
       <c r="AO22" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="49"/>
         <v>-67</v>
       </c>
       <c r="AP22" s="17">
@@ -3701,15 +3620,15 @@
         <v>132</v>
       </c>
       <c r="AT22" s="16">
-        <f t="shared" si="51"/>
+        <f t="shared" si="43"/>
         <v>-189</v>
       </c>
       <c r="AU22" s="19">
-        <f t="shared" ref="AU22:AV22" si="58">AU20+AU21</f>
+        <f t="shared" ref="AU22:AV22" si="50">AU20+AU21</f>
         <v>-38.729060000000004</v>
       </c>
       <c r="AV22" s="19">
-        <f t="shared" si="58"/>
+        <f t="shared" si="50"/>
         <v>24.51867</v>
       </c>
       <c r="AW22" s="19">
@@ -3740,7 +3659,7 @@
         <v>-55.17</v>
       </c>
       <c r="BE22" s="26">
-        <f t="shared" ref="BE20:BE22" si="59">BC22+BB22+BD22</f>
+        <f t="shared" ref="BE22" si="51">BC22+BB22+BD22</f>
         <v>-43.03</v>
       </c>
     </row>
@@ -3891,11 +3810,11 @@
         <v>45610</v>
       </c>
       <c r="D25" s="53">
-        <f t="shared" ref="D25:D27" si="60">ROUND(J25/M25,0)</f>
+        <f t="shared" ref="D25:D27" si="52">ROUND(J25/M25,0)</f>
         <v>-973</v>
       </c>
       <c r="E25" s="53">
-        <f t="shared" ref="E25:E27" si="61">ROUND(K25/M25,0)</f>
+        <f t="shared" ref="E25:E27" si="53">ROUND(K25/M25,0)</f>
         <v>-17</v>
       </c>
       <c r="F25" s="53">
@@ -3920,7 +3839,7 @@
         <v>-357</v>
       </c>
       <c r="M25" s="54">
-        <f t="shared" ref="M25:M27" si="62">L25/F25</f>
+        <f t="shared" ref="M25:M27" si="54">L25/F25</f>
         <v>0.3606060606060606</v>
       </c>
       <c r="N25" s="55">
@@ -3930,19 +3849,19 @@
         <v>191</v>
       </c>
       <c r="P25" s="55">
-        <f t="shared" ref="P25:P27" si="63">O25+N25</f>
+        <f t="shared" ref="P25:P27" si="55">O25+N25</f>
         <v>59</v>
       </c>
       <c r="Q25" s="56">
-        <f t="shared" ref="Q25:Q27" si="64">N25*0.11761</f>
+        <f t="shared" ref="Q25:Q27" si="56">N25*0.11761</f>
         <v>-15.524520000000001</v>
       </c>
       <c r="R25" s="56">
-        <f t="shared" ref="R25:R27" si="65">O25*0.14296</f>
+        <f t="shared" ref="R25:R27" si="57">O25*0.14296</f>
         <v>27.30536</v>
       </c>
       <c r="S25" s="56">
-        <f t="shared" ref="S25:S27" si="66">R25+Q25</f>
+        <f t="shared" ref="S25:S27" si="58">R25+Q25</f>
         <v>11.78084</v>
       </c>
       <c r="T25" s="56">
@@ -3950,19 +3869,19 @@
         <v>-1.32</v>
       </c>
       <c r="U25" s="20">
-        <f t="shared" ref="U25:U27" si="67">(ABS(Q25)+ABS(R25))/(ABS(N25)+ABS(O25))</f>
+        <f t="shared" ref="U25:U27" si="59">(ABS(Q25)+ABS(R25))/(ABS(N25)+ABS(O25))</f>
         <v>0.13260024767801859</v>
       </c>
       <c r="V25" s="21">
-        <f t="shared" ref="V25:V27" si="68">ABS(R25)/ABS(O25)</f>
+        <f t="shared" ref="V25:V27" si="60">ABS(R25)/ABS(O25)</f>
         <v>0.14296</v>
       </c>
       <c r="W25" s="21">
-        <f t="shared" ref="W25:W27" si="69">Q25/N25</f>
+        <f t="shared" ref="W25:W27" si="61">Q25/N25</f>
         <v>0.11761000000000001</v>
       </c>
       <c r="X25" s="22">
-        <f t="shared" ref="X25:X26" si="70">Q25+R25+T25+0.02</f>
+        <f t="shared" ref="X25:X26" si="62">Q25+R25+T25+0.02</f>
         <v>10.480839999999999</v>
       </c>
       <c r="Y25" s="23">
@@ -3981,7 +3900,7 @@
         <v>3.43</v>
       </c>
       <c r="AD25" s="22">
-        <f t="shared" ref="AD25:AD27" si="71">AC25+AB25+AA25</f>
+        <f t="shared" ref="AD25:AD27" si="63">AC25+AB25+AA25</f>
         <v>25.380000000000003</v>
       </c>
       <c r="AE25" s="56">
@@ -3994,7 +3913,7 @@
         <v>0</v>
       </c>
       <c r="AH25" s="57">
-        <f t="shared" ref="AH25:AH27" si="72">AE25+AF25+AG25</f>
+        <f t="shared" ref="AH25:AH27" si="64">AE25+AF25+AG25</f>
         <v>21.36</v>
       </c>
       <c r="AI25" s="58"/>
@@ -4031,19 +3950,19 @@
         <v>157</v>
       </c>
       <c r="AT25" s="55">
-        <f t="shared" ref="AT25:AT27" si="73">AS25+AR25</f>
+        <f t="shared" ref="AT25:AT27" si="65">AS25+AR25</f>
         <v>22</v>
       </c>
       <c r="AU25" s="56">
-        <f t="shared" ref="AU25:AU27" si="74">AR25*0.11761</f>
+        <f t="shared" ref="AU25:AU27" si="66">AR25*0.11761</f>
         <v>-15.877350000000002</v>
       </c>
       <c r="AV25" s="56">
-        <f t="shared" ref="AV25:AV27" si="75">AS25*0.14296</f>
+        <f t="shared" ref="AV25:AV27" si="67">AS25*0.14296</f>
         <v>22.44472</v>
       </c>
       <c r="AW25" s="56">
-        <f t="shared" ref="AW25:AW27" si="76">AV25+AU25</f>
+        <f t="shared" ref="AW25:AW27" si="68">AV25+AU25</f>
         <v>6.5673699999999986</v>
       </c>
       <c r="AX25" s="56">
@@ -4054,7 +3973,7 @@
         <v>0.01</v>
       </c>
       <c r="AZ25" s="22">
-        <f t="shared" ref="AZ25:AZ27" si="77">AY25+AX25+AW25</f>
+        <f t="shared" ref="AZ25:AZ27" si="69">AY25+AX25+AW25</f>
         <v>5.2273699999999987</v>
       </c>
       <c r="BA25" s="23">
@@ -4068,7 +3987,7 @@
       </c>
       <c r="BD25" s="56"/>
       <c r="BE25" s="26">
-        <f t="shared" ref="BE25:BE27" si="78">BC25+BB25+BD25</f>
+        <f t="shared" ref="BE25:BE27" si="70">BC25+BB25+BD25</f>
         <v>11.36</v>
       </c>
     </row>
@@ -4081,11 +4000,11 @@
         <v>45643</v>
       </c>
       <c r="D26" s="16">
-        <f t="shared" si="60"/>
+        <f t="shared" si="52"/>
         <v>-605</v>
       </c>
       <c r="E26" s="16">
-        <f t="shared" si="61"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="F26" s="17">
@@ -4110,7 +4029,7 @@
         <v>-206</v>
       </c>
       <c r="M26" s="18">
-        <f t="shared" si="62"/>
+        <f t="shared" si="54"/>
         <v>0.34049586776859503</v>
       </c>
       <c r="N26" s="16">
@@ -4120,38 +4039,38 @@
         <v>214</v>
       </c>
       <c r="P26" s="16">
-        <f t="shared" si="63"/>
+        <f t="shared" si="55"/>
         <v>358</v>
       </c>
       <c r="Q26" s="19">
-        <f t="shared" si="64"/>
+        <f t="shared" si="56"/>
         <v>16.935840000000002</v>
       </c>
       <c r="R26" s="19">
-        <f t="shared" si="65"/>
+        <f t="shared" si="57"/>
         <v>30.593440000000001</v>
       </c>
       <c r="S26" s="19">
-        <f t="shared" si="66"/>
+        <f t="shared" si="58"/>
         <v>47.52928</v>
       </c>
       <c r="T26" s="19">
         <v>0</v>
       </c>
       <c r="U26" s="20">
-        <f t="shared" si="67"/>
+        <f t="shared" si="59"/>
         <v>0.13276335195530725</v>
       </c>
       <c r="V26" s="21">
-        <f t="shared" si="68"/>
+        <f t="shared" si="60"/>
         <v>0.14296</v>
       </c>
       <c r="W26" s="21">
-        <f t="shared" si="69"/>
+        <f t="shared" si="61"/>
         <v>0.11761000000000002</v>
       </c>
       <c r="X26" s="22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="62"/>
         <v>47.549280000000003</v>
       </c>
       <c r="Y26" s="23">
@@ -4170,7 +4089,7 @@
         <v>8.11</v>
       </c>
       <c r="AD26" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="63"/>
         <v>92.03</v>
       </c>
       <c r="AE26" s="19">
@@ -4183,7 +4102,7 @@
         <v>0</v>
       </c>
       <c r="AH26" s="25">
-        <f t="shared" si="72"/>
+        <f t="shared" si="64"/>
         <v>22.14</v>
       </c>
       <c r="AI26" s="59"/>
@@ -4192,11 +4111,11 @@
         <v>22.14</v>
       </c>
       <c r="AK26" s="16">
-        <f t="shared" ref="AK26:AL26" si="79">AR26-AN26</f>
+        <f t="shared" ref="AK26:AL26" si="71">AR26-AN26</f>
         <v>599</v>
       </c>
       <c r="AL26" s="16">
-        <f t="shared" si="79"/>
+        <f t="shared" si="71"/>
         <v>242</v>
       </c>
       <c r="AM26" s="17">
@@ -4224,19 +4143,19 @@
         <v>242</v>
       </c>
       <c r="AT26" s="16">
-        <f t="shared" si="73"/>
+        <f t="shared" si="65"/>
         <v>442</v>
       </c>
       <c r="AU26" s="19">
-        <f t="shared" si="74"/>
+        <f t="shared" si="66"/>
         <v>23.522000000000002</v>
       </c>
       <c r="AV26" s="19">
-        <f t="shared" si="75"/>
+        <f t="shared" si="67"/>
         <v>34.596319999999999</v>
       </c>
       <c r="AW26" s="19">
-        <f t="shared" si="76"/>
+        <f t="shared" si="68"/>
         <v>58.118319999999997</v>
       </c>
       <c r="AX26" s="19">
@@ -4246,7 +4165,7 @@
         <v>0.13</v>
       </c>
       <c r="AZ26" s="22">
-        <f t="shared" si="77"/>
+        <f t="shared" si="69"/>
         <v>58.24832</v>
       </c>
       <c r="BA26" s="23">
@@ -4260,7 +4179,7 @@
       </c>
       <c r="BD26" s="19"/>
       <c r="BE26" s="26">
-        <f t="shared" si="78"/>
+        <f t="shared" si="70"/>
         <v>12.14</v>
       </c>
     </row>
@@ -4273,40 +4192,40 @@
         <v>45673</v>
       </c>
       <c r="D27" s="16">
-        <f t="shared" si="60"/>
+        <f t="shared" si="52"/>
         <v>-309</v>
       </c>
       <c r="E27" s="16">
-        <f t="shared" si="61"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="F27" s="17">
         <v>-309</v>
       </c>
       <c r="G27" s="16">
-        <f t="shared" ref="G27:H27" si="80">G28+G29</f>
+        <f t="shared" ref="G27:H27" si="72">G28+G29</f>
         <v>489</v>
       </c>
       <c r="H27" s="16">
-        <f t="shared" si="80"/>
+        <f t="shared" si="72"/>
         <v>332</v>
       </c>
       <c r="I27" s="17">
         <v>821</v>
       </c>
       <c r="J27" s="16">
-        <f t="shared" ref="J27:K27" si="81">J28+J29</f>
+        <f t="shared" ref="J27:K27" si="73">J28+J29</f>
         <v>-210</v>
       </c>
       <c r="K27" s="16">
-        <f t="shared" si="81"/>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="L27" s="17">
         <v>-210</v>
       </c>
       <c r="M27" s="18">
-        <f t="shared" si="62"/>
+        <f t="shared" si="54"/>
         <v>0.67961165048543692</v>
       </c>
       <c r="N27" s="16">
@@ -4316,34 +4235,34 @@
         <v>332</v>
       </c>
       <c r="P27" s="16">
-        <f t="shared" si="63"/>
+        <f t="shared" si="55"/>
         <v>611</v>
       </c>
       <c r="Q27" s="19">
-        <f t="shared" si="64"/>
+        <f t="shared" si="56"/>
         <v>32.813189999999999</v>
       </c>
       <c r="R27" s="19">
-        <f t="shared" si="65"/>
+        <f t="shared" si="57"/>
         <v>47.462720000000004</v>
       </c>
       <c r="S27" s="19">
-        <f t="shared" si="66"/>
+        <f t="shared" si="58"/>
         <v>80.27591000000001</v>
       </c>
       <c r="T27" s="19">
         <v>0</v>
       </c>
       <c r="U27" s="20">
-        <f t="shared" si="67"/>
+        <f t="shared" si="59"/>
         <v>0.1313844680851064</v>
       </c>
       <c r="V27" s="21">
-        <f t="shared" si="68"/>
+        <f t="shared" si="60"/>
         <v>0.14296</v>
       </c>
       <c r="W27" s="21">
-        <f t="shared" si="69"/>
+        <f t="shared" si="61"/>
         <v>0.11760999999999999</v>
       </c>
       <c r="X27" s="22">
@@ -4366,7 +4285,7 @@
         <v>12.56</v>
       </c>
       <c r="AD27" s="22">
-        <f t="shared" si="71"/>
+        <f t="shared" si="63"/>
         <v>172.51999999999998</v>
       </c>
       <c r="AE27" s="19">
@@ -4379,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="AH27" s="25">
-        <f t="shared" si="72"/>
+        <f t="shared" si="64"/>
         <v>22.53</v>
       </c>
       <c r="AI27" s="59"/>
@@ -4388,11 +4307,11 @@
         <v>22.53</v>
       </c>
       <c r="AK27" s="16">
-        <f t="shared" ref="AK27:AL27" si="82">AR27-AN27</f>
+        <f t="shared" ref="AK27:AL27" si="74">AR27-AN27</f>
         <v>693</v>
       </c>
       <c r="AL27" s="16">
-        <f t="shared" si="82"/>
+        <f t="shared" si="74"/>
         <v>231</v>
       </c>
       <c r="AM27" s="17">
@@ -4420,19 +4339,19 @@
         <v>231</v>
       </c>
       <c r="AT27" s="16">
-        <f t="shared" si="73"/>
+        <f t="shared" si="65"/>
         <v>825</v>
       </c>
       <c r="AU27" s="19">
-        <f t="shared" si="74"/>
+        <f t="shared" si="66"/>
         <v>69.860340000000008</v>
       </c>
       <c r="AV27" s="19">
-        <f t="shared" si="75"/>
+        <f t="shared" si="67"/>
         <v>33.023760000000003</v>
       </c>
       <c r="AW27" s="19">
-        <f t="shared" si="76"/>
+        <f t="shared" si="68"/>
         <v>102.88410000000002</v>
       </c>
       <c r="AX27" s="19">
@@ -4442,7 +4361,7 @@
         <v>0.25</v>
       </c>
       <c r="AZ27" s="22">
-        <f t="shared" si="77"/>
+        <f t="shared" si="69"/>
         <v>103.13410000000002</v>
       </c>
       <c r="BA27" s="24">
@@ -4456,7 +4375,7 @@
       </c>
       <c r="BD27" s="19"/>
       <c r="BE27" s="26">
-        <f t="shared" si="78"/>
+        <f t="shared" si="70"/>
         <v>12.53</v>
       </c>
     </row>
@@ -4660,15 +4579,15 @@
         <v>-10</v>
       </c>
       <c r="U30" s="20">
-        <f t="shared" ref="U30:U31" si="83">(ABS(Q30)+ABS(R30))/(ABS(N30)+ABS(O30))</f>
+        <f t="shared" ref="U30:U31" si="75">(ABS(Q30)+ABS(R30))/(ABS(N30)+ABS(O30))</f>
         <v>0.12236459709379127</v>
       </c>
       <c r="V30" s="21">
-        <f t="shared" ref="V30:V31" si="84">ABS(R30)/ABS(O30)</f>
+        <f t="shared" ref="V30:V31" si="76">ABS(R30)/ABS(O30)</f>
         <v>0.14295774647887324</v>
       </c>
       <c r="W30" s="21">
-        <f t="shared" ref="W30:W31" si="85">Q30/N30</f>
+        <f t="shared" ref="W30:W31" si="77">Q30/N30</f>
         <v>0.11760975609756097</v>
       </c>
       <c r="X30" s="22">
@@ -4705,7 +4624,7 @@
         <v>0</v>
       </c>
       <c r="AH30" s="25">
-        <f t="shared" ref="AH30:AH31" si="86">AE30+AF30+AG30</f>
+        <f t="shared" ref="AH30:AH31" si="78">AE30+AF30+AG30</f>
         <v>21.36</v>
       </c>
       <c r="AI30" s="59"/>
@@ -4714,11 +4633,11 @@
         <v>89.57</v>
       </c>
       <c r="AK30" s="16">
-        <f t="shared" ref="AK30:AL30" si="87">AR30-AN30</f>
+        <f t="shared" ref="AK30:AL30" si="79">AR30-AN30</f>
         <v>732</v>
       </c>
       <c r="AL30" s="16">
-        <f t="shared" si="87"/>
+        <f t="shared" si="79"/>
         <v>9</v>
       </c>
       <c r="AM30" s="17">
@@ -4745,7 +4664,7 @@
         <v>199</v>
       </c>
       <c r="AT30" s="16">
-        <f t="shared" ref="AT30:AT32" si="88">AS30+AR30</f>
+        <f t="shared" ref="AT30:AT32" si="80">AS30+AR30</f>
         <v>931</v>
       </c>
       <c r="AU30" s="19">
@@ -4757,7 +4676,7 @@
         <v>28.44904</v>
       </c>
       <c r="AW30" s="19">
-        <f t="shared" ref="AW30:AW31" si="89">AV30+AU30</f>
+        <f t="shared" ref="AW30:AW31" si="81">AV30+AU30</f>
         <v>114.53955999999999</v>
       </c>
       <c r="AX30" s="19">
@@ -4767,7 +4686,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="AZ30" s="22">
-        <f t="shared" ref="AZ30:AZ31" si="90">AY30+AX30+AW30</f>
+        <f t="shared" ref="AZ30:AZ31" si="82">AY30+AX30+AW30</f>
         <v>114.81956</v>
       </c>
       <c r="BA30" s="23">
@@ -4781,7 +4700,7 @@
       </c>
       <c r="BD30" s="19"/>
       <c r="BE30" s="26">
-        <f t="shared" ref="BE30:BE31" si="91">BC30+BB30+BD30</f>
+        <f t="shared" ref="BE30:BE31" si="83">BC30+BB30+BD30</f>
         <v>88.07</v>
       </c>
     </row>
@@ -4805,22 +4724,22 @@
         <v>-762</v>
       </c>
       <c r="G31" s="16">
-        <f t="shared" ref="G31:H31" si="92">G32+G33</f>
+        <f t="shared" ref="G31:H31" si="84">G32+G33</f>
         <v>321</v>
       </c>
       <c r="H31" s="16">
-        <f t="shared" si="92"/>
+        <f t="shared" si="84"/>
         <v>286</v>
       </c>
       <c r="I31" s="17">
         <v>607</v>
       </c>
       <c r="J31" s="16">
-        <f t="shared" ref="J31:K31" si="93">J32+J33</f>
+        <f t="shared" ref="J31:K31" si="85">J32+J33</f>
         <v>-304</v>
       </c>
       <c r="K31" s="16">
-        <f t="shared" si="93"/>
+        <f t="shared" si="85"/>
         <v>-1</v>
       </c>
       <c r="L31" s="17">
@@ -4840,30 +4759,30 @@
         <v>302</v>
       </c>
       <c r="Q31" s="25">
-        <f t="shared" ref="Q31:S31" si="94">Q32+Q33</f>
+        <f t="shared" ref="Q31:S31" si="86">Q32+Q33</f>
         <v>1.9100000000000001</v>
       </c>
       <c r="R31" s="25">
-        <f t="shared" si="94"/>
+        <f t="shared" si="86"/>
         <v>38.949999999999996</v>
       </c>
       <c r="S31" s="25">
-        <f t="shared" si="94"/>
+        <f t="shared" si="86"/>
         <v>40.859999999999992</v>
       </c>
       <c r="T31" s="25">
         <v>0</v>
       </c>
       <c r="U31" s="20">
-        <f t="shared" si="83"/>
+        <f t="shared" si="75"/>
         <v>0.1352980132450331</v>
       </c>
       <c r="V31" s="21">
-        <f t="shared" si="84"/>
+        <f t="shared" si="76"/>
         <v>0.13666666666666666</v>
       </c>
       <c r="W31" s="21">
-        <f t="shared" si="85"/>
+        <f t="shared" si="77"/>
         <v>0.1123529411764706</v>
       </c>
       <c r="X31" s="22">
@@ -4898,7 +4817,7 @@
         <v>0</v>
       </c>
       <c r="AH31" s="25">
-        <f t="shared" si="86"/>
+        <f t="shared" si="78"/>
         <v>21.82</v>
       </c>
       <c r="AI31" s="16"/>
@@ -4907,11 +4826,11 @@
         <v>62.77</v>
       </c>
       <c r="AK31" s="16">
-        <f t="shared" ref="AK31:AL31" si="95">AR31-AN31</f>
+        <f t="shared" ref="AK31:AL31" si="87">AR31-AN31</f>
         <v>592</v>
       </c>
       <c r="AL31" s="16">
-        <f t="shared" si="95"/>
+        <f t="shared" si="87"/>
         <v>242</v>
       </c>
       <c r="AM31" s="17">
@@ -4933,27 +4852,27 @@
         <v>0.59973753280839892</v>
       </c>
       <c r="AR31" s="16">
-        <f t="shared" ref="AR31:AS31" si="96">AR32+AR33</f>
+        <f t="shared" ref="AR31:AS31" si="88">AR32+AR33</f>
         <v>136</v>
       </c>
       <c r="AS31" s="16">
-        <f t="shared" si="96"/>
+        <f t="shared" si="88"/>
         <v>241</v>
       </c>
       <c r="AT31" s="16">
-        <f t="shared" si="88"/>
+        <f t="shared" si="80"/>
         <v>377</v>
       </c>
       <c r="AU31" s="19">
-        <f t="shared" ref="AU31:AV31" si="97">AU32+AU33</f>
+        <f t="shared" ref="AU31:AV31" si="89">AU32+AU33</f>
         <v>15.293426873</v>
       </c>
       <c r="AV31" s="19">
-        <f t="shared" si="97"/>
+        <f t="shared" si="89"/>
         <v>32.941085250999997</v>
       </c>
       <c r="AW31" s="19">
-        <f t="shared" si="89"/>
+        <f t="shared" si="81"/>
         <v>48.234512123999998</v>
       </c>
       <c r="AX31" s="19">
@@ -4963,7 +4882,7 @@
         <v>0.11</v>
       </c>
       <c r="AZ31" s="22">
-        <f t="shared" si="90"/>
+        <f t="shared" si="82"/>
         <v>48.344512123999998</v>
       </c>
       <c r="BA31" s="23">
@@ -4978,7 +4897,7 @@
       </c>
       <c r="BD31" s="19"/>
       <c r="BE31" s="26">
-        <f t="shared" si="91"/>
+        <f t="shared" si="83"/>
         <v>60.164512123999998</v>
       </c>
     </row>
@@ -5006,17 +4925,17 @@
       </c>
       <c r="L32" s="47"/>
       <c r="M32" s="45"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
+      <c r="N32" s="80"/>
+      <c r="O32" s="80"/>
       <c r="P32" s="47"/>
-      <c r="Q32" s="43">
+      <c r="Q32" s="64">
         <v>1.58</v>
       </c>
-      <c r="R32" s="43">
+      <c r="R32" s="64">
         <v>32.159999999999997</v>
       </c>
-      <c r="S32" s="47">
-        <f t="shared" ref="S32:S33" si="98">Q32+R32</f>
+      <c r="S32" s="46">
+        <f t="shared" ref="S32:S33" si="90">Q32+R32</f>
         <v>33.739999999999995</v>
       </c>
       <c r="T32" s="47"/>
@@ -5036,11 +4955,11 @@
       <c r="AH32" s="46"/>
       <c r="AI32" s="46"/>
       <c r="AJ32" s="46"/>
-      <c r="AK32" s="46"/>
-      <c r="AL32" s="47"/>
+      <c r="AK32" s="77"/>
+      <c r="AL32" s="77"/>
       <c r="AM32" s="47"/>
-      <c r="AN32" s="47"/>
-      <c r="AO32" s="47"/>
+      <c r="AN32" s="81"/>
+      <c r="AO32" s="81"/>
       <c r="AP32" s="47"/>
       <c r="AQ32" s="48"/>
       <c r="AR32" s="43">
@@ -5050,7 +4969,7 @@
         <v>200.83330000000001</v>
       </c>
       <c r="AT32" s="47">
-        <f t="shared" si="88"/>
+        <f t="shared" si="80"/>
         <v>314.16660000000002</v>
       </c>
       <c r="AU32" s="46">
@@ -5095,17 +5014,17 @@
       </c>
       <c r="L33" s="47"/>
       <c r="M33" s="45"/>
-      <c r="N33" s="47"/>
-      <c r="O33" s="47"/>
+      <c r="N33" s="80"/>
+      <c r="O33" s="80"/>
       <c r="P33" s="47"/>
-      <c r="Q33" s="43">
+      <c r="Q33" s="64">
         <v>0.33</v>
       </c>
-      <c r="R33" s="43">
+      <c r="R33" s="64">
         <v>6.79</v>
       </c>
-      <c r="S33" s="47">
-        <f t="shared" si="98"/>
+      <c r="S33" s="46">
+        <f t="shared" si="90"/>
         <v>7.12</v>
       </c>
       <c r="T33" s="47"/>
@@ -5125,11 +5044,11 @@
       <c r="AH33" s="46"/>
       <c r="AI33" s="46"/>
       <c r="AJ33" s="46"/>
-      <c r="AK33" s="46"/>
-      <c r="AL33" s="47"/>
+      <c r="AK33" s="77"/>
+      <c r="AL33" s="77"/>
       <c r="AM33" s="47"/>
-      <c r="AN33" s="47"/>
-      <c r="AO33" s="47"/>
+      <c r="AN33" s="81"/>
+      <c r="AO33" s="81"/>
       <c r="AP33" s="47"/>
       <c r="AQ33" s="48"/>
       <c r="AR33" s="43">
@@ -5280,22 +5199,22 @@
         <v>207.22</v>
       </c>
       <c r="AK34" s="16">
-        <f t="shared" ref="AK34:AL34" si="99">AR34-AN34</f>
+        <f t="shared" ref="AK34:AL34" si="91">AR34-AN34</f>
         <v>582</v>
       </c>
       <c r="AL34" s="16">
-        <f t="shared" si="99"/>
+        <f t="shared" si="91"/>
         <v>212</v>
       </c>
       <c r="AM34" s="17">
         <v>794</v>
       </c>
       <c r="AN34" s="16">
-        <f t="shared" ref="AN34:AO34" si="100">D34-J34</f>
+        <f t="shared" ref="AN34:AO34" si="92">D34-J34</f>
         <v>-670</v>
       </c>
       <c r="AO34" s="16">
-        <f t="shared" si="100"/>
+        <f t="shared" si="92"/>
         <v>-60</v>
       </c>
       <c r="AP34" s="17">

</xml_diff>

<commit_message>
add end of day notes so I'm ready for next time
</commit_message>
<xml_diff>
--- a/python-notebooks/billing.xlsx
+++ b/python-notebooks/billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\klowe\go\src\stash.teslamotors.com\kevin-personal\energy-project\python-notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8206FA0C-29F0-4133-AE10-3C08CFB3219D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1271ED25-0B8B-4CB2-ABE6-1CE535E91315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4935" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Billing" sheetId="1" r:id="rId1"/>
@@ -612,14 +612,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="2" tint="-4.9989318521683403E-2"/>
         <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFD9F2D0"/>
+        <bgColor rgb="FFD8D8D8"/>
       </patternFill>
     </fill>
   </fills>
@@ -649,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -742,11 +742,7 @@
     <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="6" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="6" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="6" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="6" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -766,6 +762,8 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,8 +982,8 @@
   <dimension ref="A1:BE1012"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AQ19" sqref="AQ19"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1038,150 +1036,150 @@
       <c r="A2" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="84" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="84"/>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84"/>
-      <c r="AF2" s="84"/>
-      <c r="AG2" s="84"/>
-      <c r="AH2" s="84"/>
-      <c r="AI2" s="84"/>
-      <c r="AJ2" s="84"/>
-      <c r="AK2" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="85"/>
-      <c r="AM2" s="85"/>
-      <c r="AN2" s="85"/>
-      <c r="AO2" s="85"/>
-      <c r="AP2" s="85"/>
-      <c r="AQ2" s="85"/>
-      <c r="AR2" s="85"/>
-      <c r="AS2" s="85"/>
-      <c r="AT2" s="85"/>
-      <c r="AU2" s="85"/>
-      <c r="AV2" s="85"/>
-      <c r="AW2" s="85"/>
-      <c r="AX2" s="85"/>
-      <c r="AY2" s="85"/>
-      <c r="AZ2" s="85"/>
-      <c r="BA2" s="85"/>
-      <c r="BB2" s="85"/>
-      <c r="BC2" s="85"/>
-      <c r="BD2" s="85"/>
-      <c r="BE2" s="85"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="80"/>
+      <c r="W2" s="80"/>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="80"/>
+      <c r="Z2" s="80"/>
+      <c r="AA2" s="80"/>
+      <c r="AB2" s="80"/>
+      <c r="AC2" s="80"/>
+      <c r="AD2" s="80"/>
+      <c r="AE2" s="80"/>
+      <c r="AF2" s="80"/>
+      <c r="AG2" s="80"/>
+      <c r="AH2" s="80"/>
+      <c r="AI2" s="80"/>
+      <c r="AJ2" s="80"/>
+      <c r="AK2" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="81"/>
+      <c r="AM2" s="81"/>
+      <c r="AN2" s="81"/>
+      <c r="AO2" s="81"/>
+      <c r="AP2" s="81"/>
+      <c r="AQ2" s="81"/>
+      <c r="AR2" s="81"/>
+      <c r="AS2" s="81"/>
+      <c r="AT2" s="81"/>
+      <c r="AU2" s="81"/>
+      <c r="AV2" s="81"/>
+      <c r="AW2" s="81"/>
+      <c r="AX2" s="81"/>
+      <c r="AY2" s="81"/>
+      <c r="AZ2" s="81"/>
+      <c r="BA2" s="81"/>
+      <c r="BB2" s="81"/>
+      <c r="BC2" s="81"/>
+      <c r="BD2" s="81"/>
+      <c r="BE2" s="81"/>
     </row>
     <row r="3" spans="1:57" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="89" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="86" t="s">
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="86" t="s">
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="86" t="s">
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="88" t="s">
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
+      <c r="Q3" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="87"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="87"/>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
-      <c r="Z3" s="87"/>
-      <c r="AA3" s="86" t="s">
+      <c r="R3" s="83"/>
+      <c r="S3" s="83"/>
+      <c r="T3" s="83"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="87"/>
-      <c r="AC3" s="87"/>
-      <c r="AD3" s="87"/>
-      <c r="AE3" s="87"/>
-      <c r="AF3" s="87"/>
-      <c r="AG3" s="87"/>
-      <c r="AH3" s="87"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="83"/>
+      <c r="AD3" s="83"/>
+      <c r="AE3" s="83"/>
+      <c r="AF3" s="83"/>
+      <c r="AG3" s="83"/>
+      <c r="AH3" s="83"/>
       <c r="AI3" s="68" t="s">
         <v>6</v>
       </c>
       <c r="AJ3" s="69"/>
-      <c r="AK3" s="86" t="s">
+      <c r="AK3" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="AL3" s="87"/>
-      <c r="AM3" s="87"/>
-      <c r="AN3" s="86" t="s">
+      <c r="AL3" s="83"/>
+      <c r="AM3" s="83"/>
+      <c r="AN3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="AO3" s="87"/>
-      <c r="AP3" s="87"/>
-      <c r="AQ3" s="87"/>
-      <c r="AR3" s="86" t="s">
+      <c r="AO3" s="83"/>
+      <c r="AP3" s="83"/>
+      <c r="AQ3" s="83"/>
+      <c r="AR3" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="AS3" s="87"/>
-      <c r="AT3" s="87"/>
-      <c r="AU3" s="88" t="s">
+      <c r="AS3" s="83"/>
+      <c r="AT3" s="83"/>
+      <c r="AU3" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="AV3" s="87"/>
-      <c r="AW3" s="87"/>
-      <c r="AX3" s="87"/>
-      <c r="AY3" s="87"/>
-      <c r="AZ3" s="87"/>
-      <c r="BA3" s="87"/>
-      <c r="BB3" s="87"/>
+      <c r="AV3" s="83"/>
+      <c r="AW3" s="83"/>
+      <c r="AX3" s="83"/>
+      <c r="AY3" s="83"/>
+      <c r="AZ3" s="83"/>
+      <c r="BA3" s="83"/>
+      <c r="BB3" s="83"/>
       <c r="BC3" s="68" t="s">
         <v>8</v>
       </c>
@@ -2057,7 +2055,7 @@
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="F9" s="87"/>
       <c r="G9" s="30">
         <v>273</v>
       </c>
@@ -2112,9 +2110,9 @@
       <c r="AK9" s="71"/>
       <c r="AL9" s="71"/>
       <c r="AM9" s="72"/>
-      <c r="AN9" s="82"/>
-      <c r="AO9" s="82"/>
-      <c r="AP9" s="72"/>
+      <c r="AN9" s="72"/>
+      <c r="AO9" s="72"/>
+      <c r="AP9" s="87"/>
       <c r="AQ9" s="29"/>
       <c r="AR9" s="29">
         <v>-269</v>
@@ -2152,7 +2150,7 @@
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
+      <c r="F10" s="87"/>
       <c r="G10" s="30">
         <v>57</v>
       </c>
@@ -2207,9 +2205,9 @@
       <c r="AK10" s="71"/>
       <c r="AL10" s="71"/>
       <c r="AM10" s="72"/>
-      <c r="AN10" s="82"/>
-      <c r="AO10" s="82"/>
-      <c r="AP10" s="72"/>
+      <c r="AN10" s="72"/>
+      <c r="AO10" s="72"/>
+      <c r="AP10" s="87"/>
       <c r="AQ10" s="29"/>
       <c r="AR10" s="29">
         <v>-89</v>
@@ -2828,9 +2826,9 @@
       <c r="AK15" s="77"/>
       <c r="AL15" s="77"/>
       <c r="AM15" s="76"/>
-      <c r="AN15" s="81"/>
-      <c r="AO15" s="81"/>
-      <c r="AP15" s="78"/>
+      <c r="AN15" s="77"/>
+      <c r="AO15" s="76"/>
+      <c r="AP15" s="87"/>
       <c r="AQ15" s="48"/>
       <c r="AR15" s="43">
         <v>-64.965500000000006</v>
@@ -2915,9 +2913,9 @@
       <c r="AK16" s="77"/>
       <c r="AL16" s="77"/>
       <c r="AM16" s="76"/>
-      <c r="AN16" s="81"/>
-      <c r="AO16" s="81"/>
-      <c r="AP16" s="78"/>
+      <c r="AN16" s="77"/>
+      <c r="AO16" s="76"/>
+      <c r="AP16" s="87"/>
       <c r="AQ16" s="45"/>
       <c r="AR16" s="47">
         <v>-249.03450000000001</v>
@@ -3338,9 +3336,9 @@
       <c r="AK20" s="71"/>
       <c r="AL20" s="71"/>
       <c r="AM20" s="72"/>
-      <c r="AN20" s="82"/>
-      <c r="AO20" s="82"/>
-      <c r="AP20" s="72"/>
+      <c r="AN20" s="71"/>
+      <c r="AO20" s="72"/>
+      <c r="AP20" s="87"/>
       <c r="AQ20" s="31"/>
       <c r="AR20" s="29">
         <v>-275</v>
@@ -3363,10 +3361,10 @@
       <c r="AW20" s="70"/>
       <c r="AX20" s="70"/>
       <c r="AY20" s="70"/>
-      <c r="AZ20" s="79"/>
-      <c r="BA20" s="79"/>
-      <c r="BB20" s="79"/>
-      <c r="BC20" s="79"/>
+      <c r="AZ20" s="78"/>
+      <c r="BA20" s="78"/>
+      <c r="BB20" s="78"/>
+      <c r="BC20" s="78"/>
       <c r="BD20" s="70"/>
       <c r="BE20" s="70"/>
     </row>
@@ -3425,9 +3423,9 @@
       <c r="AK21" s="71"/>
       <c r="AL21" s="71"/>
       <c r="AM21" s="72"/>
-      <c r="AN21" s="82"/>
-      <c r="AO21" s="82"/>
-      <c r="AP21" s="72"/>
+      <c r="AN21" s="71"/>
+      <c r="AO21" s="72"/>
+      <c r="AP21" s="87"/>
       <c r="AQ21" s="31"/>
       <c r="AR21" s="29">
         <v>-46</v>
@@ -3450,10 +3448,10 @@
       <c r="AW21" s="70"/>
       <c r="AX21" s="70"/>
       <c r="AY21" s="70"/>
-      <c r="AZ21" s="79"/>
-      <c r="BA21" s="79"/>
-      <c r="BB21" s="79"/>
-      <c r="BC21" s="79"/>
+      <c r="AZ21" s="78"/>
+      <c r="BA21" s="78"/>
+      <c r="BB21" s="78"/>
+      <c r="BC21" s="78"/>
       <c r="BD21" s="70"/>
       <c r="BE21" s="70"/>
     </row>
@@ -4925,8 +4923,12 @@
       </c>
       <c r="L32" s="47"/>
       <c r="M32" s="45"/>
-      <c r="N32" s="80"/>
-      <c r="O32" s="80"/>
+      <c r="N32" s="86">
+        <v>14.166700000000001</v>
+      </c>
+      <c r="O32" s="86">
+        <v>237.5</v>
+      </c>
       <c r="P32" s="47"/>
       <c r="Q32" s="64">
         <v>1.58</v>
@@ -4958,9 +4960,9 @@
       <c r="AK32" s="77"/>
       <c r="AL32" s="77"/>
       <c r="AM32" s="47"/>
-      <c r="AN32" s="81"/>
-      <c r="AO32" s="81"/>
-      <c r="AP32" s="47"/>
+      <c r="AN32" s="47"/>
+      <c r="AO32" s="47"/>
+      <c r="AP32" s="87"/>
       <c r="AQ32" s="48"/>
       <c r="AR32" s="43">
         <v>113.33329999999999</v>
@@ -5014,8 +5016,12 @@
       </c>
       <c r="L33" s="47"/>
       <c r="M33" s="45"/>
-      <c r="N33" s="80"/>
-      <c r="O33" s="80"/>
+      <c r="N33" s="86">
+        <v>2.8332999999999999</v>
+      </c>
+      <c r="O33" s="86">
+        <v>47.5</v>
+      </c>
       <c r="P33" s="47"/>
       <c r="Q33" s="64">
         <v>0.33</v>
@@ -5047,9 +5053,9 @@
       <c r="AK33" s="77"/>
       <c r="AL33" s="77"/>
       <c r="AM33" s="47"/>
-      <c r="AN33" s="81"/>
-      <c r="AO33" s="81"/>
-      <c r="AP33" s="47"/>
+      <c r="AN33" s="47"/>
+      <c r="AO33" s="47"/>
+      <c r="AP33" s="87"/>
       <c r="AQ33" s="48"/>
       <c r="AR33" s="43">
         <v>22.666699999999999</v>

</xml_diff>

<commit_message>
issues with september 2025 to investigate
</commit_message>
<xml_diff>
--- a/python-notebooks/billing.xlsx
+++ b/python-notebooks/billing.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\klowe\go\src\stash.teslamotors.com\kevin-personal\energy-project\python-notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1271ED25-0B8B-4CB2-ABE6-1CE535E91315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE04516A-F392-45F9-9888-4B280A0C0943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4935" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Billing" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -422,7 +423,7 @@
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,6 +467,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -649,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -743,6 +751,8 @@
     <xf numFmtId="44" fontId="6" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="6" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="6" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -762,8 +772,9 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,9 +992,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V38" sqref="V38"/>
+      <selection pane="topRight" activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1020,8 +1031,7 @@
     <col min="45" max="45" width="10.77734375" customWidth="1"/>
     <col min="46" max="46" width="8.6640625" customWidth="1"/>
     <col min="47" max="47" width="11" customWidth="1"/>
-    <col min="48" max="48" width="10.6640625" customWidth="1"/>
-    <col min="49" max="49" width="8.6640625" customWidth="1"/>
+    <col min="48" max="49" width="10.6640625" customWidth="1"/>
     <col min="50" max="50" width="11.21875" customWidth="1"/>
     <col min="51" max="51" width="12.77734375" customWidth="1"/>
     <col min="52" max="52" width="8.6640625" customWidth="1"/>
@@ -1036,150 +1046,150 @@
       <c r="A2" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="80" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="80"/>
-      <c r="U2" s="80"/>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80"/>
-      <c r="X2" s="80"/>
-      <c r="Y2" s="80"/>
-      <c r="Z2" s="80"/>
-      <c r="AA2" s="80"/>
-      <c r="AB2" s="80"/>
-      <c r="AC2" s="80"/>
-      <c r="AD2" s="80"/>
-      <c r="AE2" s="80"/>
-      <c r="AF2" s="80"/>
-      <c r="AG2" s="80"/>
-      <c r="AH2" s="80"/>
-      <c r="AI2" s="80"/>
-      <c r="AJ2" s="80"/>
-      <c r="AK2" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="81"/>
-      <c r="AM2" s="81"/>
-      <c r="AN2" s="81"/>
-      <c r="AO2" s="81"/>
-      <c r="AP2" s="81"/>
-      <c r="AQ2" s="81"/>
-      <c r="AR2" s="81"/>
-      <c r="AS2" s="81"/>
-      <c r="AT2" s="81"/>
-      <c r="AU2" s="81"/>
-      <c r="AV2" s="81"/>
-      <c r="AW2" s="81"/>
-      <c r="AX2" s="81"/>
-      <c r="AY2" s="81"/>
-      <c r="AZ2" s="81"/>
-      <c r="BA2" s="81"/>
-      <c r="BB2" s="81"/>
-      <c r="BC2" s="81"/>
-      <c r="BD2" s="81"/>
-      <c r="BE2" s="81"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="82"/>
+      <c r="W2" s="82"/>
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="82"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+      <c r="AD2" s="82"/>
+      <c r="AE2" s="82"/>
+      <c r="AF2" s="82"/>
+      <c r="AG2" s="82"/>
+      <c r="AH2" s="82"/>
+      <c r="AI2" s="82"/>
+      <c r="AJ2" s="82"/>
+      <c r="AK2" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="83"/>
+      <c r="AM2" s="83"/>
+      <c r="AN2" s="83"/>
+      <c r="AO2" s="83"/>
+      <c r="AP2" s="83"/>
+      <c r="AQ2" s="83"/>
+      <c r="AR2" s="83"/>
+      <c r="AS2" s="83"/>
+      <c r="AT2" s="83"/>
+      <c r="AU2" s="83"/>
+      <c r="AV2" s="83"/>
+      <c r="AW2" s="83"/>
+      <c r="AX2" s="83"/>
+      <c r="AY2" s="83"/>
+      <c r="AZ2" s="83"/>
+      <c r="BA2" s="83"/>
+      <c r="BB2" s="83"/>
+      <c r="BC2" s="83"/>
+      <c r="BD2" s="83"/>
+      <c r="BE2" s="83"/>
     </row>
     <row r="3" spans="1:57" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="85" t="s">
+      <c r="C3" s="81"/>
+      <c r="D3" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="82" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="82" t="s">
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="82" t="s">
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="84" t="s">
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="83"/>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="82" t="s">
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="85"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="83"/>
-      <c r="AC3" s="83"/>
-      <c r="AD3" s="83"/>
-      <c r="AE3" s="83"/>
-      <c r="AF3" s="83"/>
-      <c r="AG3" s="83"/>
-      <c r="AH3" s="83"/>
+      <c r="AB3" s="85"/>
+      <c r="AC3" s="85"/>
+      <c r="AD3" s="85"/>
+      <c r="AE3" s="85"/>
+      <c r="AF3" s="85"/>
+      <c r="AG3" s="85"/>
+      <c r="AH3" s="85"/>
       <c r="AI3" s="68" t="s">
         <v>6</v>
       </c>
       <c r="AJ3" s="69"/>
-      <c r="AK3" s="82" t="s">
+      <c r="AK3" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="AL3" s="83"/>
-      <c r="AM3" s="83"/>
-      <c r="AN3" s="82" t="s">
+      <c r="AL3" s="85"/>
+      <c r="AM3" s="85"/>
+      <c r="AN3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="AO3" s="83"/>
-      <c r="AP3" s="83"/>
-      <c r="AQ3" s="83"/>
-      <c r="AR3" s="82" t="s">
+      <c r="AO3" s="85"/>
+      <c r="AP3" s="85"/>
+      <c r="AQ3" s="85"/>
+      <c r="AR3" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="AS3" s="83"/>
-      <c r="AT3" s="83"/>
-      <c r="AU3" s="84" t="s">
+      <c r="AS3" s="85"/>
+      <c r="AT3" s="85"/>
+      <c r="AU3" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="AV3" s="83"/>
-      <c r="AW3" s="83"/>
-      <c r="AX3" s="83"/>
-      <c r="AY3" s="83"/>
-      <c r="AZ3" s="83"/>
-      <c r="BA3" s="83"/>
-      <c r="BB3" s="83"/>
+      <c r="AV3" s="85"/>
+      <c r="AW3" s="85"/>
+      <c r="AX3" s="85"/>
+      <c r="AY3" s="85"/>
+      <c r="AZ3" s="85"/>
+      <c r="BA3" s="85"/>
+      <c r="BB3" s="85"/>
       <c r="BC3" s="68" t="s">
         <v>8</v>
       </c>
@@ -1664,7 +1674,7 @@
         <v>-884</v>
       </c>
       <c r="E7" s="16">
-        <f t="shared" ref="E7:E8" si="0">ROUND(K7/M7,0)</f>
+        <f t="shared" ref="E7" si="0">ROUND(K7/M7,0)</f>
         <v>-114</v>
       </c>
       <c r="F7" s="17">
@@ -1772,11 +1782,11 @@
         <v>67.83</v>
       </c>
       <c r="AK7" s="16">
-        <f t="shared" ref="AK7:AL7" si="7">AR7-AN7</f>
+        <f>AR7-AN7</f>
         <v>298</v>
       </c>
       <c r="AL7" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="AK7:AL7" si="7">AS7-AO7</f>
         <v>97</v>
       </c>
       <c r="AM7" s="17">
@@ -1858,7 +1868,7 @@
         <v>-1411</v>
       </c>
       <c r="E8" s="16">
-        <f t="shared" si="0"/>
+        <f>ROUND(K8/M8,0)</f>
         <v>-190</v>
       </c>
       <c r="F8" s="17">
@@ -1876,38 +1886,38 @@
         <v>451</v>
       </c>
       <c r="J8" s="16">
-        <f t="shared" ref="J8:K8" si="15">J9+J10</f>
+        <f>J9+J10</f>
         <v>-704</v>
       </c>
       <c r="K8" s="16">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="K8" si="15">K9+K10</f>
         <v>-95</v>
       </c>
       <c r="L8" s="17">
         <v>-799</v>
       </c>
       <c r="M8" s="18">
-        <f t="shared" ref="M8" si="16">L8/F8</f>
+        <f>L8/F8</f>
         <v>0.49906308557151779</v>
       </c>
       <c r="N8" s="16">
-        <f t="shared" ref="N8:R8" si="17">N9+N10</f>
+        <f t="shared" ref="N8:R8" si="16">N9+N10</f>
         <v>-374</v>
       </c>
       <c r="O8" s="16">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>26</v>
       </c>
       <c r="P8" s="16">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>-348</v>
       </c>
       <c r="Q8" s="19">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>-47.806659999999994</v>
       </c>
       <c r="R8" s="19">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>3.8457699999999995</v>
       </c>
       <c r="S8" s="19">
@@ -1963,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="AH8" s="25">
-        <f t="shared" ref="AH8" si="18">AE8+AF8+AG8</f>
+        <f t="shared" ref="AH8" si="17">AE8+AF8+AG8</f>
         <v>21.75</v>
       </c>
       <c r="AI8" s="16"/>
@@ -1972,11 +1982,11 @@
         <v>21.75</v>
       </c>
       <c r="AK8" s="16">
-        <f t="shared" ref="AK8:AL8" si="19">AR8-AN8</f>
+        <f t="shared" ref="AK8:AL8" si="18">AR8-AN8</f>
         <v>349</v>
       </c>
       <c r="AL8" s="16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>102</v>
       </c>
       <c r="AM8" s="17">
@@ -1987,7 +1997,7 @@
         <v>-707</v>
       </c>
       <c r="AO8" s="16">
-        <f t="shared" si="9"/>
+        <f>E8-K8</f>
         <v>-95</v>
       </c>
       <c r="AP8" s="17">
@@ -2002,19 +2012,19 @@
         <v>-358</v>
       </c>
       <c r="AS8" s="16">
-        <f t="shared" ref="AS8:AV8" si="20">AS9+AS10</f>
+        <f t="shared" ref="AS8:AV8" si="19">AS9+AS10</f>
         <v>7</v>
       </c>
       <c r="AT8" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>-351</v>
       </c>
       <c r="AU8" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>-45.9373</v>
       </c>
       <c r="AV8" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0.77081</v>
       </c>
       <c r="AW8" s="19">
@@ -2043,7 +2053,7 @@
       </c>
       <c r="BD8" s="19"/>
       <c r="BE8" s="26">
-        <f t="shared" ref="BE8" si="21">BC8+BB8+BD8</f>
+        <f t="shared" ref="BE8" si="20">BC8+BB8+BD8</f>
         <v>11.75</v>
       </c>
     </row>
@@ -2053,9 +2063,15 @@
       <c r="C9" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="87"/>
+      <c r="D9" s="29">
+        <f>ROUND(J9/M8,0)</f>
+        <v>-1148</v>
+      </c>
+      <c r="E9" s="29">
+        <f>ROUND(K9/M8,0)</f>
+        <v>-154</v>
+      </c>
+      <c r="F9" s="29"/>
       <c r="G9" s="30">
         <v>273</v>
       </c>
@@ -2078,7 +2094,7 @@
         <v>27</v>
       </c>
       <c r="P9" s="29">
-        <f t="shared" ref="P9:P11" si="22">O9+N9</f>
+        <f t="shared" ref="P9:P11" si="21">O9+N9</f>
         <v>-273</v>
       </c>
       <c r="Q9" s="32">
@@ -2107,12 +2123,24 @@
       <c r="AH9" s="32"/>
       <c r="AI9" s="70"/>
       <c r="AJ9" s="70"/>
-      <c r="AK9" s="71"/>
-      <c r="AL9" s="71"/>
+      <c r="AK9" s="71">
+        <f>AR9-AN9</f>
+        <v>306</v>
+      </c>
+      <c r="AL9" s="71">
+        <f>AS9-AO9</f>
+        <v>90</v>
+      </c>
       <c r="AM9" s="72"/>
-      <c r="AN9" s="72"/>
-      <c r="AO9" s="72"/>
-      <c r="AP9" s="87"/>
+      <c r="AN9" s="72">
+        <f>D9-J9</f>
+        <v>-575</v>
+      </c>
+      <c r="AO9" s="72">
+        <f>E9-K9</f>
+        <v>-77</v>
+      </c>
+      <c r="AP9" s="29"/>
       <c r="AQ9" s="29"/>
       <c r="AR9" s="29">
         <v>-269</v>
@@ -2121,7 +2149,7 @@
         <v>13</v>
       </c>
       <c r="AT9" s="29">
-        <f t="shared" ref="AT9:AT11" si="23">AS9+AR9</f>
+        <f t="shared" ref="AT9:AT11" si="22">AS9+AR9</f>
         <v>-256</v>
       </c>
       <c r="AU9" s="32">
@@ -2148,9 +2176,15 @@
       <c r="C10" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="87"/>
+      <c r="D10" s="29">
+        <f>ROUND(J10/M8,0)</f>
+        <v>-262</v>
+      </c>
+      <c r="E10" s="29">
+        <f>ROUND(K10/M8,0)</f>
+        <v>-36</v>
+      </c>
+      <c r="F10" s="29"/>
       <c r="G10" s="30">
         <v>57</v>
       </c>
@@ -2173,15 +2207,15 @@
         <v>-1</v>
       </c>
       <c r="P10" s="29">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>-75</v>
       </c>
       <c r="Q10" s="32">
-        <f t="shared" ref="Q10:Q11" si="24">N10*0.13559</f>
+        <f t="shared" ref="Q10:Q11" si="23">N10*0.13559</f>
         <v>-10.033659999999999</v>
       </c>
       <c r="R10" s="32">
-        <f t="shared" ref="R10:R11" si="25">O10*0.19586</f>
+        <f t="shared" ref="R10:R11" si="24">O10*0.19586</f>
         <v>-0.19586000000000001</v>
       </c>
       <c r="S10" s="32"/>
@@ -2202,12 +2236,24 @@
       <c r="AH10" s="32"/>
       <c r="AI10" s="70"/>
       <c r="AJ10" s="70"/>
-      <c r="AK10" s="71"/>
-      <c r="AL10" s="71"/>
+      <c r="AK10" s="71">
+        <f>AR10-AN10</f>
+        <v>42</v>
+      </c>
+      <c r="AL10" s="71">
+        <f>AS10-AO10</f>
+        <v>12</v>
+      </c>
       <c r="AM10" s="72"/>
-      <c r="AN10" s="72"/>
-      <c r="AO10" s="72"/>
-      <c r="AP10" s="87"/>
+      <c r="AN10" s="72">
+        <f>D10-J10</f>
+        <v>-131</v>
+      </c>
+      <c r="AO10" s="72">
+        <f>E10-K10</f>
+        <v>-18</v>
+      </c>
+      <c r="AP10" s="29"/>
       <c r="AQ10" s="29"/>
       <c r="AR10" s="29">
         <v>-89</v>
@@ -2216,15 +2262,15 @@
         <v>-6</v>
       </c>
       <c r="AT10" s="29">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>-95</v>
       </c>
       <c r="AU10" s="32">
-        <f t="shared" ref="AU10:AU11" si="26">AR10*0.13559</f>
+        <f t="shared" ref="AU10:AU11" si="25">AR10*0.13559</f>
         <v>-12.067509999999999</v>
       </c>
       <c r="AV10" s="32">
-        <f t="shared" ref="AV10:AV11" si="27">AS10*0.19586</f>
+        <f t="shared" ref="AV10:AV11" si="26">AS10*0.19586</f>
         <v>-1.17516</v>
       </c>
       <c r="AW10" s="32"/>
@@ -2257,22 +2303,22 @@
         <v>-1750</v>
       </c>
       <c r="G11" s="16">
-        <f t="shared" ref="G11:H11" si="28">G12+G13</f>
+        <f t="shared" ref="G11:H11" si="27">G12+G13</f>
         <v>393</v>
       </c>
       <c r="H11" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>250</v>
       </c>
       <c r="I11" s="17">
         <v>643</v>
       </c>
       <c r="J11" s="16">
-        <f t="shared" ref="J11:K11" si="29">J12+J13</f>
+        <f t="shared" ref="J11:K11" si="28">J12+J13</f>
         <v>-1001</v>
       </c>
       <c r="K11" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>-131</v>
       </c>
       <c r="L11" s="17">
@@ -2289,15 +2335,15 @@
         <v>119</v>
       </c>
       <c r="P11" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>-489</v>
       </c>
       <c r="Q11" s="19">
+        <f t="shared" si="23"/>
+        <v>-82.438719999999989</v>
+      </c>
+      <c r="R11" s="19">
         <f t="shared" si="24"/>
-        <v>-82.438719999999989</v>
-      </c>
-      <c r="R11" s="19">
-        <f t="shared" si="25"/>
         <v>23.30734</v>
       </c>
       <c r="S11" s="19">
@@ -2362,11 +2408,11 @@
         <v>22.53</v>
       </c>
       <c r="AK11" s="16">
-        <f t="shared" ref="AK11:AL11" si="30">AR11-AN11</f>
+        <f t="shared" ref="AK11:AL11" si="29">AR11-AN11</f>
         <v>276</v>
       </c>
       <c r="AL11" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>53</v>
       </c>
       <c r="AM11" s="17">
@@ -2394,15 +2440,15 @@
         <v>-19</v>
       </c>
       <c r="AT11" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>-289</v>
       </c>
       <c r="AU11" s="19">
+        <f t="shared" si="25"/>
+        <v>-36.609299999999998</v>
+      </c>
+      <c r="AV11" s="19">
         <f t="shared" si="26"/>
-        <v>-36.609299999999998</v>
-      </c>
-      <c r="AV11" s="19">
-        <f t="shared" si="27"/>
         <v>-3.7213400000000001</v>
       </c>
       <c r="AW11" s="19">
@@ -2441,8 +2487,14 @@
       <c r="C12" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="D12" s="35">
+        <f>ROUND(J12/M11,0)</f>
+        <v>-1198</v>
+      </c>
+      <c r="E12" s="35">
+        <f>ROUND(K12/M11,0)</f>
+        <v>-169</v>
+      </c>
       <c r="F12" s="35"/>
       <c r="G12" s="34">
         <v>279</v>
@@ -2510,8 +2562,14 @@
       <c r="C13" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
+      <c r="D13" s="35">
+        <f>ROUND(J13/M11,0)</f>
+        <v>-349</v>
+      </c>
+      <c r="E13" s="35">
+        <f>ROUND(K13/M11,0)</f>
+        <v>-34</v>
+      </c>
       <c r="F13" s="35"/>
       <c r="G13" s="34">
         <v>114</v>
@@ -2615,23 +2673,23 @@
         <v>0.40445402298850575</v>
       </c>
       <c r="N14" s="40">
-        <f t="shared" ref="N14:P14" si="31">N15+N16</f>
+        <f t="shared" ref="N14:P14" si="30">N15+N16</f>
         <v>-267</v>
       </c>
       <c r="O14" s="40">
+        <f t="shared" si="30"/>
+        <v>86</v>
+      </c>
+      <c r="P14" s="41">
+        <f t="shared" si="30"/>
+        <v>-181</v>
+      </c>
+      <c r="Q14" s="19">
+        <f t="shared" ref="Q14:R14" si="31">SUM(Q15:Q16)</f>
+        <v>-35.405396597999996</v>
+      </c>
+      <c r="R14" s="19">
         <f t="shared" si="31"/>
-        <v>86</v>
-      </c>
-      <c r="P14" s="41">
-        <f t="shared" si="31"/>
-        <v>-181</v>
-      </c>
-      <c r="Q14" s="19">
-        <f t="shared" ref="Q14:R14" si="32">SUM(Q15:Q16)</f>
-        <v>-35.405396597999996</v>
-      </c>
-      <c r="R14" s="19">
-        <f t="shared" si="32"/>
         <v>16.917801365000003</v>
       </c>
       <c r="S14" s="19">
@@ -2696,11 +2754,11 @@
         <v>21.36</v>
       </c>
       <c r="AK14" s="16">
-        <f t="shared" ref="AK14:AL14" si="33">AR14-AN14</f>
+        <f t="shared" ref="AK14:AL14" si="32">AR14-AN14</f>
         <v>409</v>
       </c>
       <c r="AL14" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>132</v>
       </c>
       <c r="AM14" s="17">
@@ -2722,23 +2780,23 @@
         <v>0.59554597701149425</v>
       </c>
       <c r="AR14" s="16">
-        <f t="shared" ref="AR14:AT14" si="34">AR15+AR16</f>
+        <f t="shared" ref="AR14:AT14" si="33">AR15+AR16</f>
         <v>-314</v>
       </c>
       <c r="AS14" s="16">
+        <f t="shared" si="33"/>
+        <v>26</v>
+      </c>
+      <c r="AT14" s="16">
+        <f t="shared" si="33"/>
+        <v>-288</v>
+      </c>
+      <c r="AU14" s="19">
+        <f t="shared" ref="AU14:AV14" si="34">SUM(AU15:AU16)</f>
+        <v>-41.637807834999997</v>
+      </c>
+      <c r="AV14" s="19">
         <f t="shared" si="34"/>
-        <v>26</v>
-      </c>
-      <c r="AT14" s="16">
-        <f t="shared" si="34"/>
-        <v>-288</v>
-      </c>
-      <c r="AU14" s="19">
-        <f t="shared" ref="AU14:AV14" si="35">SUM(AU15:AU16)</f>
-        <v>-41.637807834999997</v>
-      </c>
-      <c r="AV14" s="19">
-        <f t="shared" si="35"/>
         <v>5.1146840949999994</v>
       </c>
       <c r="AW14" s="19">
@@ -2828,7 +2886,7 @@
       <c r="AM15" s="76"/>
       <c r="AN15" s="77"/>
       <c r="AO15" s="76"/>
-      <c r="AP15" s="87"/>
+      <c r="AP15" s="80"/>
       <c r="AQ15" s="48"/>
       <c r="AR15" s="43">
         <v>-64.965500000000006</v>
@@ -2837,7 +2895,7 @@
         <v>20.620699999999999</v>
       </c>
       <c r="AT15" s="47">
-        <f t="shared" ref="AT15:AT17" si="36">AS15+AR15</f>
+        <f t="shared" ref="AT15:AT17" si="35">AS15+AR15</f>
         <v>-44.344800000000006</v>
       </c>
       <c r="AU15" s="46">
@@ -2889,7 +2947,7 @@
         <v>-28.712348573999996</v>
       </c>
       <c r="R16" s="46">
-        <f t="shared" ref="R16:R17" si="37">O16*0.20001</f>
+        <f t="shared" ref="R16:R17" si="36">O16*0.20001</f>
         <v>3.5587979309999995</v>
       </c>
       <c r="S16" s="46"/>
@@ -2915,7 +2973,7 @@
       <c r="AM16" s="76"/>
       <c r="AN16" s="77"/>
       <c r="AO16" s="76"/>
-      <c r="AP16" s="87"/>
+      <c r="AP16" s="80"/>
       <c r="AQ16" s="45"/>
       <c r="AR16" s="47">
         <v>-249.03450000000001</v>
@@ -2924,7 +2982,7 @@
         <v>5.3792999999999997</v>
       </c>
       <c r="AT16" s="47">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>-243.65520000000001</v>
       </c>
       <c r="AU16" s="46">
@@ -2932,7 +2990,7 @@
         <v>-33.766587854999997</v>
       </c>
       <c r="AV16" s="46">
-        <f t="shared" ref="AV16:AV17" si="38">AS16*0.20001</f>
+        <f t="shared" ref="AV16:AV17" si="37">AS16*0.20001</f>
         <v>1.075913793</v>
       </c>
       <c r="AW16" s="46"/>
@@ -2965,22 +3023,22 @@
         <v>-1516</v>
       </c>
       <c r="G17" s="16">
-        <f t="shared" ref="G17:H17" si="39">G18+G19</f>
+        <f t="shared" ref="G17:H17" si="38">G18+G19</f>
         <v>175</v>
       </c>
       <c r="H17" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>145</v>
       </c>
       <c r="I17" s="17">
         <v>320</v>
       </c>
       <c r="J17" s="16">
-        <f t="shared" ref="J17:K17" si="40">J18+J19</f>
+        <f>J18+J19</f>
         <v>-386</v>
       </c>
       <c r="K17" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="K17" si="39">K18+K19</f>
         <v>-50</v>
       </c>
       <c r="L17" s="17">
@@ -2990,13 +3048,13 @@
         <f>L17/F17</f>
         <v>0.28825857519788917</v>
       </c>
-      <c r="N17" s="16">
+      <c r="N17" s="88">
         <v>-211</v>
       </c>
-      <c r="O17" s="16">
+      <c r="O17" s="88">
         <v>95</v>
       </c>
-      <c r="P17" s="16">
+      <c r="P17" s="88">
         <f>O17+N17</f>
         <v>-116</v>
       </c>
@@ -3005,7 +3063,7 @@
         <v>-25.56476</v>
       </c>
       <c r="R17" s="19">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>19.00095</v>
       </c>
       <c r="S17" s="19">
@@ -3070,11 +3128,11 @@
         <v>21.75</v>
       </c>
       <c r="AK17" s="16">
-        <f t="shared" ref="AK17:AL17" si="41">AR17-AN17</f>
+        <f t="shared" ref="AK17:AL17" si="40">AR17-AN17</f>
         <v>519</v>
       </c>
       <c r="AL17" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>203</v>
       </c>
       <c r="AM17" s="17">
@@ -3102,7 +3160,7 @@
         <v>80</v>
       </c>
       <c r="AT17" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>-354</v>
       </c>
       <c r="AU17" s="19">
@@ -3110,7 +3168,7 @@
         <v>-52.583440000000003</v>
       </c>
       <c r="AV17" s="19">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>16.000799999999998</v>
       </c>
       <c r="AW17" s="19">
@@ -3149,8 +3207,14 @@
       <c r="C18" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
+      <c r="D18" s="47">
+        <f>ROUND(J18/M17,0)</f>
+        <v>-1100</v>
+      </c>
+      <c r="E18" s="47">
+        <f>ROUND(K18/M17,0)</f>
+        <v>-153</v>
+      </c>
       <c r="F18" s="47"/>
       <c r="G18" s="43">
         <v>149</v>
@@ -3167,9 +3231,9 @@
       </c>
       <c r="L18" s="47"/>
       <c r="M18" s="45"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
+      <c r="N18" s="89"/>
+      <c r="O18" s="89"/>
+      <c r="P18" s="89"/>
       <c r="Q18" s="46"/>
       <c r="R18" s="46"/>
       <c r="S18" s="46"/>
@@ -3218,8 +3282,14 @@
       <c r="C19" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="47"/>
+      <c r="D19" s="43">
+        <f>ROUND(J19/M17,0)</f>
+        <v>-239</v>
+      </c>
+      <c r="E19" s="47">
+        <f>ROUND(K19/M17,0)</f>
+        <v>-21</v>
+      </c>
       <c r="F19" s="47"/>
       <c r="G19" s="43">
         <v>26</v>
@@ -3236,9 +3306,9 @@
       </c>
       <c r="L19" s="47"/>
       <c r="M19" s="45"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47"/>
+      <c r="N19" s="89"/>
+      <c r="O19" s="89"/>
+      <c r="P19" s="89"/>
       <c r="Q19" s="46"/>
       <c r="R19" s="46"/>
       <c r="S19" s="46"/>
@@ -3297,14 +3367,14 @@
       <c r="K20" s="29"/>
       <c r="L20" s="29"/>
       <c r="M20" s="31"/>
-      <c r="N20" s="29">
+      <c r="N20" s="90">
         <v>-145</v>
       </c>
-      <c r="O20" s="29">
+      <c r="O20" s="90">
         <v>69</v>
       </c>
-      <c r="P20" s="29">
-        <f t="shared" ref="P20:P22" si="42">O20+N20</f>
+      <c r="P20" s="90">
+        <f t="shared" ref="P20:P22" si="41">O20+N20</f>
         <v>-76</v>
       </c>
       <c r="Q20" s="32">
@@ -3338,7 +3408,7 @@
       <c r="AM20" s="72"/>
       <c r="AN20" s="71"/>
       <c r="AO20" s="72"/>
-      <c r="AP20" s="87"/>
+      <c r="AP20" s="80"/>
       <c r="AQ20" s="31"/>
       <c r="AR20" s="29">
         <v>-275</v>
@@ -3347,7 +3417,7 @@
         <v>99</v>
       </c>
       <c r="AT20" s="29">
-        <f t="shared" ref="AT20:AT22" si="43">AS20+AR20</f>
+        <f t="shared" ref="AT20:AT22" si="42">AS20+AR20</f>
         <v>-176</v>
       </c>
       <c r="AU20" s="32">
@@ -3384,14 +3454,14 @@
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
       <c r="M21" s="31"/>
-      <c r="N21" s="29">
+      <c r="N21" s="90">
         <v>2</v>
       </c>
-      <c r="O21" s="29">
+      <c r="O21" s="90">
         <v>62</v>
       </c>
-      <c r="P21" s="29">
-        <f t="shared" si="42"/>
+      <c r="P21" s="90">
+        <f t="shared" si="41"/>
         <v>64</v>
       </c>
       <c r="Q21" s="32">
@@ -3425,7 +3495,7 @@
       <c r="AM21" s="72"/>
       <c r="AN21" s="71"/>
       <c r="AO21" s="72"/>
-      <c r="AP21" s="87"/>
+      <c r="AP21" s="80"/>
       <c r="AQ21" s="31"/>
       <c r="AR21" s="29">
         <v>-46</v>
@@ -3434,7 +3504,7 @@
         <v>33</v>
       </c>
       <c r="AT21" s="29">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-13</v>
       </c>
       <c r="AU21" s="32">
@@ -3475,22 +3545,22 @@
         <v>-1292</v>
       </c>
       <c r="G22" s="16">
-        <f t="shared" ref="G22:H22" si="44">G23+G24</f>
+        <f t="shared" ref="G22:H22" si="43">G23+G24</f>
         <v>191</v>
       </c>
       <c r="H22" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>157</v>
       </c>
       <c r="I22" s="17">
         <v>348</v>
       </c>
       <c r="J22" s="16">
-        <f t="shared" ref="J22:K22" si="45">J23+J24</f>
+        <f t="shared" ref="J22:K22" si="44">J23+J24</f>
         <v>-334</v>
       </c>
       <c r="K22" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>-26</v>
       </c>
       <c r="L22" s="17">
@@ -3501,23 +3571,23 @@
         <v>0.27863777089783281</v>
       </c>
       <c r="N22" s="16">
-        <f t="shared" ref="N22:O22" si="46">N21+N20</f>
+        <f t="shared" ref="N22:O22" si="45">N21+N20</f>
         <v>-143</v>
       </c>
       <c r="O22" s="16">
+        <f t="shared" si="45"/>
+        <v>131</v>
+      </c>
+      <c r="P22" s="16">
+        <f t="shared" si="41"/>
+        <v>-12</v>
+      </c>
+      <c r="Q22" s="19">
+        <f t="shared" ref="Q22:R22" si="46">Q20+Q21</f>
+        <v>-17.332979999999999</v>
+      </c>
+      <c r="R22" s="19">
         <f t="shared" si="46"/>
-        <v>131</v>
-      </c>
-      <c r="P22" s="16">
-        <f t="shared" si="42"/>
-        <v>-12</v>
-      </c>
-      <c r="Q22" s="19">
-        <f t="shared" ref="Q22:R22" si="47">Q20+Q21</f>
-        <v>-17.332979999999999</v>
-      </c>
-      <c r="R22" s="19">
-        <f t="shared" si="47"/>
         <v>22.664209999999997</v>
       </c>
       <c r="S22" s="19">
@@ -3584,22 +3654,22 @@
         <v>-33.03</v>
       </c>
       <c r="AK22" s="16">
-        <f t="shared" ref="AK22:AL22" si="48">AR22-AN22</f>
+        <f t="shared" ref="AK22:AL22" si="47">AR22-AN22</f>
         <v>544</v>
       </c>
       <c r="AL22" s="16">
-        <f t="shared" si="48"/>
+        <f t="shared" si="47"/>
         <v>199</v>
       </c>
       <c r="AM22" s="17">
         <v>743</v>
       </c>
       <c r="AN22" s="16">
-        <f t="shared" ref="AN22:AO22" si="49">D22-J22</f>
+        <f t="shared" ref="AN22:AO22" si="48">D22-J22</f>
         <v>-865</v>
       </c>
       <c r="AO22" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>-67</v>
       </c>
       <c r="AP22" s="17">
@@ -3618,15 +3688,15 @@
         <v>132</v>
       </c>
       <c r="AT22" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-189</v>
       </c>
       <c r="AU22" s="19">
-        <f t="shared" ref="AU22:AV22" si="50">AU20+AU21</f>
+        <f t="shared" ref="AU22:AV22" si="49">AU20+AU21</f>
         <v>-38.729060000000004</v>
       </c>
       <c r="AV22" s="19">
-        <f t="shared" si="50"/>
+        <f t="shared" si="49"/>
         <v>24.51867</v>
       </c>
       <c r="AW22" s="19">
@@ -3657,7 +3727,7 @@
         <v>-55.17</v>
       </c>
       <c r="BE22" s="26">
-        <f t="shared" ref="BE22" si="51">BC22+BB22+BD22</f>
+        <f t="shared" ref="BE22" si="50">BC22+BB22+BD22</f>
         <v>-43.03</v>
       </c>
     </row>
@@ -3667,8 +3737,14 @@
       <c r="C23" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
+      <c r="D23" s="30">
+        <f>ROUND(J23/M22,0)</f>
+        <v>-983</v>
+      </c>
+      <c r="E23" s="30">
+        <f>ROUND(K23/M22,0)</f>
+        <v>-83</v>
+      </c>
       <c r="F23" s="30"/>
       <c r="G23" s="30">
         <v>129</v>
@@ -3736,8 +3812,14 @@
       <c r="C24" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
+      <c r="D24" s="30">
+        <f>ROUND(J24/M22,0)</f>
+        <v>-215</v>
+      </c>
+      <c r="E24" s="30">
+        <f>ROUND(K24/M22,0)</f>
+        <v>-11</v>
+      </c>
       <c r="F24" s="30"/>
       <c r="G24" s="30">
         <v>62</v>
@@ -3808,11 +3890,11 @@
         <v>45610</v>
       </c>
       <c r="D25" s="53">
-        <f t="shared" ref="D25:D27" si="52">ROUND(J25/M25,0)</f>
+        <f t="shared" ref="D25:D27" si="51">ROUND(J25/M25,0)</f>
         <v>-973</v>
       </c>
       <c r="E25" s="53">
-        <f t="shared" ref="E25:E27" si="53">ROUND(K25/M25,0)</f>
+        <f t="shared" ref="E25:E27" si="52">ROUND(K25/M25,0)</f>
         <v>-17</v>
       </c>
       <c r="F25" s="53">
@@ -3837,7 +3919,7 @@
         <v>-357</v>
       </c>
       <c r="M25" s="54">
-        <f t="shared" ref="M25:M27" si="54">L25/F25</f>
+        <f t="shared" ref="M25:M27" si="53">L25/F25</f>
         <v>0.3606060606060606</v>
       </c>
       <c r="N25" s="55">
@@ -3847,19 +3929,19 @@
         <v>191</v>
       </c>
       <c r="P25" s="55">
-        <f t="shared" ref="P25:P27" si="55">O25+N25</f>
+        <f t="shared" ref="P25:P27" si="54">O25+N25</f>
         <v>59</v>
       </c>
       <c r="Q25" s="56">
-        <f t="shared" ref="Q25:Q27" si="56">N25*0.11761</f>
+        <f t="shared" ref="Q25:Q27" si="55">N25*0.11761</f>
         <v>-15.524520000000001</v>
       </c>
       <c r="R25" s="56">
-        <f t="shared" ref="R25:R27" si="57">O25*0.14296</f>
+        <f t="shared" ref="R25:R27" si="56">O25*0.14296</f>
         <v>27.30536</v>
       </c>
       <c r="S25" s="56">
-        <f t="shared" ref="S25:S27" si="58">R25+Q25</f>
+        <f t="shared" ref="S25:S27" si="57">R25+Q25</f>
         <v>11.78084</v>
       </c>
       <c r="T25" s="56">
@@ -3867,19 +3949,19 @@
         <v>-1.32</v>
       </c>
       <c r="U25" s="20">
-        <f t="shared" ref="U25:U27" si="59">(ABS(Q25)+ABS(R25))/(ABS(N25)+ABS(O25))</f>
+        <f t="shared" ref="U25:U27" si="58">(ABS(Q25)+ABS(R25))/(ABS(N25)+ABS(O25))</f>
         <v>0.13260024767801859</v>
       </c>
       <c r="V25" s="21">
-        <f t="shared" ref="V25:V27" si="60">ABS(R25)/ABS(O25)</f>
+        <f t="shared" ref="V25:V27" si="59">ABS(R25)/ABS(O25)</f>
         <v>0.14296</v>
       </c>
       <c r="W25" s="21">
-        <f t="shared" ref="W25:W27" si="61">Q25/N25</f>
+        <f t="shared" ref="W25:W27" si="60">Q25/N25</f>
         <v>0.11761000000000001</v>
       </c>
       <c r="X25" s="22">
-        <f t="shared" ref="X25:X26" si="62">Q25+R25+T25+0.02</f>
+        <f t="shared" ref="X25:X26" si="61">Q25+R25+T25+0.02</f>
         <v>10.480839999999999</v>
       </c>
       <c r="Y25" s="23">
@@ -3898,7 +3980,7 @@
         <v>3.43</v>
       </c>
       <c r="AD25" s="22">
-        <f t="shared" ref="AD25:AD27" si="63">AC25+AB25+AA25</f>
+        <f t="shared" ref="AD25:AD27" si="62">AC25+AB25+AA25</f>
         <v>25.380000000000003</v>
       </c>
       <c r="AE25" s="56">
@@ -3911,7 +3993,7 @@
         <v>0</v>
       </c>
       <c r="AH25" s="57">
-        <f t="shared" ref="AH25:AH27" si="64">AE25+AF25+AG25</f>
+        <f t="shared" ref="AH25:AH27" si="63">AE25+AF25+AG25</f>
         <v>21.36</v>
       </c>
       <c r="AI25" s="58"/>
@@ -3948,19 +4030,19 @@
         <v>157</v>
       </c>
       <c r="AT25" s="55">
-        <f t="shared" ref="AT25:AT27" si="65">AS25+AR25</f>
+        <f t="shared" ref="AT25:AT27" si="64">AS25+AR25</f>
         <v>22</v>
       </c>
       <c r="AU25" s="56">
-        <f t="shared" ref="AU25:AU27" si="66">AR25*0.11761</f>
+        <f t="shared" ref="AU25:AU27" si="65">AR25*0.11761</f>
         <v>-15.877350000000002</v>
       </c>
       <c r="AV25" s="56">
-        <f t="shared" ref="AV25:AV27" si="67">AS25*0.14296</f>
+        <f t="shared" ref="AV25:AV27" si="66">AS25*0.14296</f>
         <v>22.44472</v>
       </c>
       <c r="AW25" s="56">
-        <f t="shared" ref="AW25:AW27" si="68">AV25+AU25</f>
+        <f t="shared" ref="AW25:AW27" si="67">AV25+AU25</f>
         <v>6.5673699999999986</v>
       </c>
       <c r="AX25" s="56">
@@ -3971,7 +4053,7 @@
         <v>0.01</v>
       </c>
       <c r="AZ25" s="22">
-        <f t="shared" ref="AZ25:AZ27" si="69">AY25+AX25+AW25</f>
+        <f t="shared" ref="AZ25:AZ27" si="68">AY25+AX25+AW25</f>
         <v>5.2273699999999987</v>
       </c>
       <c r="BA25" s="23">
@@ -3985,7 +4067,7 @@
       </c>
       <c r="BD25" s="56"/>
       <c r="BE25" s="26">
-        <f t="shared" ref="BE25:BE27" si="70">BC25+BB25+BD25</f>
+        <f t="shared" ref="BE25:BE27" si="69">BC25+BB25+BD25</f>
         <v>11.36</v>
       </c>
     </row>
@@ -3998,11 +4080,11 @@
         <v>45643</v>
       </c>
       <c r="D26" s="16">
+        <f t="shared" si="51"/>
+        <v>-605</v>
+      </c>
+      <c r="E26" s="16">
         <f t="shared" si="52"/>
-        <v>-605</v>
-      </c>
-      <c r="E26" s="16">
-        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="F26" s="17">
@@ -4027,7 +4109,7 @@
         <v>-206</v>
       </c>
       <c r="M26" s="18">
-        <f t="shared" si="54"/>
+        <f t="shared" si="53"/>
         <v>0.34049586776859503</v>
       </c>
       <c r="N26" s="16">
@@ -4037,38 +4119,38 @@
         <v>214</v>
       </c>
       <c r="P26" s="16">
+        <f t="shared" si="54"/>
+        <v>358</v>
+      </c>
+      <c r="Q26" s="19">
         <f t="shared" si="55"/>
-        <v>358</v>
-      </c>
-      <c r="Q26" s="19">
+        <v>16.935840000000002</v>
+      </c>
+      <c r="R26" s="19">
         <f t="shared" si="56"/>
-        <v>16.935840000000002</v>
-      </c>
-      <c r="R26" s="19">
+        <v>30.593440000000001</v>
+      </c>
+      <c r="S26" s="19">
         <f t="shared" si="57"/>
-        <v>30.593440000000001</v>
-      </c>
-      <c r="S26" s="19">
+        <v>47.52928</v>
+      </c>
+      <c r="T26" s="19">
+        <v>0</v>
+      </c>
+      <c r="U26" s="20">
         <f t="shared" si="58"/>
-        <v>47.52928</v>
-      </c>
-      <c r="T26" s="19">
-        <v>0</v>
-      </c>
-      <c r="U26" s="20">
+        <v>0.13276335195530725</v>
+      </c>
+      <c r="V26" s="21">
         <f t="shared" si="59"/>
-        <v>0.13276335195530725</v>
-      </c>
-      <c r="V26" s="21">
+        <v>0.14296</v>
+      </c>
+      <c r="W26" s="21">
         <f t="shared" si="60"/>
-        <v>0.14296</v>
-      </c>
-      <c r="W26" s="21">
+        <v>0.11761000000000002</v>
+      </c>
+      <c r="X26" s="22">
         <f t="shared" si="61"/>
-        <v>0.11761000000000002</v>
-      </c>
-      <c r="X26" s="22">
-        <f t="shared" si="62"/>
         <v>47.549280000000003</v>
       </c>
       <c r="Y26" s="23">
@@ -4087,7 +4169,7 @@
         <v>8.11</v>
       </c>
       <c r="AD26" s="22">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>92.03</v>
       </c>
       <c r="AE26" s="19">
@@ -4100,7 +4182,7 @@
         <v>0</v>
       </c>
       <c r="AH26" s="25">
-        <f t="shared" si="64"/>
+        <f t="shared" si="63"/>
         <v>22.14</v>
       </c>
       <c r="AI26" s="59"/>
@@ -4109,11 +4191,11 @@
         <v>22.14</v>
       </c>
       <c r="AK26" s="16">
-        <f t="shared" ref="AK26:AL26" si="71">AR26-AN26</f>
+        <f t="shared" ref="AK26:AL26" si="70">AR26-AN26</f>
         <v>599</v>
       </c>
       <c r="AL26" s="16">
-        <f t="shared" si="71"/>
+        <f t="shared" si="70"/>
         <v>242</v>
       </c>
       <c r="AM26" s="17">
@@ -4141,19 +4223,19 @@
         <v>242</v>
       </c>
       <c r="AT26" s="16">
+        <f t="shared" si="64"/>
+        <v>442</v>
+      </c>
+      <c r="AU26" s="19">
         <f t="shared" si="65"/>
-        <v>442</v>
-      </c>
-      <c r="AU26" s="19">
+        <v>23.522000000000002</v>
+      </c>
+      <c r="AV26" s="19">
         <f t="shared" si="66"/>
-        <v>23.522000000000002</v>
-      </c>
-      <c r="AV26" s="19">
+        <v>34.596319999999999</v>
+      </c>
+      <c r="AW26" s="19">
         <f t="shared" si="67"/>
-        <v>34.596319999999999</v>
-      </c>
-      <c r="AW26" s="19">
-        <f t="shared" si="68"/>
         <v>58.118319999999997</v>
       </c>
       <c r="AX26" s="19">
@@ -4163,7 +4245,7 @@
         <v>0.13</v>
       </c>
       <c r="AZ26" s="22">
-        <f t="shared" si="69"/>
+        <f t="shared" si="68"/>
         <v>58.24832</v>
       </c>
       <c r="BA26" s="23">
@@ -4177,7 +4259,7 @@
       </c>
       <c r="BD26" s="19"/>
       <c r="BE26" s="26">
-        <f t="shared" si="70"/>
+        <f t="shared" si="69"/>
         <v>12.14</v>
       </c>
     </row>
@@ -4190,40 +4272,40 @@
         <v>45673</v>
       </c>
       <c r="D27" s="16">
+        <f t="shared" si="51"/>
+        <v>-309</v>
+      </c>
+      <c r="E27" s="16">
         <f t="shared" si="52"/>
-        <v>-309</v>
-      </c>
-      <c r="E27" s="16">
-        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="F27" s="17">
         <v>-309</v>
       </c>
       <c r="G27" s="16">
-        <f t="shared" ref="G27:H27" si="72">G28+G29</f>
+        <f t="shared" ref="G27:H27" si="71">G28+G29</f>
         <v>489</v>
       </c>
       <c r="H27" s="16">
-        <f t="shared" si="72"/>
+        <f t="shared" si="71"/>
         <v>332</v>
       </c>
       <c r="I27" s="17">
         <v>821</v>
       </c>
       <c r="J27" s="16">
-        <f t="shared" ref="J27:K27" si="73">J28+J29</f>
+        <f t="shared" ref="J27:K27" si="72">J28+J29</f>
         <v>-210</v>
       </c>
       <c r="K27" s="16">
-        <f t="shared" si="73"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="L27" s="17">
         <v>-210</v>
       </c>
       <c r="M27" s="18">
-        <f t="shared" si="54"/>
+        <f t="shared" si="53"/>
         <v>0.67961165048543692</v>
       </c>
       <c r="N27" s="16">
@@ -4233,34 +4315,34 @@
         <v>332</v>
       </c>
       <c r="P27" s="16">
+        <f t="shared" si="54"/>
+        <v>611</v>
+      </c>
+      <c r="Q27" s="19">
         <f t="shared" si="55"/>
-        <v>611</v>
-      </c>
-      <c r="Q27" s="19">
+        <v>32.813189999999999</v>
+      </c>
+      <c r="R27" s="19">
         <f t="shared" si="56"/>
-        <v>32.813189999999999</v>
-      </c>
-      <c r="R27" s="19">
+        <v>47.462720000000004</v>
+      </c>
+      <c r="S27" s="19">
         <f t="shared" si="57"/>
-        <v>47.462720000000004</v>
-      </c>
-      <c r="S27" s="19">
+        <v>80.27591000000001</v>
+      </c>
+      <c r="T27" s="19">
+        <v>0</v>
+      </c>
+      <c r="U27" s="20">
         <f t="shared" si="58"/>
-        <v>80.27591000000001</v>
-      </c>
-      <c r="T27" s="19">
-        <v>0</v>
-      </c>
-      <c r="U27" s="20">
+        <v>0.1313844680851064</v>
+      </c>
+      <c r="V27" s="21">
         <f t="shared" si="59"/>
-        <v>0.1313844680851064</v>
-      </c>
-      <c r="V27" s="21">
+        <v>0.14296</v>
+      </c>
+      <c r="W27" s="21">
         <f t="shared" si="60"/>
-        <v>0.14296</v>
-      </c>
-      <c r="W27" s="21">
-        <f t="shared" si="61"/>
         <v>0.11760999999999999</v>
       </c>
       <c r="X27" s="22">
@@ -4283,7 +4365,7 @@
         <v>12.56</v>
       </c>
       <c r="AD27" s="22">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>172.51999999999998</v>
       </c>
       <c r="AE27" s="19">
@@ -4296,7 +4378,7 @@
         <v>0</v>
       </c>
       <c r="AH27" s="25">
-        <f t="shared" si="64"/>
+        <f t="shared" si="63"/>
         <v>22.53</v>
       </c>
       <c r="AI27" s="59"/>
@@ -4305,11 +4387,11 @@
         <v>22.53</v>
       </c>
       <c r="AK27" s="16">
-        <f t="shared" ref="AK27:AL27" si="74">AR27-AN27</f>
+        <f t="shared" ref="AK27:AL27" si="73">AR27-AN27</f>
         <v>693</v>
       </c>
       <c r="AL27" s="16">
-        <f t="shared" si="74"/>
+        <f t="shared" si="73"/>
         <v>231</v>
       </c>
       <c r="AM27" s="17">
@@ -4337,19 +4419,19 @@
         <v>231</v>
       </c>
       <c r="AT27" s="16">
+        <f t="shared" si="64"/>
+        <v>825</v>
+      </c>
+      <c r="AU27" s="19">
         <f t="shared" si="65"/>
-        <v>825</v>
-      </c>
-      <c r="AU27" s="19">
+        <v>69.860340000000008</v>
+      </c>
+      <c r="AV27" s="19">
         <f t="shared" si="66"/>
-        <v>69.860340000000008</v>
-      </c>
-      <c r="AV27" s="19">
+        <v>33.023760000000003</v>
+      </c>
+      <c r="AW27" s="19">
         <f t="shared" si="67"/>
-        <v>33.023760000000003</v>
-      </c>
-      <c r="AW27" s="19">
-        <f t="shared" si="68"/>
         <v>102.88410000000002</v>
       </c>
       <c r="AX27" s="19">
@@ -4359,7 +4441,7 @@
         <v>0.25</v>
       </c>
       <c r="AZ27" s="22">
-        <f t="shared" si="69"/>
+        <f t="shared" si="68"/>
         <v>103.13410000000002</v>
       </c>
       <c r="BA27" s="24">
@@ -4373,7 +4455,7 @@
       </c>
       <c r="BD27" s="19"/>
       <c r="BE27" s="26">
-        <f t="shared" si="70"/>
+        <f t="shared" si="69"/>
         <v>12.53</v>
       </c>
     </row>
@@ -4383,8 +4465,14 @@
       <c r="C28" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
+      <c r="D28" s="47">
+        <f>ROUND(J28/M27,0)</f>
+        <v>-283</v>
+      </c>
+      <c r="E28" s="47">
+        <f>ROUND(K28/M27,0)</f>
+        <v>0</v>
+      </c>
       <c r="F28" s="34"/>
       <c r="G28" s="34">
         <v>370</v>
@@ -4452,8 +4540,14 @@
       <c r="C29" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
+      <c r="D29" s="47">
+        <f>ROUND(J29/M27,0)</f>
+        <v>-26</v>
+      </c>
+      <c r="E29" s="47">
+        <f>ROUND(K29/M27,0)</f>
+        <v>0</v>
+      </c>
       <c r="F29" s="34"/>
       <c r="G29" s="34">
         <v>119</v>
@@ -4577,15 +4671,15 @@
         <v>-10</v>
       </c>
       <c r="U30" s="20">
-        <f t="shared" ref="U30:U31" si="75">(ABS(Q30)+ABS(R30))/(ABS(N30)+ABS(O30))</f>
+        <f t="shared" ref="U30:U31" si="74">(ABS(Q30)+ABS(R30))/(ABS(N30)+ABS(O30))</f>
         <v>0.12236459709379127</v>
       </c>
       <c r="V30" s="21">
-        <f t="shared" ref="V30:V31" si="76">ABS(R30)/ABS(O30)</f>
+        <f t="shared" ref="V30:V31" si="75">ABS(R30)/ABS(O30)</f>
         <v>0.14295774647887324</v>
       </c>
       <c r="W30" s="21">
-        <f t="shared" ref="W30:W31" si="77">Q30/N30</f>
+        <f t="shared" ref="W30:W31" si="76">Q30/N30</f>
         <v>0.11760975609756097</v>
       </c>
       <c r="X30" s="22">
@@ -4622,7 +4716,7 @@
         <v>0</v>
       </c>
       <c r="AH30" s="25">
-        <f t="shared" ref="AH30:AH31" si="78">AE30+AF30+AG30</f>
+        <f t="shared" ref="AH30:AH31" si="77">AE30+AF30+AG30</f>
         <v>21.36</v>
       </c>
       <c r="AI30" s="59"/>
@@ -4631,11 +4725,11 @@
         <v>89.57</v>
       </c>
       <c r="AK30" s="16">
-        <f t="shared" ref="AK30:AL30" si="79">AR30-AN30</f>
+        <f t="shared" ref="AK30:AL30" si="78">AR30-AN30</f>
         <v>732</v>
       </c>
       <c r="AL30" s="16">
-        <f t="shared" si="79"/>
+        <f t="shared" si="78"/>
         <v>9</v>
       </c>
       <c r="AM30" s="17">
@@ -4662,7 +4756,7 @@
         <v>199</v>
       </c>
       <c r="AT30" s="16">
-        <f t="shared" ref="AT30:AT32" si="80">AS30+AR30</f>
+        <f t="shared" ref="AT30:AT32" si="79">AS30+AR30</f>
         <v>931</v>
       </c>
       <c r="AU30" s="19">
@@ -4674,7 +4768,7 @@
         <v>28.44904</v>
       </c>
       <c r="AW30" s="19">
-        <f t="shared" ref="AW30:AW31" si="81">AV30+AU30</f>
+        <f t="shared" ref="AW30:AW31" si="80">AV30+AU30</f>
         <v>114.53955999999999</v>
       </c>
       <c r="AX30" s="19">
@@ -4684,7 +4778,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="AZ30" s="22">
-        <f t="shared" ref="AZ30:AZ31" si="82">AY30+AX30+AW30</f>
+        <f t="shared" ref="AZ30:AZ31" si="81">AY30+AX30+AW30</f>
         <v>114.81956</v>
       </c>
       <c r="BA30" s="23">
@@ -4698,7 +4792,7 @@
       </c>
       <c r="BD30" s="19"/>
       <c r="BE30" s="26">
-        <f t="shared" ref="BE30:BE31" si="83">BC30+BB30+BD30</f>
+        <f t="shared" ref="BE30:BE31" si="82">BC30+BB30+BD30</f>
         <v>88.07</v>
       </c>
     </row>
@@ -4722,22 +4816,22 @@
         <v>-762</v>
       </c>
       <c r="G31" s="16">
-        <f t="shared" ref="G31:H31" si="84">G32+G33</f>
+        <f t="shared" ref="G31:H31" si="83">G32+G33</f>
         <v>321</v>
       </c>
       <c r="H31" s="16">
-        <f t="shared" si="84"/>
+        <f t="shared" si="83"/>
         <v>286</v>
       </c>
       <c r="I31" s="17">
         <v>607</v>
       </c>
       <c r="J31" s="16">
-        <f t="shared" ref="J31:K31" si="85">J32+J33</f>
+        <f t="shared" ref="J31:K31" si="84">J32+J33</f>
         <v>-304</v>
       </c>
       <c r="K31" s="16">
-        <f t="shared" si="85"/>
+        <f t="shared" si="84"/>
         <v>-1</v>
       </c>
       <c r="L31" s="17">
@@ -4757,30 +4851,30 @@
         <v>302</v>
       </c>
       <c r="Q31" s="25">
-        <f t="shared" ref="Q31:S31" si="86">Q32+Q33</f>
+        <f t="shared" ref="Q31:S31" si="85">Q32+Q33</f>
         <v>1.9100000000000001</v>
       </c>
       <c r="R31" s="25">
-        <f t="shared" si="86"/>
+        <f t="shared" si="85"/>
         <v>38.949999999999996</v>
       </c>
       <c r="S31" s="25">
-        <f t="shared" si="86"/>
+        <f t="shared" si="85"/>
         <v>40.859999999999992</v>
       </c>
       <c r="T31" s="25">
         <v>0</v>
       </c>
       <c r="U31" s="20">
+        <f t="shared" si="74"/>
+        <v>0.1352980132450331</v>
+      </c>
+      <c r="V31" s="21">
         <f t="shared" si="75"/>
-        <v>0.1352980132450331</v>
-      </c>
-      <c r="V31" s="21">
+        <v>0.13666666666666666</v>
+      </c>
+      <c r="W31" s="21">
         <f t="shared" si="76"/>
-        <v>0.13666666666666666</v>
-      </c>
-      <c r="W31" s="21">
-        <f t="shared" si="77"/>
         <v>0.1123529411764706</v>
       </c>
       <c r="X31" s="22">
@@ -4815,7 +4909,7 @@
         <v>0</v>
       </c>
       <c r="AH31" s="25">
-        <f t="shared" si="78"/>
+        <f t="shared" si="77"/>
         <v>21.82</v>
       </c>
       <c r="AI31" s="16"/>
@@ -4824,11 +4918,11 @@
         <v>62.77</v>
       </c>
       <c r="AK31" s="16">
-        <f t="shared" ref="AK31:AL31" si="87">AR31-AN31</f>
+        <f t="shared" ref="AK31:AL31" si="86">AR31-AN31</f>
         <v>592</v>
       </c>
       <c r="AL31" s="16">
-        <f t="shared" si="87"/>
+        <f t="shared" si="86"/>
         <v>242</v>
       </c>
       <c r="AM31" s="17">
@@ -4850,27 +4944,27 @@
         <v>0.59973753280839892</v>
       </c>
       <c r="AR31" s="16">
-        <f t="shared" ref="AR31:AS31" si="88">AR32+AR33</f>
+        <f t="shared" ref="AR31:AS31" si="87">AR32+AR33</f>
         <v>136</v>
       </c>
       <c r="AS31" s="16">
+        <f t="shared" si="87"/>
+        <v>241</v>
+      </c>
+      <c r="AT31" s="16">
+        <f t="shared" si="79"/>
+        <v>377</v>
+      </c>
+      <c r="AU31" s="19">
+        <f t="shared" ref="AU31:AV31" si="88">AU32+AU33</f>
+        <v>15.293426873</v>
+      </c>
+      <c r="AV31" s="19">
         <f t="shared" si="88"/>
-        <v>241</v>
-      </c>
-      <c r="AT31" s="16">
+        <v>32.941085250999997</v>
+      </c>
+      <c r="AW31" s="19">
         <f t="shared" si="80"/>
-        <v>377</v>
-      </c>
-      <c r="AU31" s="19">
-        <f t="shared" ref="AU31:AV31" si="89">AU32+AU33</f>
-        <v>15.293426873</v>
-      </c>
-      <c r="AV31" s="19">
-        <f t="shared" si="89"/>
-        <v>32.941085250999997</v>
-      </c>
-      <c r="AW31" s="19">
-        <f t="shared" si="81"/>
         <v>48.234512123999998</v>
       </c>
       <c r="AX31" s="19">
@@ -4880,7 +4974,7 @@
         <v>0.11</v>
       </c>
       <c r="AZ31" s="22">
-        <f t="shared" si="82"/>
+        <f t="shared" si="81"/>
         <v>48.344512123999998</v>
       </c>
       <c r="BA31" s="23">
@@ -4895,7 +4989,7 @@
       </c>
       <c r="BD31" s="19"/>
       <c r="BE31" s="26">
-        <f t="shared" si="83"/>
+        <f t="shared" si="82"/>
         <v>60.164512123999998</v>
       </c>
     </row>
@@ -4905,8 +4999,14 @@
       <c r="C32" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
+      <c r="D32" s="47">
+        <f>ROUND(J32/M31,0)</f>
+        <v>-597</v>
+      </c>
+      <c r="E32" s="47">
+        <f>ROUND(K32/M31,0)</f>
+        <v>-2</v>
+      </c>
       <c r="F32" s="47"/>
       <c r="G32" s="43">
         <v>268</v>
@@ -4923,10 +5023,10 @@
       </c>
       <c r="L32" s="47"/>
       <c r="M32" s="45"/>
-      <c r="N32" s="86">
+      <c r="N32" s="79">
         <v>14.166700000000001</v>
       </c>
-      <c r="O32" s="86">
+      <c r="O32" s="79">
         <v>237.5</v>
       </c>
       <c r="P32" s="47"/>
@@ -4937,7 +5037,7 @@
         <v>32.159999999999997</v>
       </c>
       <c r="S32" s="46">
-        <f t="shared" ref="S32:S33" si="90">Q32+R32</f>
+        <f t="shared" ref="S32:S33" si="89">Q32+R32</f>
         <v>33.739999999999995</v>
       </c>
       <c r="T32" s="47"/>
@@ -4957,12 +5057,24 @@
       <c r="AH32" s="46"/>
       <c r="AI32" s="46"/>
       <c r="AJ32" s="46"/>
-      <c r="AK32" s="77"/>
-      <c r="AL32" s="77"/>
+      <c r="AK32" s="77">
+        <f>AR32-AN32</f>
+        <v>471.33330000000001</v>
+      </c>
+      <c r="AL32" s="77">
+        <f>AS32-AO32</f>
+        <v>201.83330000000001</v>
+      </c>
       <c r="AM32" s="47"/>
-      <c r="AN32" s="47"/>
-      <c r="AO32" s="47"/>
-      <c r="AP32" s="87"/>
+      <c r="AN32" s="47">
+        <f>D32-J32</f>
+        <v>-358</v>
+      </c>
+      <c r="AO32" s="47">
+        <f>E32-K32</f>
+        <v>-1</v>
+      </c>
+      <c r="AP32" s="48"/>
       <c r="AQ32" s="48"/>
       <c r="AR32" s="43">
         <v>113.33329999999999</v>
@@ -4971,7 +5083,7 @@
         <v>200.83330000000001</v>
       </c>
       <c r="AT32" s="47">
-        <f t="shared" si="80"/>
+        <f t="shared" si="79"/>
         <v>314.16660000000002</v>
       </c>
       <c r="AU32" s="46">
@@ -4998,8 +5110,14 @@
       <c r="C33" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
+      <c r="D33" s="47">
+        <f>ROUND(J33/M31,0)</f>
+        <v>-162</v>
+      </c>
+      <c r="E33" s="47">
+        <f>ROUND(K33/M31,0)</f>
+        <v>0</v>
+      </c>
       <c r="F33" s="47"/>
       <c r="G33" s="43">
         <v>53</v>
@@ -5016,10 +5134,10 @@
       </c>
       <c r="L33" s="47"/>
       <c r="M33" s="45"/>
-      <c r="N33" s="86">
+      <c r="N33" s="79">
         <v>2.8332999999999999</v>
       </c>
-      <c r="O33" s="86">
+      <c r="O33" s="79">
         <v>47.5</v>
       </c>
       <c r="P33" s="47"/>
@@ -5030,7 +5148,7 @@
         <v>6.79</v>
       </c>
       <c r="S33" s="46">
-        <f t="shared" si="90"/>
+        <f t="shared" si="89"/>
         <v>7.12</v>
       </c>
       <c r="T33" s="47"/>
@@ -5050,12 +5168,24 @@
       <c r="AH33" s="46"/>
       <c r="AI33" s="46"/>
       <c r="AJ33" s="46"/>
-      <c r="AK33" s="77"/>
-      <c r="AL33" s="77"/>
+      <c r="AK33" s="77">
+        <f>AR33-AN33</f>
+        <v>119.66669999999999</v>
+      </c>
+      <c r="AL33" s="77">
+        <f>AS33-AO33</f>
+        <v>40.166699999999999</v>
+      </c>
       <c r="AM33" s="47"/>
-      <c r="AN33" s="47"/>
-      <c r="AO33" s="47"/>
-      <c r="AP33" s="87"/>
+      <c r="AN33" s="47">
+        <f>D33-J33</f>
+        <v>-97</v>
+      </c>
+      <c r="AO33" s="47">
+        <f>E33-K33</f>
+        <v>0</v>
+      </c>
+      <c r="AP33" s="48"/>
       <c r="AQ33" s="48"/>
       <c r="AR33" s="43">
         <v>22.666699999999999</v>
@@ -5205,22 +5335,22 @@
         <v>207.22</v>
       </c>
       <c r="AK34" s="16">
-        <f t="shared" ref="AK34:AL34" si="91">AR34-AN34</f>
+        <f t="shared" ref="AK34:AL34" si="90">AR34-AN34</f>
         <v>582</v>
       </c>
       <c r="AL34" s="16">
-        <f t="shared" si="91"/>
+        <f t="shared" si="90"/>
         <v>212</v>
       </c>
       <c r="AM34" s="17">
         <v>794</v>
       </c>
       <c r="AN34" s="16">
-        <f t="shared" ref="AN34:AO34" si="92">D34-J34</f>
+        <f t="shared" ref="AN34:AO34" si="91">D34-J34</f>
         <v>-670</v>
       </c>
       <c r="AO34" s="16">
-        <f t="shared" si="92"/>
+        <f t="shared" si="91"/>
         <v>-60</v>
       </c>
       <c r="AP34" s="17">
@@ -6307,4 +6437,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2ED786-67CD-48BA-9E19-B5E9139740C0}">
+  <dimension ref="F5:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>-650</v>
+      </c>
+    </row>
+    <row r="6" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>-802</v>
+      </c>
+      <c r="G6">
+        <f>F6+F5</f>
+        <v>-1452</v>
+      </c>
+    </row>
+    <row r="8" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>-1601</v>
+      </c>
+    </row>
+    <row r="9" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>149</v>
+      </c>
+      <c r="G9">
+        <f>F9+F8</f>
+        <v>-1452</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
making progress on getting the data into sqlite proto
</commit_message>
<xml_diff>
--- a/python-notebooks/billing.xlsx
+++ b/python-notebooks/billing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klowe/repos-personal/energy-project/python-notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B15AE5-86C1-0342-A430-A63050279055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A28A1B-34C6-7F47-AE7E-CDA7A7073F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="29540" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Billing" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="101">
   <si>
     <t>303A ADU</t>
   </si>
@@ -262,11 +262,6 @@
 (36)</t>
   </si>
   <si>
-    <t xml:space="preserve"> PCE Generation Charges due in Cash 
-[$]
-(36)</t>
-  </si>
-  <si>
     <t>RES Energy Charges 
 [$]
 (31)</t>
@@ -297,10 +292,6 @@
 (41)</t>
   </si>
   <si>
-    <t>NEM True Up Adjustment
-[$]</t>
-  </si>
-  <si>
     <t>PG&amp;E Electric Delivery Charges
 [$]
 (30)</t>
@@ -326,11 +317,6 @@
 (13)</t>
   </si>
   <si>
-    <t>allocation 
-[%]
-(13)/(15)</t>
-  </si>
-  <si>
     <t>off peak [kWh]
 (21)</t>
   </si>
@@ -409,6 +395,25 @@
   </si>
   <si>
     <t xml:space="preserve">allocation [%] </t>
+  </si>
+  <si>
+    <t>Energy Commission Surcharge
+[$]
+(35)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PCE Generation Charges due in Cash 
+[$]
+(80)</t>
+  </si>
+  <si>
+    <t>allocation 
+[%]</t>
+  </si>
+  <si>
+    <t>NEM True Up Adjustment
+[$]
+(80)</t>
   </si>
 </sst>
 </file>
@@ -979,11 +984,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BE1012"/>
+  <dimension ref="A1:BF1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q40" sqref="Q40"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="AO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AL8" sqref="AL8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -999,39 +1004,39 @@
     <col min="16" max="16" width="7.1640625" customWidth="1"/>
     <col min="17" max="17" width="10.83203125" customWidth="1"/>
     <col min="18" max="19" width="10.5" customWidth="1"/>
-    <col min="20" max="24" width="10" customWidth="1"/>
-    <col min="25" max="25" width="11.1640625" customWidth="1"/>
-    <col min="26" max="26" width="13.33203125" customWidth="1"/>
-    <col min="27" max="27" width="10.83203125" customWidth="1"/>
-    <col min="28" max="29" width="8.83203125" customWidth="1"/>
-    <col min="30" max="30" width="13.83203125" customWidth="1"/>
-    <col min="31" max="31" width="8.83203125" customWidth="1"/>
-    <col min="32" max="32" width="10.5" customWidth="1"/>
-    <col min="33" max="33" width="11" customWidth="1"/>
-    <col min="34" max="34" width="13.1640625" customWidth="1"/>
-    <col min="35" max="36" width="8.83203125" customWidth="1"/>
-    <col min="37" max="38" width="8.6640625" customWidth="1"/>
-    <col min="39" max="39" width="9.83203125" customWidth="1"/>
-    <col min="40" max="41" width="8.6640625" customWidth="1"/>
-    <col min="42" max="42" width="8.83203125" customWidth="1"/>
-    <col min="43" max="44" width="10.6640625" customWidth="1"/>
-    <col min="45" max="45" width="10.83203125" customWidth="1"/>
-    <col min="46" max="46" width="8.6640625" customWidth="1"/>
-    <col min="47" max="47" width="11" customWidth="1"/>
-    <col min="48" max="49" width="10.6640625" customWidth="1"/>
-    <col min="50" max="50" width="11.1640625" customWidth="1"/>
-    <col min="51" max="51" width="12.83203125" customWidth="1"/>
-    <col min="52" max="52" width="8.6640625" customWidth="1"/>
-    <col min="53" max="54" width="11.1640625" customWidth="1"/>
-    <col min="55" max="55" width="12.6640625" customWidth="1"/>
-    <col min="56" max="56" width="10.83203125" customWidth="1"/>
-    <col min="57" max="57" width="8.6640625" customWidth="1"/>
+    <col min="20" max="25" width="10" customWidth="1"/>
+    <col min="26" max="26" width="11.1640625" customWidth="1"/>
+    <col min="27" max="27" width="13.33203125" customWidth="1"/>
+    <col min="28" max="28" width="10.83203125" customWidth="1"/>
+    <col min="29" max="30" width="8.83203125" customWidth="1"/>
+    <col min="31" max="31" width="13.83203125" customWidth="1"/>
+    <col min="32" max="32" width="8.83203125" customWidth="1"/>
+    <col min="33" max="33" width="10.5" customWidth="1"/>
+    <col min="34" max="34" width="11" customWidth="1"/>
+    <col min="35" max="35" width="13.1640625" customWidth="1"/>
+    <col min="36" max="37" width="8.83203125" customWidth="1"/>
+    <col min="38" max="39" width="8.6640625" customWidth="1"/>
+    <col min="40" max="40" width="9.83203125" customWidth="1"/>
+    <col min="41" max="42" width="8.6640625" customWidth="1"/>
+    <col min="43" max="43" width="8.83203125" customWidth="1"/>
+    <col min="44" max="45" width="10.6640625" customWidth="1"/>
+    <col min="46" max="46" width="10.83203125" customWidth="1"/>
+    <col min="47" max="47" width="8.6640625" customWidth="1"/>
+    <col min="48" max="48" width="11" customWidth="1"/>
+    <col min="49" max="50" width="10.6640625" customWidth="1"/>
+    <col min="51" max="51" width="11.1640625" customWidth="1"/>
+    <col min="52" max="52" width="12.83203125" customWidth="1"/>
+    <col min="53" max="53" width="8.6640625" customWidth="1"/>
+    <col min="54" max="55" width="11.1640625" customWidth="1"/>
+    <col min="56" max="56" width="12.6640625" customWidth="1"/>
+    <col min="57" max="57" width="10.83203125" customWidth="1"/>
+    <col min="58" max="58" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B2" s="70" t="s">
         <v>41</v>
@@ -1072,10 +1077,10 @@
       <c r="AH2" s="71"/>
       <c r="AI2" s="71"/>
       <c r="AJ2" s="71"/>
-      <c r="AK2" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="72"/>
+      <c r="AK2" s="71"/>
+      <c r="AL2" s="72" t="s">
+        <v>0</v>
+      </c>
       <c r="AM2" s="72"/>
       <c r="AN2" s="72"/>
       <c r="AO2" s="72"/>
@@ -1095,8 +1100,9 @@
       <c r="BC2" s="72"/>
       <c r="BD2" s="72"/>
       <c r="BE2" s="72"/>
+      <c r="BF2" s="72"/>
     </row>
-    <row r="3" spans="1:57" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:58" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1115,7 +1121,7 @@
       <c r="H3" s="74"/>
       <c r="I3" s="74"/>
       <c r="J3" s="73" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K3" s="74"/>
       <c r="L3" s="74"/>
@@ -1137,55 +1143,56 @@
       <c r="X3" s="74"/>
       <c r="Y3" s="74"/>
       <c r="Z3" s="74"/>
-      <c r="AA3" s="73" t="s">
+      <c r="AA3" s="74"/>
+      <c r="AB3" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="74"/>
       <c r="AC3" s="74"/>
       <c r="AD3" s="74"/>
       <c r="AE3" s="74"/>
       <c r="AF3" s="74"/>
       <c r="AG3" s="74"/>
       <c r="AH3" s="74"/>
-      <c r="AI3" s="54" t="s">
+      <c r="AI3" s="74"/>
+      <c r="AJ3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="AJ3" s="55"/>
-      <c r="AK3" s="73" t="s">
+      <c r="AK3" s="55"/>
+      <c r="AL3" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="AL3" s="74"/>
       <c r="AM3" s="74"/>
-      <c r="AN3" s="73" t="s">
+      <c r="AN3" s="74"/>
+      <c r="AO3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="AO3" s="74"/>
       <c r="AP3" s="74"/>
       <c r="AQ3" s="74"/>
-      <c r="AR3" s="73" t="s">
+      <c r="AR3" s="74"/>
+      <c r="AS3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="AS3" s="74"/>
       <c r="AT3" s="74"/>
-      <c r="AU3" s="75" t="s">
+      <c r="AU3" s="74"/>
+      <c r="AV3" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="AV3" s="74"/>
       <c r="AW3" s="74"/>
       <c r="AX3" s="74"/>
       <c r="AY3" s="74"/>
       <c r="AZ3" s="74"/>
       <c r="BA3" s="74"/>
       <c r="BB3" s="74"/>
-      <c r="BC3" s="54" t="s">
+      <c r="BC3" s="74"/>
+      <c r="BD3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="BD3" s="54" t="s">
+      <c r="BE3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="BE3" s="1"/>
+      <c r="BF3" s="1"/>
     </row>
-    <row r="4" spans="1:57" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:58" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -1250,16 +1257,16 @@
       <c r="V4" s="51"/>
       <c r="W4" s="51"/>
       <c r="X4" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y4" s="51" t="s">
         <v>14</v>
-      </c>
-      <c r="Y4" s="51" t="s">
-        <v>11</v>
       </c>
       <c r="Z4" s="51" t="s">
         <v>11</v>
       </c>
       <c r="AA4" s="51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AB4" s="51" t="s">
         <v>13</v>
@@ -1277,52 +1284,52 @@
         <v>13</v>
       </c>
       <c r="AG4" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH4" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="AH4" s="51" t="s">
+      <c r="AI4" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ4" s="52"/>
-      <c r="AK4" s="51"/>
+      <c r="AJ4" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK4" s="52"/>
       <c r="AL4" s="51"/>
-      <c r="AM4" s="51" t="s">
+      <c r="AM4" s="51"/>
+      <c r="AN4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AN4" s="51"/>
       <c r="AO4" s="51"/>
-      <c r="AP4" s="51" t="s">
+      <c r="AP4" s="51"/>
+      <c r="AQ4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AQ4" s="51"/>
-      <c r="AR4" s="51" t="s">
-        <v>11</v>
-      </c>
+      <c r="AR4" s="51"/>
       <c r="AS4" s="51" t="s">
         <v>11</v>
       </c>
       <c r="AT4" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU4" s="51" t="s">
         <v>13</v>
-      </c>
-      <c r="AU4" s="51" t="s">
-        <v>11</v>
       </c>
       <c r="AV4" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AW4" s="51"/>
-      <c r="AX4" s="51" t="s">
+      <c r="AW4" s="51" t="s">
         <v>11</v>
       </c>
+      <c r="AX4" s="51"/>
       <c r="AY4" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AZ4" s="51"/>
-      <c r="BA4" s="51" t="s">
+      <c r="AZ4" s="51" t="s">
         <v>11</v>
       </c>
+      <c r="BA4" s="51"/>
       <c r="BB4" s="51" t="s">
         <v>11</v>
       </c>
@@ -1330,11 +1337,14 @@
         <v>11</v>
       </c>
       <c r="BD4" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="BE4" s="53"/>
+        <v>11</v>
+      </c>
+      <c r="BE4" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF4" s="53"/>
     </row>
-    <row r="5" spans="1:57" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:58" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="51" t="s">
         <v>16</v>
       </c>
@@ -1391,16 +1401,16 @@
       <c r="V5" s="51"/>
       <c r="W5" s="51"/>
       <c r="X5" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y5" s="51" t="s">
         <v>14</v>
-      </c>
-      <c r="Y5" s="51" t="s">
-        <v>23</v>
       </c>
       <c r="Z5" s="51" t="s">
         <v>23</v>
       </c>
       <c r="AA5" s="51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AB5" s="51" t="s">
         <v>24</v>
@@ -1418,72 +1428,75 @@
         <v>24</v>
       </c>
       <c r="AG5" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH5" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="AH5" s="51" t="s">
+      <c r="AI5" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="AI5" s="51" t="s">
+      <c r="AJ5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="AJ5" s="52"/>
-      <c r="AK5" s="51"/>
+      <c r="AK5" s="52"/>
       <c r="AL5" s="51"/>
-      <c r="AM5" s="51" t="s">
+      <c r="AM5" s="51"/>
+      <c r="AN5" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="AN5" s="51"/>
       <c r="AO5" s="51"/>
-      <c r="AP5" s="51" t="s">
+      <c r="AP5" s="51"/>
+      <c r="AQ5" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="AQ5" s="51"/>
-      <c r="AR5" s="51" t="s">
-        <v>23</v>
-      </c>
+      <c r="AR5" s="51"/>
       <c r="AS5" s="51" t="s">
         <v>23</v>
       </c>
       <c r="AT5" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="AU5" s="51" t="s">
         <v>19</v>
-      </c>
-      <c r="AU5" s="51" t="s">
-        <v>23</v>
       </c>
       <c r="AV5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="AW5" s="51"/>
-      <c r="AX5" s="51" t="s">
+      <c r="AW5" s="51" t="s">
         <v>23</v>
       </c>
+      <c r="AX5" s="51"/>
       <c r="AY5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="AZ5" s="51"/>
-      <c r="BA5" s="51" t="s">
+      <c r="AZ5" s="51" t="s">
         <v>23</v>
       </c>
+      <c r="BA5" s="51"/>
       <c r="BB5" s="51" t="s">
         <v>23</v>
       </c>
       <c r="BC5" s="51" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="BD5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="BE5" s="53"/>
+      <c r="BE5" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="BF5" s="53"/>
     </row>
-    <row r="6" spans="1:57" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:58" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>95</v>
-      </c>
       <c r="C6" s="51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D6" s="51" t="s">
         <v>44</v>
@@ -1513,7 +1526,7 @@
         <v>52</v>
       </c>
       <c r="M6" s="51" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N6" s="51" t="s">
         <v>53</v>
@@ -1546,109 +1559,112 @@
         <v>62</v>
       </c>
       <c r="X6" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y6" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="Y6" s="51" t="s">
+      <c r="Z6" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="Z6" s="51" t="s">
+      <c r="AA6" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB6" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="AA6" s="51" t="s">
+      <c r="AC6" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="AB6" s="51" t="s">
+      <c r="AD6" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="AC6" s="51" t="s">
+      <c r="AE6" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="AD6" s="51" t="s">
+      <c r="AF6" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="AE6" s="51" t="s">
+      <c r="AG6" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="AF6" s="51" t="s">
+      <c r="AH6" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI6" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="AG6" s="51" t="s">
+      <c r="AJ6" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK6" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="AH6" s="51" t="s">
+      <c r="AL6" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="AI6" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ6" s="52" t="s">
+      <c r="AM6" s="51" t="s">
         <v>74</v>
-      </c>
-      <c r="AK6" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL6" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM6" s="51" t="s">
-        <v>77</v>
       </c>
       <c r="AN6" s="51" t="s">
         <v>75</v>
       </c>
       <c r="AO6" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="AP6" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ6" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="AP6" s="51" t="s">
+      <c r="AR6" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="AS6" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT6" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="AQ6" s="51" t="s">
+      <c r="AU6" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="AR6" s="51" t="s">
+      <c r="AV6" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW6" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="AS6" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT6" s="51" t="s">
+      <c r="AX6" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY6" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="AU6" s="51" t="s">
+      <c r="AZ6" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA6" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB6" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="AV6" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="AW6" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="AX6" s="51" t="s">
+      <c r="BC6" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="AY6" s="51" t="s">
+      <c r="BD6" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="AZ6" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="BA6" s="51" t="s">
+      <c r="BE6" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="BF6" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="BB6" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC6" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="BD6" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="BE6" s="53" t="s">
-        <v>90</v>
-      </c>
     </row>
-    <row r="7" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="13">
         <v>45419</v>
@@ -1708,7 +1724,7 @@
         <v>4.7900799999999997</v>
       </c>
       <c r="S7" s="17">
-        <f t="shared" ref="S7:S8" si="1">R7+Q7</f>
+        <f>R7+Q7</f>
         <v>-12.963229999999999</v>
       </c>
       <c r="T7" s="17">
@@ -1716,133 +1732,140 @@
         <v>-1.41</v>
       </c>
       <c r="U7" s="18">
-        <f t="shared" ref="U7:U8" si="2">(ABS(Q7)+ABS(R7))/(ABS(N7)+ABS(O7))</f>
+        <f t="shared" ref="U7:U8" si="1">(ABS(Q7)+ABS(R7))/(ABS(N7)+ABS(O7))</f>
         <v>0.130308612716763</v>
       </c>
       <c r="V7" s="19">
-        <f t="shared" ref="V7:V8" si="3">ABS(R7)/ABS(O7)</f>
+        <f t="shared" ref="V7:V8" si="2">ABS(R7)/ABS(O7)</f>
         <v>0.14968999999999999</v>
       </c>
       <c r="W7" s="19">
-        <f t="shared" ref="W7:W8" si="4">Q7/N7</f>
+        <f t="shared" ref="W7:W8" si="3">Q7/N7</f>
         <v>0.12590999999999999</v>
       </c>
       <c r="X7" s="20">
-        <f t="shared" ref="X7:X8" si="5">Q7+R7+T7+0</f>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="20">
+        <f>Q7+R7+T7+X7</f>
         <v>-14.37323</v>
       </c>
-      <c r="Y7" s="21">
+      <c r="Z7" s="21">
         <v>24.37</v>
       </c>
-      <c r="Z7" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="17">
+      <c r="AA7" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="17">
         <v>-24.4</v>
       </c>
-      <c r="AB7" s="17">
+      <c r="AC7" s="17">
         <v>11.7</v>
       </c>
-      <c r="AC7" s="17">
+      <c r="AD7" s="17">
         <v>1.1100000000000001</v>
       </c>
-      <c r="AD7" s="20">
-        <f t="shared" ref="AD7:AD8" si="6">AC7+AB7+AA7</f>
+      <c r="AE7" s="20">
+        <f t="shared" ref="AE7:AE8" si="4">AD7+AC7+AB7</f>
         <v>-11.59</v>
       </c>
-      <c r="AE7" s="17">
+      <c r="AF7" s="17">
         <v>60</v>
       </c>
-      <c r="AF7" s="17">
+      <c r="AG7" s="17">
         <v>7.83</v>
       </c>
-      <c r="AG7" s="17">
-        <v>0</v>
-      </c>
       <c r="AH7" s="17">
-        <f>AE7+AF7+AG7</f>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="17">
+        <f>AF7+AG7+AH7</f>
         <v>67.83</v>
       </c>
-      <c r="AI7" s="15"/>
-      <c r="AJ7" s="22">
-        <f>Z7+AH7+AI7</f>
+      <c r="AJ7" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="22">
+        <f>AA7+AI7+AJ7</f>
         <v>67.83</v>
       </c>
-      <c r="AK7" s="15">
-        <f>AR7-AN7</f>
+      <c r="AL7" s="15">
+        <f>AS7-AO7</f>
         <v>298</v>
       </c>
-      <c r="AL7" s="15">
-        <f t="shared" ref="AL7" si="7">AS7-AO7</f>
+      <c r="AM7" s="15">
+        <f t="shared" ref="AM7" si="5">AT7-AP7</f>
         <v>97</v>
       </c>
-      <c r="AM7" s="15">
+      <c r="AN7" s="15">
         <v>395</v>
       </c>
-      <c r="AN7" s="15">
-        <f t="shared" ref="AN7:AN14" si="8">D7-J7</f>
+      <c r="AO7" s="15">
+        <f>D7-J7</f>
         <v>-449</v>
       </c>
-      <c r="AO7" s="15">
-        <f t="shared" ref="AO7:AO14" si="9">E7-K7</f>
+      <c r="AP7" s="15">
+        <f>E7-K7</f>
         <v>-58</v>
       </c>
-      <c r="AP7" s="15">
+      <c r="AQ7" s="15">
         <v>-507</v>
       </c>
-      <c r="AQ7" s="16">
-        <f t="shared" ref="AQ7:AQ14" si="10">AP7/F7</f>
+      <c r="AR7" s="16">
+        <f>AQ7/F7</f>
         <v>0.50801603206412826</v>
       </c>
-      <c r="AR7" s="15">
+      <c r="AS7" s="15">
         <v>-151</v>
       </c>
-      <c r="AS7" s="15">
+      <c r="AT7" s="15">
         <v>39</v>
       </c>
-      <c r="AT7" s="15">
-        <f>AS7+AR7</f>
+      <c r="AU7" s="15">
+        <f>AT7+AS7</f>
         <v>-112</v>
       </c>
-      <c r="AU7" s="17">
-        <f>AR7*0.12591</f>
+      <c r="AV7" s="17">
+        <f>AS7*0.12591</f>
         <v>-19.012409999999999</v>
       </c>
-      <c r="AV7" s="17">
-        <f>AS7*0.14969</f>
+      <c r="AW7" s="17">
+        <f>AT7*0.14969</f>
         <v>5.8379099999999999</v>
       </c>
-      <c r="AW7" s="17">
-        <f t="shared" ref="AW7:AW8" si="11">AV7+AU7</f>
+      <c r="AX7" s="17">
+        <f t="shared" ref="AX7:AX8" si="6">AW7+AV7</f>
         <v>-13.174499999999998</v>
       </c>
-      <c r="AX7" s="17">
-        <f>AR7*0.01</f>
+      <c r="AY7" s="17">
+        <f>AS7*0.01</f>
         <v>-1.51</v>
       </c>
-      <c r="AY7" s="17">
-        <v>0</v>
-      </c>
-      <c r="AZ7" s="20">
-        <f t="shared" ref="AZ7:AZ8" si="12">AY7+AX7+AW7</f>
+      <c r="AZ7" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="20">
+        <f>AZ7+AY7+AX7</f>
         <v>-14.684499999999998</v>
       </c>
-      <c r="BA7" s="21">
+      <c r="BB7" s="21">
         <v>14.68</v>
       </c>
-      <c r="BB7" s="21">
-        <v>0</v>
-      </c>
-      <c r="BC7" s="20">
+      <c r="BC7" s="21">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="20">
         <v>7.83</v>
       </c>
-      <c r="BD7" s="17"/>
-      <c r="BE7" s="22">
-        <f>BC7+BB7+BD7</f>
+      <c r="BE7" s="17">
+        <v>0</v>
+      </c>
+      <c r="BF7" s="22">
+        <f>BD7+BC7+BE7</f>
         <v>7.83</v>
       </c>
     </row>
-    <row r="8" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="13">
         <v>45449</v>
@@ -1851,7 +1874,7 @@
         <v>45456</v>
       </c>
       <c r="D8" s="15">
-        <f t="shared" ref="D8" si="13">ROUND(J8/M8,0)</f>
+        <f t="shared" ref="D8" si="7">ROUND(J8/M8,0)</f>
         <v>-1411</v>
       </c>
       <c r="E8" s="15">
@@ -1862,11 +1885,11 @@
         <v>-1601</v>
       </c>
       <c r="G8" s="15">
-        <f t="shared" ref="G8:H8" si="14">G9+G10</f>
+        <f t="shared" ref="G8:H8" si="8">G9+G10</f>
         <v>330</v>
       </c>
       <c r="H8" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>121</v>
       </c>
       <c r="I8" s="15">
@@ -1888,27 +1911,27 @@
         <v>0.49906308557151779</v>
       </c>
       <c r="N8" s="15">
-        <f t="shared" ref="N8:R8" si="15">N9+N10</f>
+        <f t="shared" ref="N8:R8" si="9">N9+N10</f>
         <v>-374</v>
       </c>
       <c r="O8" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>26</v>
       </c>
       <c r="P8" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>-348</v>
       </c>
       <c r="Q8" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>-47.806659999999994</v>
       </c>
       <c r="R8" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>3.8457699999999995</v>
       </c>
       <c r="S8" s="17">
-        <f t="shared" si="1"/>
+        <f>R8+Q8</f>
         <v>-43.960889999999992</v>
       </c>
       <c r="T8" s="17">
@@ -1916,135 +1939,142 @@
         <v>-3.75</v>
       </c>
       <c r="U8" s="18">
+        <f t="shared" si="1"/>
+        <v>0.12913107499999998</v>
+      </c>
+      <c r="V8" s="19">
         <f t="shared" si="2"/>
-        <v>0.12913107499999998</v>
-      </c>
-      <c r="V8" s="19">
+        <v>0.14791423076923074</v>
+      </c>
+      <c r="W8" s="19">
         <f t="shared" si="3"/>
-        <v>0.14791423076923074</v>
-      </c>
-      <c r="W8" s="19">
+        <v>0.12782529411764704</v>
+      </c>
+      <c r="X8" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="20">
+        <f>Q8+R8+T8+X8</f>
+        <v>-47.710889999999992</v>
+      </c>
+      <c r="Z8" s="21">
+        <v>72.08</v>
+      </c>
+      <c r="AA8" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="17">
+        <v>-98.9</v>
+      </c>
+      <c r="AC8" s="17">
+        <v>33.86</v>
+      </c>
+      <c r="AD8" s="17">
+        <v>-1.43</v>
+      </c>
+      <c r="AE8" s="20">
         <f t="shared" si="4"/>
-        <v>0.12782529411764704</v>
-      </c>
-      <c r="X8" s="20">
-        <f t="shared" si="5"/>
-        <v>-47.710889999999992</v>
-      </c>
-      <c r="Y8" s="21">
-        <v>72.08</v>
-      </c>
-      <c r="Z8" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="17">
-        <v>-98.9</v>
-      </c>
-      <c r="AB8" s="17">
-        <v>33.86</v>
-      </c>
-      <c r="AC8" s="17">
-        <v>-1.43</v>
-      </c>
-      <c r="AD8" s="20">
-        <f t="shared" si="6"/>
         <v>-66.47</v>
       </c>
-      <c r="AE8" s="17">
+      <c r="AF8" s="17">
         <v>10</v>
       </c>
-      <c r="AF8" s="17">
+      <c r="AG8" s="17">
         <v>11.75</v>
       </c>
-      <c r="AG8" s="17">
-        <v>0</v>
-      </c>
       <c r="AH8" s="17">
-        <f t="shared" ref="AH8" si="16">AE8+AF8+AG8</f>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="17">
+        <f t="shared" ref="AI8" si="10">AF8+AG8+AH8</f>
         <v>21.75</v>
       </c>
-      <c r="AI8" s="15"/>
-      <c r="AJ8" s="22">
-        <f>Z8+AH8+AI8</f>
+      <c r="AJ8" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="22">
+        <f>AA8+AI8+AJ8</f>
         <v>21.75</v>
       </c>
-      <c r="AK8" s="15">
-        <f t="shared" ref="AK8:AL8" si="17">AR8-AN8</f>
+      <c r="AL8" s="15">
+        <f t="shared" ref="AL8:AM8" si="11">AS8-AO8</f>
         <v>349</v>
       </c>
-      <c r="AL8" s="15">
-        <f t="shared" si="17"/>
+      <c r="AM8" s="15">
+        <f t="shared" si="11"/>
         <v>102</v>
       </c>
-      <c r="AM8" s="15">
+      <c r="AN8" s="15">
         <v>451</v>
       </c>
-      <c r="AN8" s="15">
-        <f t="shared" si="8"/>
+      <c r="AO8" s="15">
+        <f>D8-J8</f>
         <v>-707</v>
       </c>
-      <c r="AO8" s="15">
+      <c r="AP8" s="15">
         <f>E8-K8</f>
         <v>-95</v>
       </c>
-      <c r="AP8" s="15">
+      <c r="AQ8" s="15">
         <v>-802</v>
       </c>
-      <c r="AQ8" s="16">
-        <f t="shared" si="10"/>
+      <c r="AR8" s="16">
+        <f>AQ8/F8</f>
         <v>0.50093691442848221</v>
       </c>
-      <c r="AR8" s="15">
-        <f>AR9+AR10</f>
+      <c r="AS8" s="15">
+        <f>AS9+AS10</f>
         <v>-358</v>
       </c>
-      <c r="AS8" s="15">
-        <f t="shared" ref="AS8:AV8" si="18">AS9+AS10</f>
+      <c r="AT8" s="15">
+        <f t="shared" ref="AT8:AW8" si="12">AT9+AT10</f>
         <v>7</v>
       </c>
-      <c r="AT8" s="15">
-        <f t="shared" si="18"/>
+      <c r="AU8" s="15">
+        <f t="shared" si="12"/>
         <v>-351</v>
       </c>
-      <c r="AU8" s="17">
-        <f t="shared" si="18"/>
+      <c r="AV8" s="17">
+        <f t="shared" si="12"/>
         <v>-45.9373</v>
       </c>
-      <c r="AV8" s="17">
-        <f t="shared" si="18"/>
+      <c r="AW8" s="17">
+        <f t="shared" si="12"/>
         <v>0.77081</v>
       </c>
-      <c r="AW8" s="17">
-        <f t="shared" si="11"/>
+      <c r="AX8" s="17">
+        <f t="shared" si="6"/>
         <v>-45.166490000000003</v>
       </c>
-      <c r="AX8" s="17">
-        <f>(AR10+AR9+AS10)*0.01</f>
+      <c r="AY8" s="17">
+        <f>(AS10+AS9+AT10)*0.01</f>
         <v>-3.64</v>
       </c>
-      <c r="AY8" s="17">
-        <v>0</v>
-      </c>
-      <c r="AZ8" s="20">
-        <f t="shared" si="12"/>
+      <c r="AZ8" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="20">
+        <f t="shared" ref="BA7:BA8" si="13">AZ8+AY8+AX8</f>
         <v>-48.806490000000004</v>
       </c>
-      <c r="BA8" s="21">
+      <c r="BB8" s="21">
         <v>63.49</v>
       </c>
-      <c r="BB8" s="21">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="20">
+      <c r="BC8" s="21">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="20">
         <v>11.75</v>
       </c>
-      <c r="BD8" s="17"/>
-      <c r="BE8" s="22">
-        <f t="shared" ref="BE8" si="19">BC8+BB8+BD8</f>
+      <c r="BE8" s="17">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="22">
+        <f t="shared" ref="BF8" si="14">BD8+BC8+BE8</f>
         <v>11.75</v>
       </c>
     </row>
-    <row r="9" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -2081,7 +2111,7 @@
         <v>27</v>
       </c>
       <c r="P9" s="25">
-        <f t="shared" ref="P9:P11" si="20">O9+N9</f>
+        <f t="shared" ref="P9:P11" si="15">O9+N9</f>
         <v>-273</v>
       </c>
       <c r="Q9" s="27">
@@ -2108,46 +2138,46 @@
       <c r="AF9" s="27"/>
       <c r="AG9" s="27"/>
       <c r="AH9" s="27"/>
-      <c r="AI9" s="56"/>
+      <c r="AI9" s="27"/>
       <c r="AJ9" s="56"/>
-      <c r="AK9" s="57">
-        <f>AR9-AN9</f>
-        <v>306</v>
-      </c>
+      <c r="AK9" s="56"/>
       <c r="AL9" s="57">
         <f>AS9-AO9</f>
+        <v>306</v>
+      </c>
+      <c r="AM9" s="57">
+        <f>AT9-AP9</f>
         <v>90</v>
       </c>
-      <c r="AM9" s="58"/>
-      <c r="AN9" s="58">
+      <c r="AN9" s="58"/>
+      <c r="AO9" s="58">
         <f>D9-J9</f>
         <v>-575</v>
       </c>
-      <c r="AO9" s="58">
+      <c r="AP9" s="58">
         <f>E9-K9</f>
         <v>-77</v>
       </c>
-      <c r="AP9" s="25"/>
       <c r="AQ9" s="25"/>
-      <c r="AR9" s="25">
+      <c r="AR9" s="25"/>
+      <c r="AS9" s="25">
         <v>-269</v>
       </c>
-      <c r="AS9" s="25">
+      <c r="AT9" s="25">
         <v>13</v>
       </c>
-      <c r="AT9" s="25">
-        <f t="shared" ref="AT9:AT11" si="21">AS9+AR9</f>
+      <c r="AU9" s="25">
+        <f t="shared" ref="AU9:AU11" si="16">AT9+AS9</f>
         <v>-256</v>
       </c>
-      <c r="AU9" s="27">
-        <f>AR9*0.12591</f>
+      <c r="AV9" s="27">
+        <f>AS9*0.12591</f>
         <v>-33.869790000000002</v>
       </c>
-      <c r="AV9" s="27">
-        <f>AS9*0.14969</f>
+      <c r="AW9" s="27">
+        <f>AT9*0.14969</f>
         <v>1.94597</v>
       </c>
-      <c r="AW9" s="27"/>
       <c r="AX9" s="27"/>
       <c r="AY9" s="27"/>
       <c r="AZ9" s="27"/>
@@ -2156,8 +2186,9 @@
       <c r="BC9" s="27"/>
       <c r="BD9" s="27"/>
       <c r="BE9" s="27"/>
+      <c r="BF9" s="27"/>
     </row>
-    <row r="10" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -2194,15 +2225,15 @@
         <v>-1</v>
       </c>
       <c r="P10" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>-75</v>
       </c>
       <c r="Q10" s="27">
-        <f t="shared" ref="Q10:Q11" si="22">N10*0.13559</f>
+        <f t="shared" ref="Q10:Q11" si="17">N10*0.13559</f>
         <v>-10.033659999999999</v>
       </c>
       <c r="R10" s="27">
-        <f t="shared" ref="R10:R11" si="23">O10*0.19586</f>
+        <f t="shared" ref="R10:R11" si="18">O10*0.19586</f>
         <v>-0.19586000000000001</v>
       </c>
       <c r="S10" s="27"/>
@@ -2221,46 +2252,46 @@
       <c r="AF10" s="27"/>
       <c r="AG10" s="27"/>
       <c r="AH10" s="27"/>
-      <c r="AI10" s="56"/>
+      <c r="AI10" s="27"/>
       <c r="AJ10" s="56"/>
-      <c r="AK10" s="57">
-        <f>AR10-AN10</f>
-        <v>42</v>
-      </c>
+      <c r="AK10" s="56"/>
       <c r="AL10" s="57">
         <f>AS10-AO10</f>
+        <v>42</v>
+      </c>
+      <c r="AM10" s="57">
+        <f>AT10-AP10</f>
         <v>12</v>
       </c>
-      <c r="AM10" s="58"/>
-      <c r="AN10" s="58">
+      <c r="AN10" s="58"/>
+      <c r="AO10" s="58">
         <f>D10-J10</f>
         <v>-131</v>
       </c>
-      <c r="AO10" s="58">
+      <c r="AP10" s="58">
         <f>E10-K10</f>
         <v>-18</v>
       </c>
-      <c r="AP10" s="25"/>
       <c r="AQ10" s="25"/>
-      <c r="AR10" s="25">
+      <c r="AR10" s="25"/>
+      <c r="AS10" s="25">
         <v>-89</v>
       </c>
-      <c r="AS10" s="25">
+      <c r="AT10" s="25">
         <v>-6</v>
       </c>
-      <c r="AT10" s="25">
-        <f t="shared" si="21"/>
+      <c r="AU10" s="25">
+        <f t="shared" si="16"/>
         <v>-95</v>
       </c>
-      <c r="AU10" s="27">
-        <f t="shared" ref="AU10:AU11" si="24">AR10*0.13559</f>
+      <c r="AV10" s="27">
+        <f t="shared" ref="AV10:AV11" si="19">AS10*0.13559</f>
         <v>-12.067509999999999</v>
       </c>
-      <c r="AV10" s="27">
-        <f t="shared" ref="AV10:AV11" si="25">AS10*0.19586</f>
+      <c r="AW10" s="27">
+        <f t="shared" ref="AW10:AW11" si="20">AT10*0.19586</f>
         <v>-1.17516</v>
       </c>
-      <c r="AW10" s="27"/>
       <c r="AX10" s="27"/>
       <c r="AY10" s="27"/>
       <c r="AZ10" s="27"/>
@@ -2269,8 +2300,9 @@
       <c r="BC10" s="27"/>
       <c r="BD10" s="27"/>
       <c r="BE10" s="27"/>
+      <c r="BF10" s="27"/>
     </row>
-    <row r="11" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="13">
         <v>45481</v>
@@ -2290,11 +2322,11 @@
         <v>-1750</v>
       </c>
       <c r="G11" s="15">
-        <f t="shared" ref="G11:H11" si="26">G12+G13</f>
+        <f t="shared" ref="G11:H11" si="21">G12+G13</f>
         <v>393</v>
       </c>
       <c r="H11" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>250</v>
       </c>
       <c r="I11" s="15">
@@ -2305,7 +2337,7 @@
         <v>-1001</v>
       </c>
       <c r="K11" s="15">
-        <f t="shared" ref="J11:K11" si="27">K12+K13</f>
+        <f t="shared" ref="K11" si="22">K12+K13</f>
         <v>-131</v>
       </c>
       <c r="L11" s="15">
@@ -2322,15 +2354,15 @@
         <v>119</v>
       </c>
       <c r="P11" s="15">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>-489</v>
       </c>
       <c r="Q11" s="17">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>-82.438719999999989</v>
       </c>
       <c r="R11" s="17">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>23.30734</v>
       </c>
       <c r="S11" s="17">
@@ -2354,121 +2386,128 @@
         <v>0.13558999999999999</v>
       </c>
       <c r="X11" s="20">
-        <f>Q11+R11+T11+0</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="20">
+        <f>Q11+R11+T11+X11</f>
         <v>-65.211379999999991</v>
       </c>
-      <c r="Y11" s="21">
+      <c r="Z11" s="21">
         <v>65.209999999999994</v>
       </c>
-      <c r="Z11" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="17">
+      <c r="AA11" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="17">
         <v>-148.91999999999999</v>
       </c>
-      <c r="AB11" s="17">
+      <c r="AC11" s="17">
         <v>23.84</v>
       </c>
-      <c r="AC11" s="17">
+      <c r="AD11" s="17">
         <v>-1.88</v>
       </c>
-      <c r="AD11" s="20">
-        <f>AC11+AB11+AA11</f>
+      <c r="AE11" s="20">
+        <f>AD11+AC11+AB11</f>
         <v>-126.95999999999998</v>
       </c>
-      <c r="AE11" s="17">
+      <c r="AF11" s="17">
         <v>10</v>
       </c>
-      <c r="AF11" s="17">
+      <c r="AG11" s="17">
         <v>12.53</v>
       </c>
-      <c r="AG11" s="17">
-        <v>0</v>
-      </c>
       <c r="AH11" s="17">
-        <f>AE11+AF11+AG11</f>
+        <v>0</v>
+      </c>
+      <c r="AI11" s="17">
+        <f>AF11+AG11+AH11</f>
         <v>22.53</v>
       </c>
-      <c r="AI11" s="15"/>
-      <c r="AJ11" s="22">
-        <f>Z11+AH11+AI11</f>
+      <c r="AJ11" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="22">
+        <f>AA11+AI11+AJ11</f>
         <v>22.53</v>
       </c>
-      <c r="AK11" s="15">
-        <f t="shared" ref="AK11:AL11" si="28">AR11-AN11</f>
+      <c r="AL11" s="15">
+        <f t="shared" ref="AL11:AM11" si="23">AS11-AO11</f>
         <v>276</v>
       </c>
-      <c r="AL11" s="15">
-        <f t="shared" si="28"/>
+      <c r="AM11" s="15">
+        <f t="shared" si="23"/>
         <v>53</v>
       </c>
-      <c r="AM11" s="15">
+      <c r="AN11" s="15">
         <v>329</v>
       </c>
-      <c r="AN11" s="15">
-        <f t="shared" si="8"/>
+      <c r="AO11" s="15">
+        <f>D11-J11</f>
         <v>-546</v>
       </c>
-      <c r="AO11" s="15">
-        <f t="shared" si="9"/>
+      <c r="AP11" s="15">
+        <f>E11-K11</f>
         <v>-72</v>
       </c>
-      <c r="AP11" s="15">
+      <c r="AQ11" s="15">
         <v>-618</v>
       </c>
-      <c r="AQ11" s="16">
-        <f t="shared" si="10"/>
+      <c r="AR11" s="16">
+        <f>AQ11/F11</f>
         <v>0.35314285714285715</v>
       </c>
-      <c r="AR11" s="15">
+      <c r="AS11" s="15">
         <v>-270</v>
       </c>
-      <c r="AS11" s="15">
+      <c r="AT11" s="15">
         <v>-19</v>
       </c>
-      <c r="AT11" s="15">
-        <f t="shared" si="21"/>
+      <c r="AU11" s="15">
+        <f t="shared" si="16"/>
         <v>-289</v>
       </c>
-      <c r="AU11" s="17">
-        <f t="shared" si="24"/>
+      <c r="AV11" s="17">
+        <f t="shared" si="19"/>
         <v>-36.609299999999998</v>
       </c>
-      <c r="AV11" s="17">
-        <f t="shared" si="25"/>
+      <c r="AW11" s="17">
+        <f t="shared" si="20"/>
         <v>-3.7213400000000001</v>
       </c>
-      <c r="AW11" s="17">
-        <f>AV11+AU11</f>
+      <c r="AX11" s="17">
+        <f>AW11+AV11</f>
         <v>-40.330639999999995</v>
       </c>
-      <c r="AX11" s="17">
-        <f>AT11*0.01</f>
+      <c r="AY11" s="17">
+        <f>AU11*0.01</f>
         <v>-2.89</v>
       </c>
-      <c r="AY11" s="17">
-        <v>0</v>
-      </c>
-      <c r="AZ11" s="20">
-        <f>AY11+AX11+AW11</f>
+      <c r="AZ11" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA11" s="20">
+        <f>AZ11+AY11+AX11</f>
         <v>-43.220639999999996</v>
       </c>
-      <c r="BA11" s="21">
+      <c r="BB11" s="21">
         <v>106.71</v>
       </c>
-      <c r="BB11" s="21">
-        <v>0</v>
-      </c>
-      <c r="BC11" s="20">
+      <c r="BC11" s="21">
+        <v>0</v>
+      </c>
+      <c r="BD11" s="20">
         <v>12.53</v>
       </c>
-      <c r="BD11" s="17"/>
-      <c r="BE11" s="22">
-        <f>BC11+BB11+BD11</f>
+      <c r="BE11" s="17">
+        <v>0</v>
+      </c>
+      <c r="BF11" s="22">
+        <f>BD11+BC11+BE11</f>
         <v>12.53</v>
       </c>
     </row>
-    <row r="12" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="28"/>
       <c r="C12" s="29" t="s">
@@ -2520,18 +2559,18 @@
       <c r="AG12" s="32"/>
       <c r="AH12" s="32"/>
       <c r="AI12" s="32"/>
-      <c r="AJ12" s="59"/>
-      <c r="AK12" s="60"/>
+      <c r="AJ12" s="32"/>
+      <c r="AK12" s="59"/>
       <c r="AL12" s="60"/>
-      <c r="AM12" s="61"/>
-      <c r="AN12" s="60"/>
+      <c r="AM12" s="60"/>
+      <c r="AN12" s="61"/>
       <c r="AO12" s="60"/>
-      <c r="AP12" s="61"/>
+      <c r="AP12" s="60"/>
       <c r="AQ12" s="61"/>
-      <c r="AR12" s="29"/>
+      <c r="AR12" s="61"/>
       <c r="AS12" s="29"/>
       <c r="AT12" s="29"/>
-      <c r="AU12" s="32"/>
+      <c r="AU12" s="29"/>
       <c r="AV12" s="32"/>
       <c r="AW12" s="32"/>
       <c r="AX12" s="32"/>
@@ -2542,8 +2581,9 @@
       <c r="BC12" s="32"/>
       <c r="BD12" s="32"/>
       <c r="BE12" s="32"/>
+      <c r="BF12" s="32"/>
     </row>
-    <row r="13" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="28"/>
       <c r="C13" s="29" t="s">
@@ -2595,18 +2635,18 @@
       <c r="AG13" s="32"/>
       <c r="AH13" s="32"/>
       <c r="AI13" s="32"/>
-      <c r="AJ13" s="59"/>
-      <c r="AK13" s="60"/>
+      <c r="AJ13" s="32"/>
+      <c r="AK13" s="59"/>
       <c r="AL13" s="60"/>
-      <c r="AM13" s="61"/>
-      <c r="AN13" s="60"/>
+      <c r="AM13" s="60"/>
+      <c r="AN13" s="61"/>
       <c r="AO13" s="60"/>
-      <c r="AP13" s="61"/>
+      <c r="AP13" s="60"/>
       <c r="AQ13" s="61"/>
-      <c r="AR13" s="29"/>
+      <c r="AR13" s="61"/>
       <c r="AS13" s="29"/>
       <c r="AT13" s="29"/>
-      <c r="AU13" s="32"/>
+      <c r="AU13" s="29"/>
       <c r="AV13" s="32"/>
       <c r="AW13" s="32"/>
       <c r="AX13" s="32"/>
@@ -2617,8 +2657,9 @@
       <c r="BC13" s="32"/>
       <c r="BD13" s="32"/>
       <c r="BE13" s="32"/>
+      <c r="BF13" s="32"/>
     </row>
-    <row r="14" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="13">
         <v>45510</v>
@@ -2660,23 +2701,23 @@
         <v>0.40445402298850575</v>
       </c>
       <c r="N14" s="33">
-        <f t="shared" ref="N14:P14" si="29">N15+N16</f>
+        <f t="shared" ref="N14:P14" si="24">N15+N16</f>
         <v>-267</v>
       </c>
       <c r="O14" s="33">
-        <f t="shared" si="29"/>
+        <f t="shared" si="24"/>
         <v>86</v>
       </c>
       <c r="P14" s="34">
-        <f t="shared" si="29"/>
+        <f t="shared" si="24"/>
         <v>-181</v>
       </c>
       <c r="Q14" s="17">
-        <f t="shared" ref="Q14:R14" si="30">SUM(Q15:Q16)</f>
+        <f t="shared" ref="Q14:R14" si="25">SUM(Q15:Q16)</f>
         <v>-35.405396597999996</v>
       </c>
       <c r="R14" s="17">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>16.917801365000003</v>
       </c>
       <c r="S14" s="17">
@@ -2700,123 +2741,130 @@
         <v>0.13260448164044941</v>
       </c>
       <c r="X14" s="20">
-        <f>Q14+R14+T14+0</f>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="20">
+        <f>Q14+R14+T14+X14</f>
         <v>-21.157595232999995</v>
       </c>
-      <c r="Y14" s="21">
+      <c r="Z14" s="21">
         <v>158.44</v>
       </c>
-      <c r="Z14" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="17">
+      <c r="AA14" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="17">
         <v>-46.8</v>
       </c>
-      <c r="AB14" s="17">
+      <c r="AC14" s="17">
         <v>17.72</v>
       </c>
-      <c r="AC14" s="17">
+      <c r="AD14" s="17">
         <v>0.24</v>
       </c>
-      <c r="AD14" s="20">
-        <f>AC14+AB14+AA14</f>
+      <c r="AE14" s="20">
+        <f>AD14+AC14+AB14</f>
         <v>-28.84</v>
       </c>
-      <c r="AE14" s="17">
+      <c r="AF14" s="17">
         <v>10</v>
       </c>
-      <c r="AF14" s="17">
+      <c r="AG14" s="17">
         <v>11.36</v>
       </c>
-      <c r="AG14" s="17">
-        <v>0</v>
-      </c>
       <c r="AH14" s="17">
-        <f>AE14+AF14+AG14</f>
+        <v>0</v>
+      </c>
+      <c r="AI14" s="17">
+        <f>AF14+AG14+AH14</f>
         <v>21.36</v>
       </c>
-      <c r="AI14" s="15"/>
-      <c r="AJ14" s="22">
-        <f>Z14+AH14+AI14</f>
+      <c r="AJ14" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="22">
+        <f>AA14+AI14+AJ14</f>
         <v>21.36</v>
       </c>
-      <c r="AK14" s="15">
-        <f t="shared" ref="AK14:AL14" si="31">AR14-AN14</f>
+      <c r="AL14" s="15">
+        <f t="shared" ref="AL14:AM14" si="26">AS14-AO14</f>
         <v>409</v>
       </c>
-      <c r="AL14" s="15">
-        <f t="shared" si="31"/>
+      <c r="AM14" s="15">
+        <f t="shared" si="26"/>
         <v>132</v>
       </c>
-      <c r="AM14" s="15">
+      <c r="AN14" s="15">
         <v>541</v>
       </c>
-      <c r="AN14" s="15">
-        <f t="shared" si="8"/>
+      <c r="AO14" s="15">
+        <f>D14-J14</f>
         <v>-723</v>
       </c>
-      <c r="AO14" s="15">
-        <f t="shared" si="9"/>
+      <c r="AP14" s="15">
+        <f>E14-K14</f>
         <v>-106</v>
       </c>
-      <c r="AP14" s="15">
+      <c r="AQ14" s="15">
         <v>-829</v>
       </c>
-      <c r="AQ14" s="16">
-        <f t="shared" si="10"/>
+      <c r="AR14" s="16">
+        <f>AQ14/F14</f>
         <v>0.59554597701149425</v>
       </c>
-      <c r="AR14" s="15">
-        <f t="shared" ref="AR14:AT14" si="32">AR15+AR16</f>
+      <c r="AS14" s="15">
+        <f t="shared" ref="AS14:AU14" si="27">AS15+AS16</f>
         <v>-314</v>
       </c>
-      <c r="AS14" s="15">
-        <f t="shared" si="32"/>
+      <c r="AT14" s="15">
+        <f t="shared" si="27"/>
         <v>26</v>
       </c>
-      <c r="AT14" s="15">
-        <f t="shared" si="32"/>
+      <c r="AU14" s="15">
+        <f t="shared" si="27"/>
         <v>-288</v>
       </c>
-      <c r="AU14" s="17">
-        <f t="shared" ref="AU14:AV14" si="33">SUM(AU15:AU16)</f>
+      <c r="AV14" s="17">
+        <f t="shared" ref="AV14:AW14" si="28">SUM(AV15:AV16)</f>
         <v>-41.637807834999997</v>
       </c>
-      <c r="AV14" s="17">
-        <f t="shared" si="33"/>
+      <c r="AW14" s="17">
+        <f t="shared" si="28"/>
         <v>5.1146840949999994</v>
       </c>
-      <c r="AW14" s="17">
-        <f>AV14+AU14</f>
+      <c r="AX14" s="17">
+        <f>AW14+AV14</f>
         <v>-36.523123739999996</v>
       </c>
-      <c r="AX14" s="17">
-        <f>(AR16+AR15)*0.01</f>
+      <c r="AY14" s="17">
+        <f>(AS16+AS15)*0.01</f>
         <v>-3.14</v>
       </c>
-      <c r="AY14" s="17">
-        <v>0</v>
-      </c>
-      <c r="AZ14" s="20">
-        <f>AY14+AX14+AW14</f>
+      <c r="AZ14" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA14" s="20">
+        <f>AZ14+AY14+AX14</f>
         <v>-39.663123739999996</v>
       </c>
-      <c r="BA14" s="21">
+      <c r="BB14" s="21">
         <v>146.37</v>
       </c>
-      <c r="BB14" s="21">
-        <v>0</v>
-      </c>
-      <c r="BC14" s="20">
+      <c r="BC14" s="21">
+        <v>0</v>
+      </c>
+      <c r="BD14" s="20">
         <v>11.36</v>
       </c>
-      <c r="BD14" s="17"/>
-      <c r="BE14" s="22">
-        <f>BC14+BB14+BD14</f>
+      <c r="BE14" s="17">
+        <v>0</v>
+      </c>
+      <c r="BF14" s="22">
+        <f>BD14+BC14+BE14</f>
         <v>11.36</v>
       </c>
     </row>
-    <row r="15" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36" t="s">
@@ -2867,33 +2915,33 @@
       <c r="AG15" s="39"/>
       <c r="AH15" s="39"/>
       <c r="AI15" s="39"/>
-      <c r="AJ15" s="62"/>
-      <c r="AK15" s="63"/>
+      <c r="AJ15" s="39"/>
+      <c r="AK15" s="62"/>
       <c r="AL15" s="63"/>
-      <c r="AM15" s="62"/>
-      <c r="AN15" s="63"/>
-      <c r="AO15" s="62"/>
-      <c r="AP15" s="66"/>
-      <c r="AQ15" s="38"/>
-      <c r="AR15" s="36">
+      <c r="AM15" s="63"/>
+      <c r="AN15" s="62"/>
+      <c r="AO15" s="63"/>
+      <c r="AP15" s="62"/>
+      <c r="AQ15" s="66"/>
+      <c r="AR15" s="38"/>
+      <c r="AS15" s="36">
         <v>-64.965500000000006</v>
       </c>
-      <c r="AS15" s="36">
+      <c r="AT15" s="36">
         <v>20.620699999999999</v>
       </c>
-      <c r="AT15" s="36">
-        <f t="shared" ref="AT15:AT17" si="34">AS15+AR15</f>
+      <c r="AU15" s="36">
+        <f t="shared" ref="AU15:AU17" si="29">AT15+AS15</f>
         <v>-44.344800000000006</v>
       </c>
-      <c r="AU15" s="39">
-        <f>AR15*0.12116</f>
+      <c r="AV15" s="39">
+        <f>AS15*0.12116</f>
         <v>-7.8712199800000011</v>
       </c>
-      <c r="AV15" s="39">
-        <f>AS15*0.19586</f>
+      <c r="AW15" s="39">
+        <f>AT15*0.19586</f>
         <v>4.0387703019999996</v>
       </c>
-      <c r="AW15" s="39"/>
       <c r="AX15" s="39"/>
       <c r="AY15" s="39"/>
       <c r="AZ15" s="39"/>
@@ -2902,8 +2950,9 @@
       <c r="BC15" s="39"/>
       <c r="BD15" s="39"/>
       <c r="BE15" s="39"/>
+      <c r="BF15" s="39"/>
     </row>
-    <row r="16" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36" t="s">
@@ -2934,7 +2983,7 @@
         <v>-28.712348573999996</v>
       </c>
       <c r="R16" s="39">
-        <f t="shared" ref="R16:R17" si="35">O16*0.20001</f>
+        <f t="shared" ref="R16:R17" si="30">O16*0.20001</f>
         <v>3.5587979309999995</v>
       </c>
       <c r="S16" s="39"/>
@@ -2954,33 +3003,33 @@
       <c r="AG16" s="39"/>
       <c r="AH16" s="39"/>
       <c r="AI16" s="39"/>
-      <c r="AJ16" s="62"/>
-      <c r="AK16" s="63"/>
+      <c r="AJ16" s="39"/>
+      <c r="AK16" s="62"/>
       <c r="AL16" s="63"/>
-      <c r="AM16" s="62"/>
-      <c r="AN16" s="63"/>
-      <c r="AO16" s="62"/>
-      <c r="AP16" s="66"/>
-      <c r="AQ16" s="38"/>
-      <c r="AR16" s="36">
+      <c r="AM16" s="63"/>
+      <c r="AN16" s="62"/>
+      <c r="AO16" s="63"/>
+      <c r="AP16" s="62"/>
+      <c r="AQ16" s="66"/>
+      <c r="AR16" s="38"/>
+      <c r="AS16" s="36">
         <v>-249.03450000000001</v>
       </c>
-      <c r="AS16" s="36">
+      <c r="AT16" s="36">
         <v>5.3792999999999997</v>
       </c>
-      <c r="AT16" s="36">
-        <f t="shared" si="34"/>
+      <c r="AU16" s="36">
+        <f t="shared" si="29"/>
         <v>-243.65520000000001</v>
       </c>
-      <c r="AU16" s="39">
-        <f>AR16*0.13559</f>
+      <c r="AV16" s="39">
+        <f>AS16*0.13559</f>
         <v>-33.766587854999997</v>
       </c>
-      <c r="AV16" s="39">
-        <f t="shared" ref="AV16:AV17" si="36">AS16*0.20001</f>
+      <c r="AW16" s="39">
+        <f t="shared" ref="AW16:AW17" si="31">AT16*0.20001</f>
         <v>1.075913793</v>
       </c>
-      <c r="AW16" s="39"/>
       <c r="AX16" s="39"/>
       <c r="AY16" s="39"/>
       <c r="AZ16" s="39"/>
@@ -2989,8 +3038,9 @@
       <c r="BC16" s="39"/>
       <c r="BD16" s="39"/>
       <c r="BE16" s="39"/>
+      <c r="BF16" s="39"/>
     </row>
-    <row r="17" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="13">
         <v>45540</v>
@@ -3010,11 +3060,11 @@
         <v>-1516</v>
       </c>
       <c r="G17" s="15">
-        <f t="shared" ref="G17:H17" si="37">G18+G19</f>
+        <f t="shared" ref="G17:H17" si="32">G18+G19</f>
         <v>175</v>
       </c>
       <c r="H17" s="15">
-        <f t="shared" si="37"/>
+        <f t="shared" si="32"/>
         <v>145</v>
       </c>
       <c r="I17" s="15">
@@ -3025,7 +3075,7 @@
         <v>-386</v>
       </c>
       <c r="K17" s="15">
-        <f t="shared" ref="K17" si="38">K18+K19</f>
+        <f t="shared" ref="K17" si="33">K18+K19</f>
         <v>-50</v>
       </c>
       <c r="L17" s="15">
@@ -3050,7 +3100,7 @@
         <v>-25.56476</v>
       </c>
       <c r="R17" s="17">
-        <f t="shared" si="35"/>
+        <f t="shared" si="30"/>
         <v>19.00095</v>
       </c>
       <c r="S17" s="17">
@@ -3074,121 +3124,128 @@
         <v>0.12116</v>
       </c>
       <c r="X17" s="20">
-        <f>Q17+R17+T17+0</f>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="20">
+        <f>Q17+R17+T17+X17</f>
         <v>-8.6738099999999996</v>
       </c>
-      <c r="Y17" s="21">
+      <c r="Z17" s="21">
         <v>167.11</v>
       </c>
-      <c r="Z17" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="17">
+      <c r="AA17" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="17">
         <v>-27.53</v>
       </c>
-      <c r="AB17" s="17">
+      <c r="AC17" s="17">
         <v>11.37</v>
       </c>
-      <c r="AC17" s="17">
+      <c r="AD17" s="17">
         <v>0.64</v>
       </c>
-      <c r="AD17" s="20">
-        <f>AC17+AB17+AA17</f>
+      <c r="AE17" s="20">
+        <f>AD17+AC17+AB17</f>
         <v>-15.520000000000001</v>
       </c>
-      <c r="AE17" s="17">
+      <c r="AF17" s="17">
         <v>10</v>
       </c>
-      <c r="AF17" s="17">
+      <c r="AG17" s="17">
         <v>11.75</v>
       </c>
-      <c r="AG17" s="17">
-        <v>0</v>
-      </c>
       <c r="AH17" s="17">
-        <f>AE17+AF17+AG17</f>
+        <v>0</v>
+      </c>
+      <c r="AI17" s="17">
+        <f>AF17+AG17+AH17</f>
         <v>21.75</v>
       </c>
-      <c r="AI17" s="15"/>
-      <c r="AJ17" s="22">
-        <f>Z17+AH17+AI17</f>
+      <c r="AJ17" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="22">
+        <f>AA17+AI17+AJ17</f>
         <v>21.75</v>
       </c>
-      <c r="AK17" s="15">
-        <f t="shared" ref="AK17:AL17" si="39">AR17-AN17</f>
+      <c r="AL17" s="15">
+        <f t="shared" ref="AL17:AM17" si="34">AS17-AO17</f>
         <v>519</v>
       </c>
-      <c r="AL17" s="15">
-        <f t="shared" si="39"/>
+      <c r="AM17" s="15">
+        <f t="shared" si="34"/>
         <v>203</v>
       </c>
-      <c r="AM17" s="15">
+      <c r="AN17" s="15">
         <v>726</v>
       </c>
-      <c r="AN17" s="15">
+      <c r="AO17" s="15">
         <f>D17-J17</f>
         <v>-953</v>
       </c>
-      <c r="AO17" s="15">
+      <c r="AP17" s="15">
         <f>E17-K17</f>
         <v>-123</v>
       </c>
-      <c r="AP17" s="15">
+      <c r="AQ17" s="15">
         <v>-1079</v>
       </c>
-      <c r="AQ17" s="16">
-        <f>AP17/F17</f>
+      <c r="AR17" s="16">
+        <f>AQ17/F17</f>
         <v>0.71174142480211078</v>
       </c>
-      <c r="AR17" s="15">
+      <c r="AS17" s="15">
         <v>-434</v>
       </c>
-      <c r="AS17" s="15">
+      <c r="AT17" s="15">
         <v>80</v>
       </c>
-      <c r="AT17" s="15">
-        <f t="shared" si="34"/>
+      <c r="AU17" s="15">
+        <f t="shared" si="29"/>
         <v>-354</v>
       </c>
-      <c r="AU17" s="17">
-        <f>AR17*0.12116</f>
+      <c r="AV17" s="17">
+        <f>AS17*0.12116</f>
         <v>-52.583440000000003</v>
       </c>
-      <c r="AV17" s="17">
-        <f t="shared" si="36"/>
+      <c r="AW17" s="17">
+        <f t="shared" si="31"/>
         <v>16.000799999999998</v>
       </c>
-      <c r="AW17" s="17">
-        <f>AV17+AU17</f>
+      <c r="AX17" s="17">
+        <f>AW17+AV17</f>
         <v>-36.582640000000005</v>
       </c>
-      <c r="AX17" s="17">
-        <f>AR17*0.01</f>
+      <c r="AY17" s="17">
+        <f>AS17*0.01</f>
         <v>-4.34</v>
       </c>
-      <c r="AY17" s="17">
-        <v>0</v>
-      </c>
-      <c r="AZ17" s="20">
-        <f>AY17+AX17+AW17</f>
+      <c r="AZ17" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA17" s="20">
+        <f>AZ17+AY17+AX17</f>
         <v>-40.922640000000001</v>
       </c>
-      <c r="BA17" s="21">
+      <c r="BB17" s="21">
         <v>187.29</v>
       </c>
-      <c r="BB17" s="21">
-        <v>0</v>
-      </c>
-      <c r="BC17" s="20">
+      <c r="BC17" s="21">
+        <v>0</v>
+      </c>
+      <c r="BD17" s="20">
         <v>11.75</v>
       </c>
-      <c r="BD17" s="17"/>
-      <c r="BE17" s="22">
-        <f>BC17+BB17+BD17</f>
+      <c r="BE17" s="17">
+        <v>0</v>
+      </c>
+      <c r="BF17" s="22">
+        <f>BD17+BC17+BE17</f>
         <v>11.75</v>
       </c>
     </row>
-    <row r="18" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36" t="s">
@@ -3241,17 +3298,17 @@
       <c r="AH18" s="39"/>
       <c r="AI18" s="39"/>
       <c r="AJ18" s="39"/>
-      <c r="AK18" s="36"/>
+      <c r="AK18" s="39"/>
       <c r="AL18" s="36"/>
       <c r="AM18" s="36"/>
       <c r="AN18" s="36"/>
       <c r="AO18" s="36"/>
       <c r="AP18" s="36"/>
-      <c r="AQ18" s="38"/>
-      <c r="AR18" s="36"/>
+      <c r="AQ18" s="36"/>
+      <c r="AR18" s="38"/>
       <c r="AS18" s="36"/>
       <c r="AT18" s="36"/>
-      <c r="AU18" s="39"/>
+      <c r="AU18" s="36"/>
       <c r="AV18" s="39"/>
       <c r="AW18" s="39"/>
       <c r="AX18" s="39"/>
@@ -3262,8 +3319,9 @@
       <c r="BC18" s="39"/>
       <c r="BD18" s="39"/>
       <c r="BE18" s="39"/>
+      <c r="BF18" s="39"/>
     </row>
-    <row r="19" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36" t="s">
@@ -3316,17 +3374,17 @@
       <c r="AH19" s="39"/>
       <c r="AI19" s="39"/>
       <c r="AJ19" s="39"/>
-      <c r="AK19" s="36"/>
+      <c r="AK19" s="39"/>
       <c r="AL19" s="36"/>
       <c r="AM19" s="36"/>
       <c r="AN19" s="36"/>
       <c r="AO19" s="36"/>
       <c r="AP19" s="36"/>
-      <c r="AQ19" s="38"/>
-      <c r="AR19" s="36"/>
+      <c r="AQ19" s="36"/>
+      <c r="AR19" s="38"/>
       <c r="AS19" s="36"/>
       <c r="AT19" s="36"/>
-      <c r="AU19" s="39"/>
+      <c r="AU19" s="36"/>
       <c r="AV19" s="39"/>
       <c r="AW19" s="39"/>
       <c r="AX19" s="39"/>
@@ -3337,8 +3395,9 @@
       <c r="BC19" s="39"/>
       <c r="BD19" s="39"/>
       <c r="BE19" s="39"/>
+      <c r="BF19" s="39"/>
     </row>
-    <row r="20" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23" t="s">
@@ -3361,7 +3420,7 @@
         <v>69</v>
       </c>
       <c r="P20" s="69">
-        <f t="shared" ref="P20:P22" si="40">O20+N20</f>
+        <f t="shared" ref="P20:P22" si="35">O20+N20</f>
         <v>-76</v>
       </c>
       <c r="Q20" s="27">
@@ -3389,43 +3448,44 @@
       <c r="AG20" s="27"/>
       <c r="AH20" s="27"/>
       <c r="AI20" s="27"/>
-      <c r="AJ20" s="56"/>
-      <c r="AK20" s="57"/>
+      <c r="AJ20" s="27"/>
+      <c r="AK20" s="56"/>
       <c r="AL20" s="57"/>
-      <c r="AM20" s="58"/>
-      <c r="AN20" s="57"/>
-      <c r="AO20" s="58"/>
-      <c r="AP20" s="66"/>
-      <c r="AQ20" s="26"/>
-      <c r="AR20" s="25">
+      <c r="AM20" s="57"/>
+      <c r="AN20" s="58"/>
+      <c r="AO20" s="57"/>
+      <c r="AP20" s="58"/>
+      <c r="AQ20" s="66"/>
+      <c r="AR20" s="26"/>
+      <c r="AS20" s="25">
         <v>-275</v>
       </c>
-      <c r="AS20" s="25">
+      <c r="AT20" s="25">
         <v>99</v>
       </c>
-      <c r="AT20" s="25">
-        <f t="shared" ref="AT20:AT22" si="41">AS20+AR20</f>
+      <c r="AU20" s="25">
+        <f t="shared" ref="AU20:AU22" si="36">AT20+AS20</f>
         <v>-176</v>
       </c>
-      <c r="AU20" s="27">
-        <f>AR20*0.12116</f>
+      <c r="AV20" s="27">
+        <f>AS20*0.12116</f>
         <v>-33.319000000000003</v>
       </c>
-      <c r="AV20" s="27">
-        <f>AS20*0.20001</f>
+      <c r="AW20" s="27">
+        <f>AT20*0.20001</f>
         <v>19.800989999999999</v>
       </c>
-      <c r="AW20" s="56"/>
       <c r="AX20" s="56"/>
       <c r="AY20" s="56"/>
-      <c r="AZ20" s="64"/>
+      <c r="AZ20" s="56"/>
       <c r="BA20" s="64"/>
       <c r="BB20" s="64"/>
       <c r="BC20" s="64"/>
-      <c r="BD20" s="56"/>
+      <c r="BD20" s="64"/>
       <c r="BE20" s="56"/>
+      <c r="BF20" s="56"/>
     </row>
-    <row r="21" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23" t="s">
@@ -3448,7 +3508,7 @@
         <v>62</v>
       </c>
       <c r="P21" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="35"/>
         <v>64</v>
       </c>
       <c r="Q21" s="27">
@@ -3476,43 +3536,44 @@
       <c r="AG21" s="27"/>
       <c r="AH21" s="27"/>
       <c r="AI21" s="27"/>
-      <c r="AJ21" s="56"/>
-      <c r="AK21" s="57"/>
+      <c r="AJ21" s="27"/>
+      <c r="AK21" s="56"/>
       <c r="AL21" s="57"/>
-      <c r="AM21" s="58"/>
-      <c r="AN21" s="57"/>
-      <c r="AO21" s="58"/>
-      <c r="AP21" s="66"/>
-      <c r="AQ21" s="26"/>
-      <c r="AR21" s="25">
+      <c r="AM21" s="57"/>
+      <c r="AN21" s="58"/>
+      <c r="AO21" s="57"/>
+      <c r="AP21" s="58"/>
+      <c r="AQ21" s="66"/>
+      <c r="AR21" s="26"/>
+      <c r="AS21" s="25">
         <v>-46</v>
       </c>
-      <c r="AS21" s="25">
+      <c r="AT21" s="25">
         <v>33</v>
       </c>
-      <c r="AT21" s="25">
-        <f t="shared" si="41"/>
+      <c r="AU21" s="25">
+        <f t="shared" si="36"/>
         <v>-13</v>
       </c>
-      <c r="AU21" s="27">
-        <f>AR21*0.11761</f>
+      <c r="AV21" s="27">
+        <f>AS21*0.11761</f>
         <v>-5.4100600000000005</v>
       </c>
-      <c r="AV21" s="27">
-        <f>AS21*0.14296</f>
+      <c r="AW21" s="27">
+        <f>AT21*0.14296</f>
         <v>4.7176800000000005</v>
       </c>
-      <c r="AW21" s="56"/>
       <c r="AX21" s="56"/>
       <c r="AY21" s="56"/>
-      <c r="AZ21" s="64"/>
+      <c r="AZ21" s="56"/>
       <c r="BA21" s="64"/>
       <c r="BB21" s="64"/>
       <c r="BC21" s="64"/>
-      <c r="BD21" s="56"/>
+      <c r="BD21" s="64"/>
       <c r="BE21" s="56"/>
+      <c r="BF21" s="56"/>
     </row>
-    <row r="22" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="13">
         <v>45571</v>
@@ -3532,22 +3593,22 @@
         <v>-1292</v>
       </c>
       <c r="G22" s="15">
-        <f t="shared" ref="G22:H22" si="42">G23+G24</f>
+        <f t="shared" ref="G22:H22" si="37">G23+G24</f>
         <v>191</v>
       </c>
       <c r="H22" s="15">
-        <f t="shared" si="42"/>
+        <f t="shared" si="37"/>
         <v>157</v>
       </c>
       <c r="I22" s="15">
         <v>348</v>
       </c>
       <c r="J22" s="15">
-        <f t="shared" ref="J22:K22" si="43">J23+J24</f>
+        <f t="shared" ref="J22:K22" si="38">J23+J24</f>
         <v>-334</v>
       </c>
       <c r="K22" s="15">
-        <f t="shared" si="43"/>
+        <f t="shared" si="38"/>
         <v>-26</v>
       </c>
       <c r="L22" s="15">
@@ -3558,23 +3619,23 @@
         <v>0.27863777089783281</v>
       </c>
       <c r="N22" s="15">
-        <f t="shared" ref="N22:O22" si="44">N21+N20</f>
+        <f t="shared" ref="N22:O22" si="39">N21+N20</f>
         <v>-143</v>
       </c>
       <c r="O22" s="15">
-        <f t="shared" si="44"/>
+        <f t="shared" si="39"/>
         <v>131</v>
       </c>
       <c r="P22" s="15">
+        <f t="shared" si="35"/>
+        <v>-12</v>
+      </c>
+      <c r="Q22" s="17">
+        <f t="shared" ref="Q22:R22" si="40">Q20+Q21</f>
+        <v>-17.332979999999999</v>
+      </c>
+      <c r="R22" s="17">
         <f t="shared" si="40"/>
-        <v>-12</v>
-      </c>
-      <c r="Q22" s="17">
-        <f t="shared" ref="Q22:R22" si="45">Q20+Q21</f>
-        <v>-17.332979999999999</v>
-      </c>
-      <c r="R22" s="17">
-        <f t="shared" si="45"/>
         <v>22.664209999999997</v>
       </c>
       <c r="S22" s="17">
@@ -3598,127 +3659,130 @@
         <v>0.12120965034965034</v>
       </c>
       <c r="X22" s="20">
-        <f>Q22+R22+T22+0</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="20">
+        <f>Q22+R22+T22+X22</f>
         <v>3.8812299999999977</v>
       </c>
-      <c r="Y22" s="21">
+      <c r="Z22" s="21">
         <v>163.22999999999999</v>
       </c>
-      <c r="Z22" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="17">
+      <c r="AA22" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="17">
         <v>4.42</v>
       </c>
-      <c r="AB22" s="17">
+      <c r="AC22" s="17">
         <v>1.01</v>
       </c>
-      <c r="AC22" s="17">
+      <c r="AD22" s="17">
         <v>2.1</v>
       </c>
-      <c r="AD22" s="20">
-        <f>AC22+AB22+AA22</f>
+      <c r="AE22" s="20">
+        <f>AD22+AC22+AB22</f>
         <v>7.53</v>
       </c>
-      <c r="AE22" s="17">
+      <c r="AF22" s="17">
         <v>10</v>
       </c>
-      <c r="AF22" s="17">
+      <c r="AG22" s="17">
         <v>12.14</v>
       </c>
-      <c r="AG22" s="17">
-        <v>0</v>
-      </c>
       <c r="AH22" s="17">
-        <f>AE22+AF22+AG22</f>
+        <v>0</v>
+      </c>
+      <c r="AI22" s="17">
+        <f>AF22+AG22+AH22</f>
         <v>22.14</v>
       </c>
-      <c r="AI22" s="17">
+      <c r="AJ22" s="17">
         <v>-55.17</v>
       </c>
-      <c r="AJ22" s="22">
-        <f>Z22+AH22+AI22</f>
+      <c r="AK22" s="22">
+        <f>AA22+AI22+AJ22</f>
         <v>-33.03</v>
       </c>
-      <c r="AK22" s="15">
-        <f t="shared" ref="AK22:AL22" si="46">AR22-AN22</f>
+      <c r="AL22" s="15">
+        <f t="shared" ref="AL22:AM22" si="41">AS22-AO22</f>
         <v>544</v>
       </c>
-      <c r="AL22" s="15">
-        <f t="shared" si="46"/>
+      <c r="AM22" s="15">
+        <f t="shared" si="41"/>
         <v>199</v>
       </c>
-      <c r="AM22" s="15">
+      <c r="AN22" s="15">
         <v>743</v>
       </c>
-      <c r="AN22" s="15">
-        <f t="shared" ref="AN22:AO22" si="47">D22-J22</f>
+      <c r="AO22" s="15">
+        <f>D22-J22</f>
         <v>-865</v>
       </c>
-      <c r="AO22" s="15">
-        <f t="shared" si="47"/>
+      <c r="AP22" s="15">
+        <f>E22-K22</f>
         <v>-67</v>
       </c>
-      <c r="AP22" s="15">
+      <c r="AQ22" s="15">
         <v>-932</v>
       </c>
-      <c r="AQ22" s="16">
-        <f>AP22/F22</f>
+      <c r="AR22" s="16">
+        <f>AQ22/F22</f>
         <v>0.72136222910216719</v>
       </c>
-      <c r="AR22" s="15">
-        <f>AR20+AR21</f>
+      <c r="AS22" s="15">
+        <f>AS20+AS21</f>
         <v>-321</v>
       </c>
-      <c r="AS22" s="15">
-        <f>AS21+AS20</f>
+      <c r="AT22" s="15">
+        <f>AT21+AT20</f>
         <v>132</v>
       </c>
-      <c r="AT22" s="15">
-        <f t="shared" si="41"/>
+      <c r="AU22" s="15">
+        <f t="shared" si="36"/>
         <v>-189</v>
       </c>
-      <c r="AU22" s="17">
-        <f t="shared" ref="AU22:AV22" si="48">AU20+AU21</f>
+      <c r="AV22" s="17">
+        <f t="shared" ref="AV22:AW22" si="42">AV20+AV21</f>
         <v>-38.729060000000004</v>
       </c>
-      <c r="AV22" s="17">
-        <f t="shared" si="48"/>
+      <c r="AW22" s="17">
+        <f t="shared" si="42"/>
         <v>24.51867</v>
       </c>
-      <c r="AW22" s="17">
-        <f>AV22+AU22</f>
+      <c r="AX22" s="17">
+        <f>AW22+AV22</f>
         <v>-14.210390000000004</v>
       </c>
-      <c r="AX22" s="17">
-        <f>(AR20+AR21)*0.01</f>
+      <c r="AY22" s="17">
+        <f>(AS20+AS21)*0.01</f>
         <v>-3.21</v>
       </c>
-      <c r="AY22" s="17">
-        <v>0</v>
-      </c>
-      <c r="AZ22" s="20">
-        <f>AY22+AX22+AW22</f>
+      <c r="AZ22" s="17">
+        <v>0</v>
+      </c>
+      <c r="BA22" s="20">
+        <f>AZ22+AY22+AX22</f>
         <v>-17.420390000000005</v>
       </c>
-      <c r="BA22" s="21">
+      <c r="BB22" s="21">
         <v>204.71</v>
       </c>
-      <c r="BB22" s="21">
-        <v>0</v>
-      </c>
-      <c r="BC22" s="20">
+      <c r="BC22" s="21">
+        <v>0</v>
+      </c>
+      <c r="BD22" s="20">
         <v>12.14</v>
       </c>
-      <c r="BD22" s="17">
+      <c r="BE22" s="17">
         <v>-55.17</v>
       </c>
-      <c r="BE22" s="22">
-        <f t="shared" ref="BE22" si="49">BC22+BB22+BD22</f>
+      <c r="BF22" s="22">
+        <f t="shared" ref="BF22" si="43">BD22+BC22+BE22</f>
         <v>-43.03</v>
       </c>
     </row>
-    <row r="23" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="40"/>
       <c r="C23" s="25" t="s">
@@ -3769,19 +3833,19 @@
       <c r="AF23" s="27"/>
       <c r="AG23" s="27"/>
       <c r="AH23" s="27"/>
-      <c r="AI23" s="41"/>
-      <c r="AJ23" s="27"/>
-      <c r="AK23" s="25"/>
+      <c r="AI23" s="27"/>
+      <c r="AJ23" s="41"/>
+      <c r="AK23" s="27"/>
       <c r="AL23" s="25"/>
       <c r="AM23" s="25"/>
       <c r="AN23" s="25"/>
       <c r="AO23" s="25"/>
       <c r="AP23" s="25"/>
-      <c r="AQ23" s="26"/>
-      <c r="AR23" s="25"/>
+      <c r="AQ23" s="25"/>
+      <c r="AR23" s="26"/>
       <c r="AS23" s="25"/>
       <c r="AT23" s="25"/>
-      <c r="AU23" s="27"/>
+      <c r="AU23" s="25"/>
       <c r="AV23" s="27"/>
       <c r="AW23" s="27"/>
       <c r="AX23" s="27"/>
@@ -3792,8 +3856,9 @@
       <c r="BC23" s="27"/>
       <c r="BD23" s="27"/>
       <c r="BE23" s="27"/>
+      <c r="BF23" s="27"/>
     </row>
-    <row r="24" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="40"/>
       <c r="C24" s="25" t="s">
@@ -3844,19 +3909,19 @@
       <c r="AF24" s="27"/>
       <c r="AG24" s="27"/>
       <c r="AH24" s="27"/>
-      <c r="AI24" s="41"/>
-      <c r="AJ24" s="27"/>
-      <c r="AK24" s="25"/>
+      <c r="AI24" s="27"/>
+      <c r="AJ24" s="41"/>
+      <c r="AK24" s="27"/>
       <c r="AL24" s="25"/>
       <c r="AM24" s="25"/>
       <c r="AN24" s="25"/>
       <c r="AO24" s="25"/>
       <c r="AP24" s="25"/>
-      <c r="AQ24" s="26"/>
-      <c r="AR24" s="25"/>
+      <c r="AQ24" s="25"/>
+      <c r="AR24" s="26"/>
       <c r="AS24" s="25"/>
       <c r="AT24" s="25"/>
-      <c r="AU24" s="27"/>
+      <c r="AU24" s="25"/>
       <c r="AV24" s="27"/>
       <c r="AW24" s="27"/>
       <c r="AX24" s="27"/>
@@ -3867,8 +3932,9 @@
       <c r="BC24" s="27"/>
       <c r="BD24" s="27"/>
       <c r="BE24" s="27"/>
+      <c r="BF24" s="27"/>
     </row>
-    <row r="25" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="42">
         <v>45600</v>
@@ -3916,19 +3982,19 @@
         <v>191</v>
       </c>
       <c r="P25" s="43">
-        <f t="shared" ref="P25:P27" si="50">O25+N25</f>
+        <f t="shared" ref="P25:P27" si="44">O25+N25</f>
         <v>59</v>
       </c>
       <c r="Q25" s="45">
-        <f t="shared" ref="Q25:Q27" si="51">N25*0.11761</f>
+        <f t="shared" ref="Q25:Q27" si="45">N25*0.11761</f>
         <v>-15.524520000000001</v>
       </c>
       <c r="R25" s="45">
-        <f t="shared" ref="R25:R27" si="52">O25*0.14296</f>
+        <f t="shared" ref="R25:R27" si="46">O25*0.14296</f>
         <v>27.30536</v>
       </c>
       <c r="S25" s="45">
-        <f t="shared" ref="S25:S27" si="53">R25+Q25</f>
+        <f t="shared" ref="S25:S27" si="47">R25+Q25</f>
         <v>11.78084</v>
       </c>
       <c r="T25" s="45">
@@ -3936,129 +4002,136 @@
         <v>-1.32</v>
       </c>
       <c r="U25" s="18">
-        <f t="shared" ref="U25:U27" si="54">(ABS(Q25)+ABS(R25))/(ABS(N25)+ABS(O25))</f>
+        <f t="shared" ref="U25:U27" si="48">(ABS(Q25)+ABS(R25))/(ABS(N25)+ABS(O25))</f>
         <v>0.13260024767801859</v>
       </c>
       <c r="V25" s="19">
-        <f t="shared" ref="V25:V27" si="55">ABS(R25)/ABS(O25)</f>
+        <f t="shared" ref="V25:V27" si="49">ABS(R25)/ABS(O25)</f>
         <v>0.14296</v>
       </c>
       <c r="W25" s="19">
-        <f t="shared" ref="W25:W27" si="56">Q25/N25</f>
+        <f t="shared" ref="W25:W27" si="50">Q25/N25</f>
         <v>0.11761000000000001</v>
       </c>
       <c r="X25" s="20">
-        <f t="shared" ref="X25:X26" si="57">Q25+R25+T25+0.02</f>
+        <v>0.02</v>
+      </c>
+      <c r="Y25" s="20">
+        <f>Q25+R25+T25+X25</f>
         <v>10.480839999999999</v>
       </c>
-      <c r="Y25" s="21">
+      <c r="Z25" s="21">
         <v>152.74</v>
       </c>
-      <c r="Z25" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA25" s="45">
+      <c r="AA25" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="45">
         <v>27.92</v>
       </c>
-      <c r="AB25" s="45">
+      <c r="AC25" s="45">
         <v>-5.97</v>
       </c>
-      <c r="AC25" s="45">
+      <c r="AD25" s="45">
         <v>3.43</v>
       </c>
-      <c r="AD25" s="20">
-        <f t="shared" ref="AD25:AD27" si="58">AC25+AB25+AA25</f>
+      <c r="AE25" s="20">
+        <f t="shared" ref="AE25:AE27" si="51">AD25+AC25+AB25</f>
         <v>25.380000000000003</v>
       </c>
-      <c r="AE25" s="45">
+      <c r="AF25" s="45">
         <v>10</v>
       </c>
-      <c r="AF25" s="45">
+      <c r="AG25" s="45">
         <v>11.36</v>
       </c>
-      <c r="AG25" s="45">
-        <v>0</v>
-      </c>
       <c r="AH25" s="45">
-        <f t="shared" ref="AH25:AH27" si="59">AE25+AF25+AG25</f>
+        <v>0</v>
+      </c>
+      <c r="AI25" s="45">
+        <f t="shared" ref="AI25:AI27" si="52">AF25+AG25+AH25</f>
         <v>21.36</v>
       </c>
-      <c r="AI25" s="46"/>
-      <c r="AJ25" s="22">
-        <f>Z25+AH25+AI25</f>
+      <c r="AJ25" s="46">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="22">
+        <f>AA25+AI25+AJ25</f>
         <v>21.36</v>
       </c>
-      <c r="AK25" s="43">
+      <c r="AL25" s="43">
         <v>487</v>
       </c>
-      <c r="AL25" s="43">
+      <c r="AM25" s="43">
         <v>168</v>
       </c>
-      <c r="AM25" s="43">
+      <c r="AN25" s="43">
         <v>655</v>
       </c>
-      <c r="AN25" s="43">
+      <c r="AO25" s="43">
         <v>-622</v>
       </c>
-      <c r="AO25" s="43">
+      <c r="AP25" s="43">
         <v>-11</v>
       </c>
-      <c r="AP25" s="43">
+      <c r="AQ25" s="43">
         <v>-633</v>
       </c>
-      <c r="AQ25" s="44">
-        <f>AP25/F25</f>
+      <c r="AR25" s="44">
+        <f>AQ25/F25</f>
         <v>0.6393939393939394</v>
       </c>
-      <c r="AR25" s="43">
+      <c r="AS25" s="43">
         <v>-135</v>
       </c>
-      <c r="AS25" s="43">
+      <c r="AT25" s="43">
         <v>157</v>
       </c>
-      <c r="AT25" s="43">
-        <f t="shared" ref="AT25:AT27" si="60">AS25+AR25</f>
+      <c r="AU25" s="43">
+        <f t="shared" ref="AU25:AU27" si="53">AT25+AS25</f>
         <v>22</v>
       </c>
-      <c r="AU25" s="45">
-        <f t="shared" ref="AU25:AU27" si="61">AR25*0.11761</f>
+      <c r="AV25" s="45">
+        <f t="shared" ref="AV25:AV27" si="54">AS25*0.11761</f>
         <v>-15.877350000000002</v>
       </c>
-      <c r="AV25" s="45">
-        <f t="shared" ref="AV25:AV27" si="62">AS25*0.14296</f>
+      <c r="AW25" s="45">
+        <f t="shared" ref="AW25:AW27" si="55">AT25*0.14296</f>
         <v>22.44472</v>
       </c>
-      <c r="AW25" s="45">
-        <f t="shared" ref="AW25:AW27" si="63">AV25+AU25</f>
+      <c r="AX25" s="45">
+        <f t="shared" ref="AX25:AX27" si="56">AW25+AV25</f>
         <v>6.5673699999999986</v>
       </c>
-      <c r="AX25" s="45">
-        <f>AR25*0.01</f>
+      <c r="AY25" s="45">
+        <f>AS25*0.01</f>
         <v>-1.35</v>
       </c>
-      <c r="AY25" s="45">
+      <c r="AZ25" s="45">
         <v>0.01</v>
       </c>
-      <c r="AZ25" s="20">
-        <f t="shared" ref="AZ25:AZ27" si="64">AY25+AX25+AW25</f>
+      <c r="BA25" s="20">
+        <f t="shared" ref="BA25:BA27" si="57">AZ25+AY25+AX25</f>
         <v>5.2273699999999987</v>
       </c>
-      <c r="BA25" s="21">
+      <c r="BB25" s="21">
         <v>199.49</v>
       </c>
-      <c r="BB25" s="21">
-        <v>0</v>
-      </c>
-      <c r="BC25" s="20">
+      <c r="BC25" s="21">
+        <v>0</v>
+      </c>
+      <c r="BD25" s="20">
         <v>11.36</v>
       </c>
-      <c r="BD25" s="45"/>
-      <c r="BE25" s="22">
-        <f t="shared" ref="BE25:BE27" si="65">BC25+BB25+BD25</f>
+      <c r="BE25" s="45">
+        <v>0</v>
+      </c>
+      <c r="BF25" s="22">
+        <f t="shared" ref="BF25:BF27" si="58">BD25+BC25+BE25</f>
         <v>11.36</v>
       </c>
     </row>
-    <row r="26" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="13">
         <v>45631</v>
@@ -4071,7 +4144,7 @@
         <v>-605</v>
       </c>
       <c r="E26" s="15">
-        <f t="shared" ref="E25:E27" si="66">ROUND(K26/M26,0)</f>
+        <f t="shared" ref="E26:E27" si="59">ROUND(K26/M26,0)</f>
         <v>0</v>
       </c>
       <c r="F26" s="15">
@@ -4096,7 +4169,7 @@
         <v>-206</v>
       </c>
       <c r="M26" s="16">
-        <f t="shared" ref="M25:M27" si="67">L26/F26</f>
+        <f t="shared" ref="M26" si="60">L26/F26</f>
         <v>0.34049586776859503</v>
       </c>
       <c r="N26" s="15">
@@ -4106,151 +4179,158 @@
         <v>214</v>
       </c>
       <c r="P26" s="15">
+        <f t="shared" si="44"/>
+        <v>358</v>
+      </c>
+      <c r="Q26" s="17">
+        <f t="shared" si="45"/>
+        <v>16.935840000000002</v>
+      </c>
+      <c r="R26" s="17">
+        <f t="shared" si="46"/>
+        <v>30.593440000000001</v>
+      </c>
+      <c r="S26" s="17">
+        <f t="shared" si="47"/>
+        <v>47.52928</v>
+      </c>
+      <c r="T26" s="17">
+        <v>0</v>
+      </c>
+      <c r="U26" s="18">
+        <f t="shared" si="48"/>
+        <v>0.13276335195530725</v>
+      </c>
+      <c r="V26" s="19">
+        <f t="shared" si="49"/>
+        <v>0.14296</v>
+      </c>
+      <c r="W26" s="19">
         <f t="shared" si="50"/>
-        <v>358</v>
-      </c>
-      <c r="Q26" s="17">
+        <v>0.11761000000000002</v>
+      </c>
+      <c r="X26" s="20">
+        <v>0.02</v>
+      </c>
+      <c r="Y26" s="20">
+        <f>Q26+R26+T26+X26</f>
+        <v>47.549280000000003</v>
+      </c>
+      <c r="Z26" s="21">
+        <v>105.1</v>
+      </c>
+      <c r="AA26" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="17">
+        <v>120.14</v>
+      </c>
+      <c r="AC26" s="17">
+        <v>-36.22</v>
+      </c>
+      <c r="AD26" s="17">
+        <v>8.11</v>
+      </c>
+      <c r="AE26" s="20">
         <f t="shared" si="51"/>
-        <v>16.935840000000002</v>
-      </c>
-      <c r="R26" s="17">
+        <v>92.03</v>
+      </c>
+      <c r="AF26" s="17">
+        <v>10</v>
+      </c>
+      <c r="AG26" s="17">
+        <v>12.14</v>
+      </c>
+      <c r="AH26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="17">
         <f t="shared" si="52"/>
-        <v>30.593440000000001</v>
-      </c>
-      <c r="S26" s="17">
-        <f t="shared" si="53"/>
-        <v>47.52928</v>
-      </c>
-      <c r="T26" s="17">
-        <v>0</v>
-      </c>
-      <c r="U26" s="18">
-        <f t="shared" si="54"/>
-        <v>0.13276335195530725</v>
-      </c>
-      <c r="V26" s="19">
-        <f t="shared" si="55"/>
-        <v>0.14296</v>
-      </c>
-      <c r="W26" s="19">
-        <f t="shared" si="56"/>
-        <v>0.11761000000000002</v>
-      </c>
-      <c r="X26" s="20">
-        <f t="shared" si="57"/>
-        <v>47.549280000000003</v>
-      </c>
-      <c r="Y26" s="21">
-        <v>105.1</v>
-      </c>
-      <c r="Z26" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA26" s="17">
-        <v>120.14</v>
-      </c>
-      <c r="AB26" s="17">
-        <v>-36.22</v>
-      </c>
-      <c r="AC26" s="17">
-        <v>8.11</v>
-      </c>
-      <c r="AD26" s="20">
-        <f t="shared" si="58"/>
-        <v>92.03</v>
-      </c>
-      <c r="AE26" s="17">
-        <v>10</v>
-      </c>
-      <c r="AF26" s="17">
-        <v>12.14</v>
-      </c>
-      <c r="AG26" s="17">
-        <v>0</v>
-      </c>
-      <c r="AH26" s="17">
-        <f t="shared" si="59"/>
         <v>22.14</v>
       </c>
-      <c r="AI26" s="47"/>
-      <c r="AJ26" s="22">
-        <f>Z26+AH26+AI26</f>
+      <c r="AJ26" s="47">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="22">
+        <f>AA26+AI26+AJ26</f>
         <v>22.14</v>
       </c>
-      <c r="AK26" s="15">
-        <f t="shared" ref="AK26:AL26" si="68">AR26-AN26</f>
+      <c r="AL26" s="15">
+        <f t="shared" ref="AL26:AM26" si="61">AS26-AO26</f>
         <v>599</v>
       </c>
-      <c r="AL26" s="15">
-        <f t="shared" si="68"/>
+      <c r="AM26" s="15">
+        <f t="shared" si="61"/>
         <v>242</v>
       </c>
-      <c r="AM26" s="15">
+      <c r="AN26" s="15">
         <v>841</v>
       </c>
-      <c r="AN26" s="15">
+      <c r="AO26" s="15">
         <f>D26-J26</f>
         <v>-399</v>
       </c>
-      <c r="AO26" s="15">
+      <c r="AP26" s="15">
         <f>E26-K26</f>
         <v>0</v>
       </c>
-      <c r="AP26" s="15">
+      <c r="AQ26" s="15">
         <v>-399</v>
       </c>
-      <c r="AQ26" s="16">
-        <f>AP26/F26</f>
+      <c r="AR26" s="16">
+        <f>AQ26/F26</f>
         <v>0.65950413223140492</v>
       </c>
-      <c r="AR26" s="15">
+      <c r="AS26" s="15">
         <v>200</v>
       </c>
-      <c r="AS26" s="15">
+      <c r="AT26" s="15">
         <v>242</v>
       </c>
-      <c r="AT26" s="15">
-        <f t="shared" si="60"/>
+      <c r="AU26" s="15">
+        <f t="shared" si="53"/>
         <v>442</v>
       </c>
-      <c r="AU26" s="17">
-        <f t="shared" si="61"/>
+      <c r="AV26" s="17">
+        <f t="shared" si="54"/>
         <v>23.522000000000002</v>
       </c>
-      <c r="AV26" s="17">
-        <f t="shared" si="62"/>
+      <c r="AW26" s="17">
+        <f t="shared" si="55"/>
         <v>34.596319999999999</v>
       </c>
-      <c r="AW26" s="17">
-        <f t="shared" si="63"/>
+      <c r="AX26" s="17">
+        <f t="shared" si="56"/>
         <v>58.118319999999997</v>
       </c>
-      <c r="AX26" s="17">
-        <v>0</v>
-      </c>
       <c r="AY26" s="17">
+        <v>0</v>
+      </c>
+      <c r="AZ26" s="17">
         <v>0.13</v>
       </c>
-      <c r="AZ26" s="20">
-        <f t="shared" si="64"/>
+      <c r="BA26" s="20">
+        <f t="shared" si="57"/>
         <v>58.24832</v>
       </c>
-      <c r="BA26" s="21">
+      <c r="BB26" s="21">
         <v>141.24</v>
       </c>
-      <c r="BB26" s="21">
-        <v>0</v>
-      </c>
-      <c r="BC26" s="20">
+      <c r="BC26" s="21">
+        <v>0</v>
+      </c>
+      <c r="BD26" s="20">
         <v>12.14</v>
       </c>
-      <c r="BD26" s="17"/>
-      <c r="BE26" s="22">
-        <f t="shared" si="65"/>
+      <c r="BE26" s="17">
+        <v>0</v>
+      </c>
+      <c r="BF26" s="22">
+        <f t="shared" si="58"/>
         <v>12.14</v>
       </c>
     </row>
-    <row r="27" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="13">
         <v>45663</v>
@@ -4259,33 +4339,33 @@
         <v>45673</v>
       </c>
       <c r="D27" s="15">
-        <f t="shared" ref="D25:D27" si="69">ROUND(J27/M27,0)</f>
+        <f t="shared" ref="D27" si="62">ROUND(J27/M27,0)</f>
         <v>-309</v>
       </c>
       <c r="E27" s="15">
-        <f t="shared" si="66"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="F27" s="15">
         <v>-309</v>
       </c>
       <c r="G27" s="15">
-        <f t="shared" ref="G27:H27" si="70">G28+G29</f>
+        <f t="shared" ref="G27:H27" si="63">G28+G29</f>
         <v>489</v>
       </c>
       <c r="H27" s="15">
-        <f t="shared" si="70"/>
+        <f t="shared" si="63"/>
         <v>332</v>
       </c>
       <c r="I27" s="15">
         <v>821</v>
       </c>
       <c r="J27" s="15">
-        <f t="shared" ref="J27:K27" si="71">J28+J29</f>
+        <f t="shared" ref="J27:K27" si="64">J28+J29</f>
         <v>-210</v>
       </c>
       <c r="K27" s="15">
-        <f t="shared" si="71"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="L27" s="15">
@@ -4302,151 +4382,158 @@
         <v>332</v>
       </c>
       <c r="P27" s="15">
+        <f t="shared" si="44"/>
+        <v>611</v>
+      </c>
+      <c r="Q27" s="17">
+        <f t="shared" si="45"/>
+        <v>32.813189999999999</v>
+      </c>
+      <c r="R27" s="17">
+        <f t="shared" si="46"/>
+        <v>47.462720000000004</v>
+      </c>
+      <c r="S27" s="17">
+        <f t="shared" si="47"/>
+        <v>80.27591000000001</v>
+      </c>
+      <c r="T27" s="17">
+        <v>0</v>
+      </c>
+      <c r="U27" s="18">
+        <f t="shared" si="48"/>
+        <v>0.1313844680851064</v>
+      </c>
+      <c r="V27" s="19">
+        <f t="shared" si="49"/>
+        <v>0.14296</v>
+      </c>
+      <c r="W27" s="19">
         <f t="shared" si="50"/>
-        <v>611</v>
-      </c>
-      <c r="Q27" s="17">
+        <v>0.11760999999999999</v>
+      </c>
+      <c r="X27" s="20">
+        <v>0.18</v>
+      </c>
+      <c r="Y27" s="20">
+        <f>Q27+R27+T27+X27</f>
+        <v>80.455910000000017</v>
+      </c>
+      <c r="Z27" s="21">
+        <v>24.65</v>
+      </c>
+      <c r="AA27" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="17">
+        <v>201.73</v>
+      </c>
+      <c r="AC27" s="17">
+        <v>-41.77</v>
+      </c>
+      <c r="AD27" s="17">
+        <v>12.56</v>
+      </c>
+      <c r="AE27" s="20">
         <f t="shared" si="51"/>
-        <v>32.813189999999999</v>
-      </c>
-      <c r="R27" s="17">
+        <v>172.51999999999998</v>
+      </c>
+      <c r="AF27" s="17">
+        <v>10</v>
+      </c>
+      <c r="AG27" s="17">
+        <v>12.53</v>
+      </c>
+      <c r="AH27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="17">
         <f t="shared" si="52"/>
-        <v>47.462720000000004</v>
-      </c>
-      <c r="S27" s="17">
-        <f t="shared" si="53"/>
-        <v>80.27591000000001</v>
-      </c>
-      <c r="T27" s="17">
-        <v>0</v>
-      </c>
-      <c r="U27" s="18">
-        <f t="shared" si="54"/>
-        <v>0.1313844680851064</v>
-      </c>
-      <c r="V27" s="19">
-        <f t="shared" si="55"/>
-        <v>0.14296</v>
-      </c>
-      <c r="W27" s="19">
-        <f t="shared" si="56"/>
-        <v>0.11760999999999999</v>
-      </c>
-      <c r="X27" s="20">
-        <f>Q27+R27+T27+0.18</f>
-        <v>80.455910000000017</v>
-      </c>
-      <c r="Y27" s="21">
-        <v>24.65</v>
-      </c>
-      <c r="Z27" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="17">
-        <v>201.73</v>
-      </c>
-      <c r="AB27" s="17">
-        <v>-41.77</v>
-      </c>
-      <c r="AC27" s="17">
-        <v>12.56</v>
-      </c>
-      <c r="AD27" s="20">
-        <f t="shared" si="58"/>
-        <v>172.51999999999998</v>
-      </c>
-      <c r="AE27" s="17">
-        <v>10</v>
-      </c>
-      <c r="AF27" s="17">
-        <v>12.53</v>
-      </c>
-      <c r="AG27" s="17">
-        <v>0</v>
-      </c>
-      <c r="AH27" s="17">
-        <f t="shared" si="59"/>
         <v>22.53</v>
       </c>
-      <c r="AI27" s="47"/>
-      <c r="AJ27" s="22">
-        <f>Z27+AH27+AI27</f>
+      <c r="AJ27" s="47">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="22">
+        <f>AA27+AI27+AJ27</f>
         <v>22.53</v>
       </c>
-      <c r="AK27" s="15">
-        <f t="shared" ref="AK27:AL27" si="72">AR27-AN27</f>
+      <c r="AL27" s="15">
+        <f t="shared" ref="AL27:AM27" si="65">AS27-AO27</f>
         <v>693</v>
       </c>
-      <c r="AL27" s="15">
-        <f t="shared" si="72"/>
+      <c r="AM27" s="15">
+        <f t="shared" si="65"/>
         <v>231</v>
       </c>
-      <c r="AM27" s="15">
+      <c r="AN27" s="15">
         <v>924</v>
       </c>
-      <c r="AN27" s="15">
+      <c r="AO27" s="15">
         <f>D27-J27</f>
         <v>-99</v>
       </c>
-      <c r="AO27" s="15">
+      <c r="AP27" s="15">
         <f>E27-K27</f>
         <v>0</v>
       </c>
-      <c r="AP27" s="15">
+      <c r="AQ27" s="15">
         <v>-99</v>
       </c>
-      <c r="AQ27" s="16">
-        <f>AP27/F27</f>
+      <c r="AR27" s="16">
+        <f>AQ27/F27</f>
         <v>0.32038834951456313</v>
       </c>
-      <c r="AR27" s="15">
+      <c r="AS27" s="15">
         <v>594</v>
       </c>
-      <c r="AS27" s="15">
+      <c r="AT27" s="15">
         <v>231</v>
       </c>
-      <c r="AT27" s="15">
-        <f t="shared" si="60"/>
+      <c r="AU27" s="15">
+        <f t="shared" si="53"/>
         <v>825</v>
       </c>
-      <c r="AU27" s="17">
-        <f t="shared" si="61"/>
+      <c r="AV27" s="17">
+        <f t="shared" si="54"/>
         <v>69.860340000000008</v>
       </c>
-      <c r="AV27" s="17">
-        <f t="shared" si="62"/>
+      <c r="AW27" s="17">
+        <f t="shared" si="55"/>
         <v>33.023760000000003</v>
       </c>
-      <c r="AW27" s="17">
-        <f t="shared" si="63"/>
+      <c r="AX27" s="17">
+        <f t="shared" si="56"/>
         <v>102.88410000000002</v>
       </c>
-      <c r="AX27" s="17">
-        <v>0</v>
-      </c>
       <c r="AY27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AZ27" s="17">
         <v>0.25</v>
       </c>
-      <c r="AZ27" s="20">
-        <f t="shared" si="64"/>
+      <c r="BA27" s="20">
+        <f t="shared" si="57"/>
         <v>103.13410000000002</v>
       </c>
-      <c r="BA27" s="21">
+      <c r="BB27" s="21">
         <v>38.11</v>
       </c>
-      <c r="BB27" s="21">
-        <v>0</v>
-      </c>
-      <c r="BC27" s="20">
+      <c r="BC27" s="21">
+        <v>0</v>
+      </c>
+      <c r="BD27" s="20">
         <v>12.53</v>
       </c>
-      <c r="BD27" s="17"/>
-      <c r="BE27" s="22">
-        <f t="shared" si="65"/>
+      <c r="BE27" s="17">
+        <v>0</v>
+      </c>
+      <c r="BF27" s="22">
+        <f t="shared" si="58"/>
         <v>12.53</v>
       </c>
     </row>
-    <row r="28" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="28"/>
       <c r="C28" s="29" t="s">
@@ -4497,19 +4584,19 @@
       <c r="AF28" s="32"/>
       <c r="AG28" s="32"/>
       <c r="AH28" s="32"/>
-      <c r="AI28" s="48"/>
-      <c r="AJ28" s="32"/>
-      <c r="AK28" s="29"/>
+      <c r="AI28" s="32"/>
+      <c r="AJ28" s="48"/>
+      <c r="AK28" s="32"/>
       <c r="AL28" s="29"/>
       <c r="AM28" s="29"/>
       <c r="AN28" s="29"/>
       <c r="AO28" s="29"/>
       <c r="AP28" s="29"/>
-      <c r="AQ28" s="30"/>
-      <c r="AR28" s="29"/>
+      <c r="AQ28" s="29"/>
+      <c r="AR28" s="30"/>
       <c r="AS28" s="29"/>
       <c r="AT28" s="29"/>
-      <c r="AU28" s="32"/>
+      <c r="AU28" s="29"/>
       <c r="AV28" s="32"/>
       <c r="AW28" s="32"/>
       <c r="AX28" s="32"/>
@@ -4520,8 +4607,9 @@
       <c r="BC28" s="32"/>
       <c r="BD28" s="32"/>
       <c r="BE28" s="32"/>
+      <c r="BF28" s="32"/>
     </row>
-    <row r="29" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="28"/>
       <c r="C29" s="29" t="s">
@@ -4572,19 +4660,19 @@
       <c r="AF29" s="32"/>
       <c r="AG29" s="32"/>
       <c r="AH29" s="32"/>
-      <c r="AI29" s="48"/>
-      <c r="AJ29" s="32"/>
-      <c r="AK29" s="29"/>
+      <c r="AI29" s="32"/>
+      <c r="AJ29" s="48"/>
+      <c r="AK29" s="32"/>
       <c r="AL29" s="29"/>
       <c r="AM29" s="29"/>
       <c r="AN29" s="29"/>
       <c r="AO29" s="29"/>
       <c r="AP29" s="29"/>
-      <c r="AQ29" s="30"/>
-      <c r="AR29" s="29"/>
+      <c r="AQ29" s="29"/>
+      <c r="AR29" s="30"/>
       <c r="AS29" s="29"/>
       <c r="AT29" s="29"/>
-      <c r="AU29" s="32"/>
+      <c r="AU29" s="29"/>
       <c r="AV29" s="32"/>
       <c r="AW29" s="32"/>
       <c r="AX29" s="32"/>
@@ -4595,8 +4683,9 @@
       <c r="BC29" s="32"/>
       <c r="BD29" s="32"/>
       <c r="BE29" s="32"/>
+      <c r="BF29" s="32"/>
     </row>
-    <row r="30" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="13">
         <v>45692</v>
@@ -4658,132 +4747,139 @@
         <v>-10</v>
       </c>
       <c r="U30" s="18">
-        <f t="shared" ref="U30:U31" si="73">(ABS(Q30)+ABS(R30))/(ABS(N30)+ABS(O30))</f>
+        <f t="shared" ref="U30:U31" si="66">(ABS(Q30)+ABS(R30))/(ABS(N30)+ABS(O30))</f>
         <v>0.12236459709379127</v>
       </c>
       <c r="V30" s="19">
-        <f t="shared" ref="V30:V31" si="74">ABS(R30)/ABS(O30)</f>
+        <f t="shared" ref="V30:V31" si="67">ABS(R30)/ABS(O30)</f>
         <v>0.14295774647887324</v>
       </c>
       <c r="W30" s="19">
-        <f t="shared" ref="W30:W31" si="75">Q30/N30</f>
+        <f t="shared" ref="W30:W31" si="68">Q30/N30</f>
         <v>0.11760975609756097</v>
       </c>
       <c r="X30" s="20">
-        <f>Q30+R30+T30</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="20">
+        <f>Q30+R30+T30+X30</f>
         <v>82.63</v>
       </c>
-      <c r="Y30" s="21">
-        <v>0</v>
-      </c>
       <c r="Z30" s="21">
-        <f>X30-14.65+0.23</f>
+        <v>0</v>
+      </c>
+      <c r="AA30" s="21">
+        <f>Y30-14.65+0.23</f>
         <v>68.209999999999994</v>
       </c>
-      <c r="AA30" s="17">
+      <c r="AB30" s="17">
         <v>248.1</v>
       </c>
-      <c r="AB30" s="17">
+      <c r="AC30" s="17">
         <v>-37.92</v>
       </c>
-      <c r="AC30" s="17">
+      <c r="AD30" s="17">
         <v>14.16</v>
       </c>
-      <c r="AD30" s="20">
-        <f>AC30+AB30+AA30</f>
+      <c r="AE30" s="20">
+        <f>AD30+AC30+AB30</f>
         <v>224.34</v>
       </c>
-      <c r="AE30" s="17">
+      <c r="AF30" s="17">
         <v>10</v>
       </c>
-      <c r="AF30" s="17">
+      <c r="AG30" s="17">
         <v>11.36</v>
       </c>
-      <c r="AG30" s="17">
-        <v>0</v>
-      </c>
       <c r="AH30" s="17">
-        <f t="shared" ref="AH30:AH31" si="76">AE30+AF30+AG30</f>
+        <v>0</v>
+      </c>
+      <c r="AI30" s="17">
+        <f t="shared" ref="AI30:AI31" si="69">AF30+AG30+AH30</f>
         <v>21.36</v>
       </c>
-      <c r="AI30" s="47"/>
-      <c r="AJ30" s="22">
-        <f>Z30+AH30+AI30</f>
+      <c r="AJ30" s="47">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="22">
+        <f>AA30+AI30+AJ30</f>
         <v>89.57</v>
       </c>
-      <c r="AK30" s="15">
-        <f t="shared" ref="AK30:AL30" si="77">AR30-AN30</f>
+      <c r="AL30" s="15">
+        <f t="shared" ref="AL30:AM30" si="70">AS30-AO30</f>
         <v>732</v>
       </c>
-      <c r="AL30" s="15">
-        <f t="shared" si="77"/>
+      <c r="AM30" s="15">
+        <f t="shared" si="70"/>
         <v>9</v>
       </c>
-      <c r="AM30" s="15">
+      <c r="AN30" s="15">
         <v>741</v>
       </c>
-      <c r="AN30" s="15">
-        <f t="shared" ref="AN30:AO33" si="78">D30-J30</f>
-        <v>0</v>
-      </c>
       <c r="AO30" s="15">
-        <f t="shared" si="78"/>
+        <f>D30-J30</f>
+        <v>0</v>
+      </c>
+      <c r="AP30" s="15">
+        <f>E30-K30</f>
         <v>190</v>
       </c>
-      <c r="AP30" s="15">
+      <c r="AQ30" s="15">
         <v>190</v>
       </c>
-      <c r="AQ30" s="49" t="s">
+      <c r="AR30" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="AR30" s="15">
+      <c r="AS30" s="15">
         <v>732</v>
       </c>
-      <c r="AS30" s="15">
+      <c r="AT30" s="15">
         <v>199</v>
       </c>
-      <c r="AT30" s="15">
-        <f t="shared" ref="AT30:AT32" si="79">AS30+AR30</f>
+      <c r="AU30" s="15">
+        <f t="shared" ref="AU30:AU32" si="71">AT30+AS30</f>
         <v>931</v>
       </c>
-      <c r="AU30" s="17">
-        <f>AR30*0.11761</f>
+      <c r="AV30" s="17">
+        <f>AS30*0.11761</f>
         <v>86.090519999999998</v>
       </c>
-      <c r="AV30" s="17">
-        <f>AS30*0.14296</f>
+      <c r="AW30" s="17">
+        <f>AT30*0.14296</f>
         <v>28.44904</v>
       </c>
-      <c r="AW30" s="17">
-        <f t="shared" ref="AW30:AW31" si="80">AV30+AU30</f>
+      <c r="AX30" s="17">
+        <f t="shared" ref="AX30:AX31" si="72">AW30+AV30</f>
         <v>114.53955999999999</v>
       </c>
-      <c r="AX30" s="17">
-        <v>0</v>
-      </c>
       <c r="AY30" s="17">
+        <v>0</v>
+      </c>
+      <c r="AZ30" s="17">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AZ30" s="20">
-        <f t="shared" ref="AZ30:AZ31" si="81">AY30+AX30+AW30</f>
+      <c r="BA30" s="20">
+        <f t="shared" ref="BA30:BA31" si="73">AZ30+AY30+AX30</f>
         <v>114.81956</v>
       </c>
-      <c r="BA30" s="21">
-        <v>0</v>
-      </c>
       <c r="BB30" s="21">
+        <v>0</v>
+      </c>
+      <c r="BC30" s="21">
         <v>76.709999999999994</v>
       </c>
-      <c r="BC30" s="20">
+      <c r="BD30" s="20">
         <v>11.36</v>
       </c>
-      <c r="BD30" s="17"/>
-      <c r="BE30" s="22">
-        <f t="shared" ref="BE30:BE31" si="82">BC30+BB30+BD30</f>
+      <c r="BE30" s="17">
+        <v>0</v>
+      </c>
+      <c r="BF30" s="22">
+        <f t="shared" ref="BF30:BF31" si="74">BD30+BC30+BE30</f>
         <v>88.07</v>
       </c>
     </row>
-    <row r="31" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="13">
         <v>45722</v>
@@ -4803,22 +4899,22 @@
         <v>-762</v>
       </c>
       <c r="G31" s="15">
-        <f t="shared" ref="G31:H31" si="83">G32+G33</f>
+        <f t="shared" ref="G31:H31" si="75">G32+G33</f>
         <v>321</v>
       </c>
       <c r="H31" s="15">
-        <f t="shared" si="83"/>
+        <f t="shared" si="75"/>
         <v>286</v>
       </c>
       <c r="I31" s="15">
         <v>607</v>
       </c>
       <c r="J31" s="15">
-        <f t="shared" ref="J31:K31" si="84">J32+J33</f>
+        <f t="shared" ref="J31:K31" si="76">J32+J33</f>
         <v>-304</v>
       </c>
       <c r="K31" s="15">
-        <f t="shared" si="84"/>
+        <f t="shared" si="76"/>
         <v>-1</v>
       </c>
       <c r="L31" s="15">
@@ -4838,149 +4934,156 @@
         <v>302</v>
       </c>
       <c r="Q31" s="17">
-        <f t="shared" ref="Q31:S31" si="85">Q32+Q33</f>
+        <f t="shared" ref="Q31:S31" si="77">Q32+Q33</f>
         <v>1.9100000000000001</v>
       </c>
       <c r="R31" s="17">
-        <f t="shared" si="85"/>
+        <f t="shared" si="77"/>
         <v>38.949999999999996</v>
       </c>
       <c r="S31" s="17">
-        <f t="shared" si="85"/>
+        <f t="shared" si="77"/>
         <v>40.859999999999992</v>
       </c>
       <c r="T31" s="17">
         <v>0</v>
       </c>
       <c r="U31" s="18">
-        <f t="shared" si="73"/>
+        <f t="shared" si="66"/>
         <v>0.1352980132450331</v>
       </c>
       <c r="V31" s="19">
-        <f t="shared" si="74"/>
+        <f t="shared" si="67"/>
         <v>0.13666666666666666</v>
       </c>
       <c r="W31" s="19">
-        <f t="shared" si="75"/>
+        <f t="shared" si="68"/>
         <v>0.1123529411764706</v>
       </c>
       <c r="X31" s="20">
-        <f>Q31+R31+T31+0.09</f>
+        <v>0.09</v>
+      </c>
+      <c r="Y31" s="20">
+        <f>Q31+R31+T31+X31</f>
         <v>40.950000000000003</v>
       </c>
-      <c r="Y31" s="21">
-        <v>0</v>
-      </c>
       <c r="Z31" s="21">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="21">
         <v>40.950000000000003</v>
       </c>
-      <c r="AA31" s="17">
+      <c r="AB31" s="17">
         <v>106.04</v>
       </c>
-      <c r="AB31" s="17">
+      <c r="AC31" s="17">
         <v>-30.72</v>
       </c>
-      <c r="AC31" s="17">
+      <c r="AD31" s="17">
         <v>6.77</v>
       </c>
-      <c r="AD31" s="20">
+      <c r="AE31" s="20">
         <v>82.09</v>
       </c>
-      <c r="AE31" s="17">
+      <c r="AF31" s="17">
         <v>10</v>
       </c>
-      <c r="AF31" s="17">
+      <c r="AG31" s="17">
         <v>11.82</v>
       </c>
-      <c r="AG31" s="17">
-        <v>0</v>
-      </c>
       <c r="AH31" s="17">
-        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="AI31" s="17">
+        <f t="shared" si="69"/>
         <v>21.82</v>
       </c>
-      <c r="AI31" s="15"/>
-      <c r="AJ31" s="22">
-        <f>Z31+AH31+AI31</f>
+      <c r="AJ31" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="22">
+        <f>AA31+AI31+AJ31</f>
         <v>62.77</v>
       </c>
-      <c r="AK31" s="15">
-        <f t="shared" ref="AK31:AL31" si="86">AR31-AN31</f>
+      <c r="AL31" s="15">
+        <f t="shared" ref="AL31:AM31" si="78">AS31-AO31</f>
         <v>592</v>
       </c>
-      <c r="AL31" s="15">
-        <f t="shared" si="86"/>
+      <c r="AM31" s="15">
+        <f t="shared" si="78"/>
         <v>242</v>
       </c>
-      <c r="AM31" s="15">
+      <c r="AN31" s="15">
         <v>834</v>
       </c>
-      <c r="AN31" s="15">
-        <f t="shared" si="78"/>
+      <c r="AO31" s="15">
+        <f>D31-J31</f>
         <v>-456</v>
       </c>
-      <c r="AO31" s="15">
-        <f t="shared" si="78"/>
+      <c r="AP31" s="15">
+        <f>E31-K31</f>
         <v>-1</v>
       </c>
-      <c r="AP31" s="15">
+      <c r="AQ31" s="15">
         <v>-457</v>
       </c>
-      <c r="AQ31" s="16">
-        <f>AP31/F31</f>
+      <c r="AR31" s="16">
+        <f>AQ31/F31</f>
         <v>0.59973753280839892</v>
       </c>
-      <c r="AR31" s="15">
-        <f t="shared" ref="AR31:AS31" si="87">AR32+AR33</f>
+      <c r="AS31" s="15">
+        <f t="shared" ref="AS31:AT31" si="79">AS32+AS33</f>
         <v>136</v>
-      </c>
-      <c r="AS31" s="15">
-        <f t="shared" si="87"/>
-        <v>241</v>
       </c>
       <c r="AT31" s="15">
         <f t="shared" si="79"/>
+        <v>241</v>
+      </c>
+      <c r="AU31" s="15">
+        <f t="shared" si="71"/>
         <v>377</v>
       </c>
-      <c r="AU31" s="17">
-        <f t="shared" ref="AU31:AV31" si="88">AU32+AU33</f>
+      <c r="AV31" s="17">
+        <f t="shared" ref="AV31:AW31" si="80">AV32+AV33</f>
         <v>15.293426873</v>
-      </c>
-      <c r="AV31" s="17">
-        <f t="shared" si="88"/>
-        <v>32.941085250999997</v>
       </c>
       <c r="AW31" s="17">
         <f t="shared" si="80"/>
+        <v>32.941085250999997</v>
+      </c>
+      <c r="AX31" s="17">
+        <f t="shared" si="72"/>
         <v>48.234512123999998</v>
       </c>
-      <c r="AX31" s="17">
-        <v>0</v>
-      </c>
       <c r="AY31" s="17">
+        <v>0</v>
+      </c>
+      <c r="AZ31" s="17">
         <v>0.11</v>
       </c>
-      <c r="AZ31" s="20">
-        <f t="shared" si="81"/>
+      <c r="BA31" s="20">
+        <f t="shared" si="73"/>
         <v>48.344512123999998</v>
       </c>
-      <c r="BA31" s="21">
-        <v>0</v>
-      </c>
       <c r="BB31" s="21">
-        <f>AZ31</f>
+        <v>0</v>
+      </c>
+      <c r="BC31" s="21">
+        <f>BA31</f>
         <v>48.344512123999998</v>
       </c>
-      <c r="BC31" s="20">
+      <c r="BD31" s="20">
         <v>11.82</v>
       </c>
-      <c r="BD31" s="17"/>
-      <c r="BE31" s="22">
-        <f t="shared" si="82"/>
+      <c r="BE31" s="17">
+        <v>0</v>
+      </c>
+      <c r="BF31" s="22">
+        <f t="shared" si="74"/>
         <v>60.164512123999998</v>
       </c>
     </row>
-    <row r="32" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="50"/>
       <c r="C32" s="36" t="s">
@@ -5024,7 +5127,7 @@
         <v>32.159999999999997</v>
       </c>
       <c r="S32" s="39">
-        <f t="shared" ref="S32:S33" si="89">Q32+R32</f>
+        <f t="shared" ref="S32:S33" si="81">Q32+R32</f>
         <v>33.739999999999995</v>
       </c>
       <c r="T32" s="36"/>
@@ -5034,54 +5137,54 @@
       <c r="X32" s="36"/>
       <c r="Y32" s="36"/>
       <c r="Z32" s="36"/>
-      <c r="AA32" s="39"/>
+      <c r="AA32" s="36"/>
       <c r="AB32" s="39"/>
       <c r="AC32" s="39"/>
       <c r="AD32" s="39"/>
-      <c r="AE32" s="36"/>
-      <c r="AF32" s="39"/>
+      <c r="AE32" s="39"/>
+      <c r="AF32" s="36"/>
       <c r="AG32" s="39"/>
       <c r="AH32" s="39"/>
       <c r="AI32" s="39"/>
       <c r="AJ32" s="39"/>
-      <c r="AK32" s="63">
-        <f>AR32-AN32</f>
-        <v>471.33330000000001</v>
-      </c>
+      <c r="AK32" s="39"/>
       <c r="AL32" s="63">
         <f>AS32-AO32</f>
+        <v>471.33330000000001</v>
+      </c>
+      <c r="AM32" s="63">
+        <f>AT32-AP32</f>
         <v>201.83330000000001</v>
       </c>
-      <c r="AM32" s="36"/>
-      <c r="AN32" s="36">
-        <f t="shared" si="78"/>
+      <c r="AN32" s="36"/>
+      <c r="AO32" s="36">
+        <f>D32-J32</f>
         <v>-358</v>
       </c>
-      <c r="AO32" s="36">
-        <f t="shared" si="78"/>
+      <c r="AP32" s="36">
+        <f>E32-K32</f>
         <v>-1</v>
       </c>
-      <c r="AP32" s="38"/>
       <c r="AQ32" s="38"/>
-      <c r="AR32" s="36">
+      <c r="AR32" s="38"/>
+      <c r="AS32" s="36">
         <v>113.33329999999999</v>
       </c>
-      <c r="AS32" s="36">
+      <c r="AT32" s="36">
         <v>200.83330000000001</v>
       </c>
-      <c r="AT32" s="36">
-        <f t="shared" si="79"/>
+      <c r="AU32" s="36">
+        <f t="shared" si="71"/>
         <v>314.16660000000002</v>
       </c>
-      <c r="AU32" s="39">
-        <f>AR32*0.11142</f>
+      <c r="AV32" s="39">
+        <f>AS32*0.11142</f>
         <v>12.627596285999999</v>
       </c>
-      <c r="AV32" s="39">
-        <f>AS32*0.13543</f>
+      <c r="AW32" s="39">
+        <f>AT32*0.13543</f>
         <v>27.198853819</v>
       </c>
-      <c r="AW32" s="39"/>
       <c r="AX32" s="39"/>
       <c r="AY32" s="39"/>
       <c r="AZ32" s="39"/>
@@ -5090,8 +5193,9 @@
       <c r="BC32" s="39"/>
       <c r="BD32" s="39"/>
       <c r="BE32" s="39"/>
+      <c r="BF32" s="39"/>
     </row>
-    <row r="33" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="50"/>
       <c r="C33" s="36" t="s">
@@ -5135,7 +5239,7 @@
         <v>6.79</v>
       </c>
       <c r="S33" s="39">
-        <f t="shared" si="89"/>
+        <f t="shared" si="81"/>
         <v>7.12</v>
       </c>
       <c r="T33" s="36"/>
@@ -5145,54 +5249,54 @@
       <c r="X33" s="36"/>
       <c r="Y33" s="36"/>
       <c r="Z33" s="36"/>
-      <c r="AA33" s="39"/>
+      <c r="AA33" s="36"/>
       <c r="AB33" s="39"/>
       <c r="AC33" s="39"/>
-      <c r="AD33" s="36"/>
+      <c r="AD33" s="39"/>
       <c r="AE33" s="36"/>
-      <c r="AF33" s="39"/>
+      <c r="AF33" s="36"/>
       <c r="AG33" s="39"/>
       <c r="AH33" s="39"/>
       <c r="AI33" s="39"/>
       <c r="AJ33" s="39"/>
-      <c r="AK33" s="63">
-        <f>AR33-AN33</f>
-        <v>119.66669999999999</v>
-      </c>
+      <c r="AK33" s="39"/>
       <c r="AL33" s="63">
         <f>AS33-AO33</f>
+        <v>119.66669999999999</v>
+      </c>
+      <c r="AM33" s="63">
+        <f>AT33-AP33</f>
         <v>40.166699999999999</v>
       </c>
-      <c r="AM33" s="36"/>
-      <c r="AN33" s="36">
-        <f t="shared" si="78"/>
+      <c r="AN33" s="36"/>
+      <c r="AO33" s="36">
+        <f>D33-J33</f>
         <v>-97</v>
       </c>
-      <c r="AO33" s="36">
-        <f t="shared" si="78"/>
-        <v>0</v>
-      </c>
-      <c r="AP33" s="38"/>
+      <c r="AP33" s="36">
+        <f>E33-K33</f>
+        <v>0</v>
+      </c>
       <c r="AQ33" s="38"/>
-      <c r="AR33" s="36">
+      <c r="AR33" s="38"/>
+      <c r="AS33" s="36">
         <v>22.666699999999999</v>
       </c>
-      <c r="AS33" s="36">
+      <c r="AT33" s="36">
         <v>40.166699999999999</v>
       </c>
-      <c r="AT33" s="36">
-        <f>AR33+AS33</f>
+      <c r="AU33" s="36">
+        <f>AS33+AT33</f>
         <v>62.833399999999997</v>
       </c>
-      <c r="AU33" s="39">
-        <f>AR33*0.11761</f>
+      <c r="AV33" s="39">
+        <f>AS33*0.11761</f>
         <v>2.6658305869999999</v>
       </c>
-      <c r="AV33" s="39">
-        <f>AS33*0.14296</f>
+      <c r="AW33" s="39">
+        <f>AT33*0.14296</f>
         <v>5.7422314319999996</v>
       </c>
-      <c r="AW33" s="39"/>
       <c r="AX33" s="39"/>
       <c r="AY33" s="39"/>
       <c r="AZ33" s="39"/>
@@ -5201,8 +5305,9 @@
       <c r="BC33" s="39"/>
       <c r="BD33" s="39"/>
       <c r="BE33" s="39"/>
+      <c r="BF33" s="39"/>
     </row>
-    <row r="34" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="13">
         <v>45753</v>
@@ -5280,166 +5385,170 @@
         <v>0.11142857142857142</v>
       </c>
       <c r="X34" s="20">
-        <f>Q34+R34+T34+0.18</f>
+        <v>0.18</v>
+      </c>
+      <c r="Y34" s="20">
+        <f>Q34+R34+T34+X34</f>
         <v>6.1700000000000008</v>
       </c>
-      <c r="Y34" s="21">
-        <v>0</v>
-      </c>
       <c r="Z34" s="21">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="21">
         <v>6</v>
       </c>
-      <c r="AA34" s="17">
-        <v>0</v>
-      </c>
       <c r="AB34" s="17">
         <v>0</v>
       </c>
       <c r="AC34" s="17">
         <v>0</v>
       </c>
-      <c r="AD34" s="20">
+      <c r="AD34" s="17">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="20">
         <v>236.95</v>
       </c>
-      <c r="AE34" s="17">
+      <c r="AF34" s="17">
         <v>10</v>
       </c>
-      <c r="AF34" s="17">
+      <c r="AG34" s="17">
         <v>12.5</v>
       </c>
-      <c r="AG34" s="17">
+      <c r="AH34" s="17">
         <v>236.95</v>
       </c>
-      <c r="AH34" s="17">
-        <f>AE34+AF34+AG34</f>
+      <c r="AI34" s="17">
+        <f>AF34+AG34+AH34</f>
         <v>259.45</v>
       </c>
-      <c r="AI34" s="17">
+      <c r="AJ34" s="17">
         <v>-58.23</v>
       </c>
-      <c r="AJ34" s="22">
-        <f>Z34+AH34+AI34</f>
+      <c r="AK34" s="22">
+        <f>AA34+AI34+AJ34</f>
         <v>207.22</v>
       </c>
-      <c r="AK34" s="15">
-        <f t="shared" ref="AK34:AL34" si="90">AR34-AN34</f>
+      <c r="AL34" s="15">
+        <f t="shared" ref="AL34:AM34" si="82">AS34-AO34</f>
         <v>582</v>
       </c>
-      <c r="AL34" s="15">
-        <f t="shared" si="90"/>
+      <c r="AM34" s="15">
+        <f t="shared" si="82"/>
         <v>212</v>
       </c>
-      <c r="AM34" s="15">
+      <c r="AN34" s="15">
         <v>794</v>
       </c>
-      <c r="AN34" s="15">
-        <f t="shared" ref="AN34:AO34" si="91">D34-J34</f>
+      <c r="AO34" s="15">
+        <f t="shared" ref="AO34:AP34" si="83">D34-J34</f>
         <v>-670</v>
       </c>
-      <c r="AO34" s="15">
-        <f t="shared" si="91"/>
+      <c r="AP34" s="15">
+        <f t="shared" si="83"/>
         <v>-60</v>
       </c>
-      <c r="AP34" s="15">
+      <c r="AQ34" s="15">
         <v>-730</v>
       </c>
-      <c r="AQ34" s="16">
-        <f>AP34/F34</f>
+      <c r="AR34" s="16">
+        <f>AQ34/F34</f>
         <v>0.61916878710771839</v>
       </c>
-      <c r="AR34" s="15">
+      <c r="AS34" s="15">
         <v>-88</v>
       </c>
-      <c r="AS34" s="15">
+      <c r="AT34" s="15">
         <v>152</v>
       </c>
-      <c r="AT34" s="15">
-        <f>AS34+AR34</f>
+      <c r="AU34" s="15">
+        <f>AT34+AS34</f>
         <v>64</v>
       </c>
-      <c r="AU34" s="17">
+      <c r="AV34" s="17">
         <v>-9.8000000000000007</v>
       </c>
-      <c r="AV34" s="17">
+      <c r="AW34" s="17">
         <v>20.59</v>
       </c>
-      <c r="AW34" s="17">
-        <f>AV34+AU34</f>
+      <c r="AX34" s="17">
+        <f>AW34+AV34</f>
         <v>10.79</v>
       </c>
-      <c r="AX34" s="17">
+      <c r="AY34" s="17">
         <v>-0.88</v>
       </c>
-      <c r="AY34" s="17">
+      <c r="AZ34" s="17">
         <v>0.02</v>
       </c>
-      <c r="AZ34" s="20">
-        <f>AY34+AX34+AW34</f>
+      <c r="BA34" s="20">
+        <f>AZ34+AY34+AX34</f>
         <v>9.93</v>
       </c>
-      <c r="BA34" s="21">
-        <v>0</v>
-      </c>
       <c r="BB34" s="21">
+        <v>0</v>
+      </c>
+      <c r="BC34" s="21">
         <v>9.93</v>
       </c>
-      <c r="BC34" s="20">
+      <c r="BD34" s="20">
         <v>369.51</v>
       </c>
-      <c r="BD34" s="17">
+      <c r="BE34" s="17">
         <v>-58.23</v>
       </c>
-      <c r="BE34" s="22">
-        <f>BC34+BB34+BD34</f>
+      <c r="BF34" s="22">
+        <f>BD34+BC34+BE34</f>
         <v>321.20999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y35" s="9"/>
-      <c r="AD35" s="9"/>
+    <row r="35" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z35" s="9"/>
+      <c r="AE35" s="9"/>
     </row>
-    <row r="36" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="V36" s="9"/>
       <c r="W36" s="9"/>
       <c r="X36" s="9"/>
+      <c r="Y36" s="9"/>
     </row>
-    <row r="37" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Z37" s="10"/>
+    <row r="37" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA37" s="10"/>
+      <c r="AB37" s="10"/>
     </row>
-    <row r="38" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T38" s="11"/>
-      <c r="Y38" s="9"/>
-      <c r="Z38" s="12"/>
-      <c r="AA38" s="9"/>
+      <c r="Z38" s="9"/>
+      <c r="AA38" s="12"/>
+      <c r="AB38" s="9"/>
     </row>
-    <row r="39" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P39" s="9"/>
       <c r="T39" s="11"/>
-      <c r="Z39" s="12"/>
-      <c r="AA39" s="9"/>
+      <c r="AA39" s="12"/>
+      <c r="AB39" s="9"/>
     </row>
-    <row r="40" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T41" s="11"/>
     </row>
-    <row r="42" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T43" s="11"/>
-      <c r="Z43" s="9"/>
       <c r="AA43" s="9"/>
+      <c r="AB43" s="9"/>
     </row>
-    <row r="44" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Z45" s="9"/>
+    <row r="44" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA45" s="9"/>
+      <c r="AB45" s="9"/>
     </row>
-    <row r="46" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Z46" s="9"/>
+    <row r="46" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA46" s="9"/>
+      <c r="AB46" s="9"/>
     </row>
-    <row r="47" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6407,18 +6516,18 @@
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:AJ2"/>
-    <mergeCell ref="AK2:BE2"/>
-    <mergeCell ref="AN3:AQ3"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="AU3:BB3"/>
+    <mergeCell ref="D2:AK2"/>
+    <mergeCell ref="AL2:BF2"/>
+    <mergeCell ref="AO3:AR3"/>
+    <mergeCell ref="AS3:AU3"/>
+    <mergeCell ref="AV3:BC3"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N3:P3"/>
-    <mergeCell ref="AA3:AH3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="Q3:Z3"/>
+    <mergeCell ref="AB3:AI3"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="Q3:AA3"/>
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>